<commit_message>
Added RAD BeforePayments Test Cases to Test Suite.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5120543-E5A6-480C-ACE4-A7193C481020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6F8E85-2EFC-446D-A307-A01DC9C3D2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="2565" windowWidth="21420" windowHeight="13620" firstSheet="1" activeTab="5" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView xWindow="-23910" yWindow="1065" windowWidth="21450" windowHeight="16320" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="34">
   <si>
     <t>Result</t>
   </si>
@@ -516,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
@@ -1339,7 +1339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
@@ -1453,7 +1453,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,6 +1487,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1498,6 +1501,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1509,6 +1515,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1520,6 +1529,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1531,6 +1543,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1551,7 +1566,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,10 +1576,11 @@
     <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
     <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1580,11 +1596,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Added RAD Test Cases and data for new FEIN/SSN fields.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6F8E85-2EFC-446D-A307-A01DC9C3D2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{790BA1B7-6ECA-44B9-B4D2-876C0831BDE4}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-23910" yWindow="1065" windowWidth="21450" windowHeight="16320" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView activeTab="6" firstSheet="4" windowHeight="16905" windowWidth="14865" xWindow="2535" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="375"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
-    <sheet name="Existing" sheetId="2" r:id="rId2"/>
-    <sheet name="Extension" sheetId="3" r:id="rId3"/>
-    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
-    <sheet name="Personal" sheetId="5" r:id="rId5"/>
-    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
-    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
-    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
+    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
+    <sheet name="Existing" r:id="rId2" sheetId="2"/>
+    <sheet name="Extension" r:id="rId3" sheetId="3"/>
+    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
+    <sheet name="Personal" r:id="rId5" sheetId="5"/>
+    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
+    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
+    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="44">
   <si>
     <t>Result</t>
   </si>
@@ -145,12 +145,43 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>FeinSsn</t>
+  </si>
+  <si>
+    <t>FEINSSN</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Wed Sep 27 21:05:17 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Sep 27 21:06:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Sep 27 21:22:54 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Sep 27 21:23:50 EDT 2023</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Wed Sep 27 21:34:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Sep 27 21:35:51 EDT 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,19 +224,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -222,10 +253,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -260,7 +291,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -312,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -423,21 +454,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -454,7 +485,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -506,33 +537,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,8 +586,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2" s="1" t="s">
@@ -574,7 +609,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
@@ -591,7 +626,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
@@ -607,8 +642,11 @@
       <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
@@ -624,8 +662,11 @@
       <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
@@ -641,8 +682,11 @@
       <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
@@ -658,10 +702,13 @@
       <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -669,24 +716,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
+      <selection activeCell="D11" sqref="D11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="48.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="48" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,8 +749,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
@@ -714,7 +764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
@@ -725,7 +775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
@@ -736,7 +786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
@@ -746,8 +796,11 @@
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
@@ -757,8 +810,11 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
@@ -769,7 +825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
@@ -780,7 +836,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
@@ -791,7 +847,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
@@ -802,7 +858,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
@@ -812,8 +868,11 @@
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
@@ -823,9 +882,12 @@
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -833,7 +895,458 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -842,17 +1355,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="18" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="56.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="54.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -871,42 +1382,33 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
@@ -914,156 +1416,26 @@
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="49.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="45.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1072,10 +1444,10 @@
         <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,241 +1458,6 @@
         <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1328,7 +1465,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1336,21 +1473,146 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1374,6 +1636,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
@@ -1388,6 +1656,12 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
@@ -1444,125 +1718,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1571,13 +1732,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1609,6 +1769,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added RAD Test Cases and data for MRF.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A65BA59-ED26-4422-9A50-73C10F053085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91EE705-30A3-4985-AFD5-8F62015CA4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="87">
   <si>
     <t>Result</t>
   </si>
@@ -159,124 +159,151 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Fri Sep 29 16:26:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:27:50 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:38:16 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:39:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:39:48 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:40:34 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:41:20 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:42:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:42:49 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:43:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:44:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:45:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:46:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:56:41 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:57:27 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:58:26 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 16:59:25 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:00:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:01:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:08:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:09:49 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:10:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:11:46 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:12:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:13:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:14:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:15:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:16:38 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:17:37 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:18:36 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:19:34 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:20:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:21:32 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:22:30 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:28:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:31:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:32:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:37:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:38:37 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 29 17:39:23 EDT 2023</t>
+    <t>Mon Oct 02 18:35:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:36:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:37:23 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:38:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:39:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:40:19 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:43:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:44:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:44:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:45:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:46:10 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:46:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:47:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:48:20 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:49:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:49:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:50:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:51:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:52:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:53:12 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:54:10 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:55:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:56:05 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:57:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:57:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:58:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 18:59:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:00:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:01:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:02:23 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:03:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:04:20 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:05:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:06:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:06:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:07:58 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:08:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:09:54 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:10:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:11:35 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:12:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:12:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:13:35 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:14:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:14:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:15:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:16:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:17:17 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 02 19:18:03 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -649,7 +676,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D4" sqref="D4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +723,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -716,10 +743,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -738,6 +765,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
@@ -758,6 +791,12 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
@@ -778,6 +817,12 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
@@ -798,6 +843,12 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
@@ -869,7 +920,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -886,7 +937,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -903,7 +954,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -920,7 +971,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -940,7 +991,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -960,7 +1011,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -977,7 +1028,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
@@ -994,7 +1045,7 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -1011,7 +1062,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
@@ -1028,7 +1079,7 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
@@ -1048,7 +1099,7 @@
         <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -1076,7 +1127,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="D4" sqref="D4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1174,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1143,10 +1194,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1166,7 +1217,7 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1189,7 +1240,7 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1212,7 +1263,7 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1235,7 +1286,7 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1265,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,10 +1357,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1329,7 +1380,7 @@
         <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1352,7 +1403,7 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1375,7 +1426,7 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1398,7 +1449,7 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1418,10 +1469,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1441,7 +1492,7 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
@@ -1464,7 +1515,7 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -1487,7 +1538,7 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
@@ -1510,7 +1561,7 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
@@ -1530,10 +1581,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -1553,7 +1604,7 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
@@ -1576,7 +1627,7 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>33</v>
@@ -1599,7 +1650,7 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>33</v>
@@ -1622,7 +1673,7 @@
         <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>33</v>
@@ -1818,7 +1869,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1838,7 +1889,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1854,6 +1905,12 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
@@ -1868,6 +1925,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
@@ -1882,6 +1945,12 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1904,7 +1973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
@@ -1943,7 +2012,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1963,7 +2032,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1980,10 +2049,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1999,6 +2068,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
@@ -2013,6 +2088,12 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
@@ -2071,7 +2152,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Added more RAD Test Cases and Data for MRF.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91EE705-30A3-4985-AFD5-8F62015CA4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A91EE705-30A3-4985-AFD5-8F62015CA4F2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView activeTab="3" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
-    <sheet name="Existing" sheetId="2" r:id="rId2"/>
-    <sheet name="Extension" sheetId="3" r:id="rId3"/>
-    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
-    <sheet name="Personal" sheetId="5" r:id="rId5"/>
-    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
-    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
-    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
+    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
+    <sheet name="Existing" r:id="rId2" sheetId="2"/>
+    <sheet name="Extension" r:id="rId3" sheetId="3"/>
+    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
+    <sheet name="Personal" r:id="rId5" sheetId="5"/>
+    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
+    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
+    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="89">
   <si>
     <t>Result</t>
   </si>
@@ -304,12 +304,19 @@
   </si>
   <si>
     <t>Mon Oct 02 19:18:03 EDT 2023</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Tue Oct 03 12:07:52 EDT 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,19 +359,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -381,10 +388,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -419,7 +426,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -471,7 +478,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -582,21 +589,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -613,7 +620,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -665,15 +672,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4:E7"/>
@@ -681,15 +688,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -723,7 +730,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -869,8 +876,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -878,8 +885,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11:E12"/>
@@ -887,12 +894,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="37.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1115,7 +1122,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1123,8 +1130,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4:E7"/>
@@ -1132,15 +1139,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="18" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1305,7 +1312,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1313,8 +1320,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
@@ -1322,14 +1329,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1692,7 +1699,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1700,8 +1707,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C7"/>
@@ -1709,15 +1716,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1819,7 +1826,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1827,8 +1834,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C4"/>
@@ -1836,12 +1843,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,13 +1972,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C6"/>
@@ -1979,12 +1986,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2108,13 +2115,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
@@ -2122,12 +2129,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2165,6 +2172,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RAD to add MD Central Registration Number to 2 tax forms.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{A91EE705-30A3-4985-AFD5-8F62015CA4F2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{03DAE8C6-717B-4CB1-906E-09EB92EBACFC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="-120"/>
+    <workbookView windowHeight="16620" windowWidth="18810" xWindow="4170" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="615"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" r:id="rId1" sheetId="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="164">
   <si>
     <t>Result</t>
   </si>
@@ -159,120 +159,6 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Mon Oct 02 18:35:48 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:36:37 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:37:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:38:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:39:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:40:19 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:43:15 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:44:00 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:44:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:45:27 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:46:10 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:46:53 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:47:37 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:48:20 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:49:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:49:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:50:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:51:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:52:29 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:53:12 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:54:10 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:55:07 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:56:05 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:57:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:57:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:58:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 18:59:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:00:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:01:41 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:02:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:03:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:04:20 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:05:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:06:16 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:06:59 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:07:58 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:08:56 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:09:54 EDT 2023</t>
-  </si>
-  <si>
     <t>Mon Oct 02 19:10:53 EDT 2023</t>
   </si>
   <si>
@@ -306,10 +192,349 @@
     <t>Mon Oct 02 19:18:03 EDT 2023</t>
   </si>
   <si>
+    <t>Wed Oct 04 18:52:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 18:53:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 18:54:05 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 18:54:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 18:55:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 18:56:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 18:58:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 18:58:51 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 18:59:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:00:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:00:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:01:38 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:02:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:03:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:03:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:04:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:05:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:18:49 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:20:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:21:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:36:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:43:28 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:44:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:53:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:53:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:54:28 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:55:10 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:55:51 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:56:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:57:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:57:54 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:58:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:59:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 19:59:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 20:00:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 20:01:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 20:02:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 04 20:02:43 EDT 2023</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Tue Oct 03 12:07:52 EDT 2023</t>
+    <t>Fri Oct 06 12:04:39 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:05:22 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:06:05 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:06:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:07:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:08:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:08:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:09:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:10:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:11:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:11:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:12:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:13:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:14:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:15:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:17:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:17:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:18:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:19:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:20:06 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:20:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:21:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:22:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:22:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:23:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:24:23 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:25:05 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:25:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:26:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:27:12 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:27:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:28:38 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:29:22 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:30:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:30:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:31:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:32:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:32:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:33:39 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:34:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:35:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:35:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:36:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:37:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:38:26 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:39:12 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:39:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:40:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Oct 06 12:42:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:07:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:07:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:08:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:09:20 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:10:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:10:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:11:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:12:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:12:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:13:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:14:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:14:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:15:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:16:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:16:57 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:17:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 16:18:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 17:13:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 17:14:09 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 17:14:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 17:15:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 17:16:06 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 17:16:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 17:17:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 17:18:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 17:18:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 17:19:43 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -682,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +978,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -773,10 +998,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -799,10 +1024,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -825,10 +1050,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -851,10 +1076,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -889,13 +1114,13 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:E12"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
     <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
@@ -927,7 +1152,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -944,7 +1169,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -961,7 +1186,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -978,7 +1203,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>140</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -998,7 +1223,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1018,7 +1243,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>142</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1035,7 +1260,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
@@ -1052,7 +1277,7 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -1069,7 +1294,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
@@ -1083,10 +1308,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
@@ -1103,10 +1328,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>147</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -1134,13 +1359,13 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E7"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
     <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
@@ -1181,7 +1406,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1204,7 +1429,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1221,10 +1446,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>150</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1244,10 +1469,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>151</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1267,10 +1492,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1290,10 +1515,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1323,7 +1548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1367,7 +1592,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1384,10 +1609,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1407,10 +1632,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1430,10 +1655,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1453,10 +1678,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1479,7 +1704,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1496,10 +1721,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
@@ -1519,10 +1744,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -1542,10 +1767,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
@@ -1565,10 +1790,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
@@ -1591,7 +1816,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -1608,10 +1833,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
@@ -1631,10 +1856,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>123</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>33</v>
@@ -1654,10 +1879,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>33</v>
@@ -1677,10 +1902,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>33</v>
@@ -1876,7 +2101,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>154</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1896,7 +2121,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1916,7 +2141,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>156</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1936,7 +2161,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1956,7 +2181,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>158</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -2019,7 +2244,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -2039,7 +2264,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>160</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -2059,7 +2284,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -2079,7 +2304,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -2099,7 +2324,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -2159,7 +2384,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Made changes to RAD FEIN/SSN object recognition.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{03DAE8C6-717B-4CB1-906E-09EB92EBACFC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{6EDFE210-2E41-4336-80A2-49D855DB2D6D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="16620" windowWidth="18810" xWindow="4170" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="615"/>
+    <workbookView activeTab="1" windowHeight="14565" windowWidth="18810" xWindow="-21300" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="1350"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" r:id="rId1" sheetId="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="131">
   <si>
     <t>Result</t>
   </si>
@@ -159,529 +159,283 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Mon Oct 02 19:10:53 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:11:35 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:12:15 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:12:55 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:13:35 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:14:15 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:14:56 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:15:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:16:30 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:17:17 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 02 19:18:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 18:52:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 18:53:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 18:54:05 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 18:54:48 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 18:55:31 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 18:56:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 18:58:07 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 18:58:51 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 18:59:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:00:14 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:00:56 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:01:38 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:02:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:03:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:03:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:04:27 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:05:27 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:18:49 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:20:31 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:21:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:36:55 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:43:28 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:44:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:53:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:53:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:54:28 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:55:10 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:55:51 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:56:32 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:57:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:57:54 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:58:36 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:59:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 19:59:59 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 20:00:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 20:01:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 20:02:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Oct 04 20:02:43 EDT 2023</t>
+    <t>Mon Oct 09 23:29:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:30:05 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:30:44 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:31:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:32:03 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:32:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:33:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:34:03 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:34:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:35:23 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:36:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:36:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:37:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:38:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:38:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:39:22 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:40:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:40:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:41:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:42:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:42:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:43:23 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:44:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:44:39 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:45:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:45:54 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:46:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:47:11 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:47:54 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:48:39 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:49:22 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Oct 09 23:50:06 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 13:40:12 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 13:41:08 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 13:42:03 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 13:42:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 13:43:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 13:44:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 14:41:44 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 14:44:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 14:45:19 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 14:46:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 14:47:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 14:48:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 14:50:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 14:59:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:00:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:01:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:18:40 EDT 2023</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Fri Oct 06 12:04:39 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:05:22 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:06:05 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:06:48 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:07:32 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:08:15 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:08:59 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:09:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:10:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:11:07 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:11:50 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:12:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:13:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:14:53 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:15:37 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:17:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:17:56 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:18:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:19:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:20:06 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:20:48 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:21:31 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:22:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:22:56 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:23:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:24:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:25:05 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:25:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:26:30 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:27:12 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:27:55 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:28:38 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:29:22 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:30:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:30:48 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:31:30 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:32:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:32:56 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:33:39 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:34:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:35:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:35:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:36:36 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:37:31 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:38:26 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:39:12 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:39:59 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:40:59 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Oct 06 12:42:00 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:07:15 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:07:56 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:08:37 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:09:20 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:10:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:10:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:11:25 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:12:07 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:12:48 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:13:31 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:14:14 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:14:55 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:15:36 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:16:16 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:16:57 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:17:37 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 16:18:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 17:13:25 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 17:14:09 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 17:14:48 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 17:15:27 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 17:16:06 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 17:16:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 17:17:29 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 17:18:14 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 17:18:59 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 17:19:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:18:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:18:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:19:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:20:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:20:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:21:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:22:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:22:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:23:22 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:24:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:24:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:25:22 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:26:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:26:44 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:27:25 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:28:05 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:28:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:29:25 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:30:05 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:30:44 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:31:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:32:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:32:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:33:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:34:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:34:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:35:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:36:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:36:41 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:37:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:38:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:38:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:39:22 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:40:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:40:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:41:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:42:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:42:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:43:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:44:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:44:39 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:45:16 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:45:54 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:46:31 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:47:11 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:47:54 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:48:39 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:49:22 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:50:06 EDT 2023</t>
+    <t>Tue Oct 31 15:30:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:31:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:32:06 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:32:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:33:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:34:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:35:39 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:36:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:37:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:38:19 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 15:39:11 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:41:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:42:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:43:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:44:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:45:26 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:46:19 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:47:49 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:48:44 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:49:38 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:50:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:51:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:52:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:53:11 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:54:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:54:58 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:55:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:56:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:57:35 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:58:28 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:59:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:00:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:08:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:12:49 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:13:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:14:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:15:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:16:12 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:17:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:18:54 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:19:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:20:46 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 17:21:42 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -1054,15 +808,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="32.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
@@ -1102,7 +856,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1125,7 +879,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1148,7 +902,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1174,7 +928,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>73</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1200,7 +954,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>74</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1226,7 +980,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1260,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1053,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1316,7 +1070,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1333,7 +1087,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1350,7 +1104,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>91</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1370,7 +1124,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1390,7 +1144,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>93</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1407,7 +1161,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
@@ -1424,7 +1178,7 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>95</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -1441,7 +1195,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>96</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
@@ -1458,7 +1212,7 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>97</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
@@ -1478,7 +1232,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>98</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -1553,7 +1307,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1576,7 +1330,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1596,7 +1350,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>101</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1619,7 +1373,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>102</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1642,7 +1396,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1665,7 +1419,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>104</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1739,7 +1493,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1759,7 +1513,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1782,7 +1536,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>107</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1805,7 +1559,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>108</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1828,7 +1582,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>109</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1851,7 +1605,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>110</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1871,7 +1625,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>111</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
@@ -1894,7 +1648,7 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>112</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -1917,7 +1671,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>113</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
@@ -1940,7 +1694,7 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>114</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
@@ -1963,7 +1717,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>197</v>
+        <v>115</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -1983,7 +1737,7 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>198</v>
+        <v>116</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
@@ -2006,7 +1760,7 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>199</v>
+        <v>117</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>33</v>
@@ -2029,7 +1783,7 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>118</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>33</v>
@@ -2052,7 +1806,7 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>201</v>
+        <v>119</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>33</v>
@@ -2248,7 +2002,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>121</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -2268,7 +2022,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -2288,7 +2042,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>123</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -2308,7 +2062,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -2328,7 +2082,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>125</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -2391,7 +2145,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -2411,7 +2165,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -2431,7 +2185,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -2451,7 +2205,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>129</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -2471,7 +2225,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>130</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -2531,7 +2285,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Removed Extension Payments Tax Type from execution.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6EDFE210-2E41-4336-80A2-49D855DB2D6D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{0B25E585-3E20-4D14-8258-54376897700F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="14565" windowWidth="18810" xWindow="-21300" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="1350"/>
+    <workbookView activeTab="5" firstSheet="3" windowHeight="14565" windowWidth="18810" xWindow="8505" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="1395"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" r:id="rId1" sheetId="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="98">
   <si>
     <t>Result</t>
   </si>
@@ -156,286 +156,187 @@
     <t>Pass</t>
   </si>
   <si>
+    <t>Tue Oct 31 16:41:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:42:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:43:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:44:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:45:26 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Oct 31 16:46:19 EDT 2023</t>
+  </si>
+  <si>
+    <t>DONOTRUN</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:11:28 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:12:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:13:15 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:14:09 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:15:03 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:15:56 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:16:50 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:17:43 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:18:36 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:19:29 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:20:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:21:14 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:22:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:23:02 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:23:56 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:24:51 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:25:45 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:26:39 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:27:33 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:28:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:29:19 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:30:13 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:31:07 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:32:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:32:54 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:33:47 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:34:40 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:35:32 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:36:25 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:37:19 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:38:12 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:39:05 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:39:59 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:40:51 EST 2023</t>
+  </si>
+  <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>Mon Oct 09 23:29:25 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:30:05 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:30:44 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:31:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:32:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:32:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:33:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:34:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:34:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:35:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:36:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:36:41 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:37:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:38:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:38:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:39:22 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:40:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:40:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:41:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:42:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:42:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:43:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:44:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:44:39 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:45:16 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:45:54 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:46:31 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:47:11 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:47:54 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:48:39 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:49:22 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Oct 09 23:50:06 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 13:40:12 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 13:41:08 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 13:42:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 13:42:56 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 13:43:48 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 13:44:41 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 14:41:44 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 14:44:27 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 14:45:19 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 14:46:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 14:47:07 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 14:48:00 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 14:50:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 14:59:41 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:00:37 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:01:30 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:18:40 EDT 2023</t>
+    <t>Thu Dec 07 22:41:41 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:43:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:44:00 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:44:50 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:45:41 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:46:40 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:48:15 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:49:11 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Dec 07 22:50:07 EST 2023</t>
+  </si>
+  <si>
+    <t>DoNotRun</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Tue Oct 31 15:30:16 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:31:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:32:06 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:32:59 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:33:53 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:34:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:35:39 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:36:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:37:25 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:38:19 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 15:39:11 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:41:50 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:42:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:43:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:44:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:45:26 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:46:19 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:47:49 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:48:44 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:49:38 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:50:32 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:51:25 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:52:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:53:11 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:54:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:54:58 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:55:50 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:56:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:57:35 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:58:28 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:59:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:00:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:08:29 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:12:49 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:13:41 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:14:31 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:15:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:16:12 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:17:55 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:18:54 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:19:50 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:20:46 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 17:21:42 EDT 2023</t>
+    <t>Fri Dec 08 10:50:48 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Dec 08 10:51:38 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Dec 08 10:52:28 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Dec 08 10:53:18 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Dec 08 10:54:09 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Dec 08 10:55:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Dec 08 10:56:04 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Dec 08 10:57:02 EST 2023</t>
   </si>
 </sst>
 </file>
@@ -856,7 +757,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -879,7 +780,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -902,7 +803,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -928,7 +829,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -954,7 +855,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -980,7 +881,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1014,7 +915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
@@ -1053,7 +954,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1070,7 +971,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1087,7 +988,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1104,7 +1005,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1124,7 +1025,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1144,7 +1045,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1161,7 +1062,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
@@ -1178,7 +1079,7 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -1195,7 +1096,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
@@ -1212,7 +1113,7 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
@@ -1232,7 +1133,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -1260,14 +1161,14 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.140625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
     <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
@@ -1307,10 +1208,10 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -1330,10 +1231,10 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
@@ -1350,10 +1251,10 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
@@ -1373,10 +1274,10 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
@@ -1396,10 +1297,10 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
@@ -1419,10 +1320,10 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>15</v>
@@ -1493,7 +1394,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -1513,7 +1414,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -1536,7 +1437,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -1559,7 +1460,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1582,7 +1483,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1605,7 +1506,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -1625,7 +1526,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
@@ -1648,7 +1549,7 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -1671,7 +1572,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
@@ -1694,7 +1595,7 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
@@ -1717,7 +1618,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
@@ -1737,7 +1638,7 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
@@ -1760,7 +1661,7 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>33</v>
@@ -1783,7 +1684,7 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>33</v>
@@ -1806,7 +1707,7 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>33</v>
@@ -1837,14 +1738,14 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
     <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
@@ -1897,7 +1798,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
@@ -1963,15 +1864,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.140625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
     <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
@@ -2002,7 +1903,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -2019,13 +1920,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
@@ -2042,7 +1943,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -2062,7 +1963,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -2082,7 +1983,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -2107,14 +2008,14 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
     <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
@@ -2145,7 +2046,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -2162,13 +2063,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
@@ -2185,7 +2086,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>
@@ -2205,7 +2106,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -2225,7 +2126,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -2285,7 +2186,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Fixed RAD Phase 3 Summary and BeforePayments Test Cases and Data.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DA0C8B-CB52-4C14-90D5-91415020A1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932A80B1-517B-40C4-9FA3-3E73650877C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="2280" windowWidth="24525" windowHeight="14010" activeTab="3" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView xWindow="2415" yWindow="1965" windowWidth="24525" windowHeight="14010" activeTab="7" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="101">
   <si>
     <t>Result</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t>Sales and Use Tax</t>
+  </si>
+  <si>
+    <t>Mon Jan 15 21:03:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Mon Jan 15 21:05:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Mon Jan 15 21:07:19 EST 2024</t>
   </si>
 </sst>
 </file>
@@ -922,7 +931,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1207,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1208,8 +1217,11 @@
       <c r="E17" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1220,7 +1232,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1231,7 +1243,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1444,14 +1456,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
     <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
@@ -1819,7 +1831,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1833,7 +1845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1847,7 +1859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1861,7 +1873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1875,7 +1887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>32</v>
       </c>
@@ -1889,7 +1901,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
@@ -1903,7 +1915,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1917,7 +1929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1931,7 +1943,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>32</v>
       </c>
@@ -1945,7 +1957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1958,8 +1970,17 @@
       <c r="F26" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1973,7 +1994,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
       </c>
@@ -1987,7 +2014,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>100</v>
+      </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
       </c>
@@ -2001,7 +2034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>32</v>
       </c>
@@ -2015,7 +2048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
@@ -2029,7 +2062,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>32</v>
       </c>
@@ -2043,7 +2076,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>32</v>
       </c>
@@ -2057,7 +2090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>32</v>
       </c>
@@ -2071,7 +2104,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>32</v>
       </c>
@@ -2085,7 +2118,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>32</v>
       </c>
@@ -2099,7 +2132,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>32</v>
       </c>
@@ -2113,7 +2146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>32</v>
       </c>
@@ -2127,7 +2160,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>32</v>
       </c>
@@ -2140,8 +2173,11 @@
       <c r="F39" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>32</v>
       </c>
@@ -2155,7 +2191,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>32</v>
       </c>
@@ -2169,7 +2205,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>32</v>
       </c>
@@ -2183,7 +2219,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
         <v>32</v>
       </c>
@@ -2197,7 +2233,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>32</v>
       </c>
@@ -2211,7 +2247,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>32</v>
       </c>
@@ -2225,7 +2261,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>32</v>
       </c>
@@ -2239,7 +2275,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
         <v>32</v>
       </c>
@@ -2253,7 +2289,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>32</v>
       </c>
@@ -2267,7 +2303,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>32</v>
       </c>
@@ -2281,7 +2317,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>32</v>
       </c>
@@ -2295,7 +2331,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
         <v>32</v>
       </c>
@@ -2309,7 +2345,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
         <v>32</v>
       </c>
@@ -2322,8 +2358,11 @@
       <c r="F52" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>32</v>
       </c>
@@ -2337,7 +2376,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
         <v>32</v>
       </c>
@@ -2351,7 +2390,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
         <v>32</v>
       </c>
@@ -2791,7 +2830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made changes to RAD Summary and BeforePayments test data.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5456CEA0-7AAB-480A-B884-BF54E315C558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7205EAE8-2027-44B4-8658-389E6F1849CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26235" yWindow="3315" windowWidth="24525" windowHeight="14010" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView xWindow="-26250" yWindow="3450" windowWidth="24525" windowHeight="14010" activeTab="5" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="167">
   <si>
     <t>Result</t>
   </si>
@@ -186,57 +186,6 @@
     <t>DoNotRun</t>
   </si>
   <si>
-    <t>Mon Dec 11 15:32:54 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:33:36 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:34:22 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:35:04 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:35:47 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:36:28 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:37:10 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:37:53 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:38:35 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:39:18 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:40:01 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:41:21 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:42:03 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:42:47 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:43:28 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:44:10 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:44:51 EST 2023</t>
-  </si>
-  <si>
     <t>Mon Dec 11 15:45:32 EST 2023</t>
   </si>
   <si>
@@ -264,33 +213,6 @@
     <t>Mon Dec 11 15:51:05 EST 2023</t>
   </si>
   <si>
-    <t>Mon Dec 11 18:09:41 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 18:10:27 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 18:11:09 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 18:11:55 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 18:12:38 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 18:13:36 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:12:12 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:13:25 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:14:09 EST 2023</t>
-  </si>
-  <si>
     <t>Mon Dec 11 21:14:49 EST 2023</t>
   </si>
   <si>
@@ -339,13 +261,289 @@
     <t>Sales and Use Tax</t>
   </si>
   <si>
-    <t>Mon Jan 15 21:03:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Mon Jan 15 21:05:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Mon Jan 15 21:07:19 EST 2024</t>
+    <t>App ID</t>
+  </si>
+  <si>
+    <t>738</t>
+  </si>
+  <si>
+    <t>773</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 17:11:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 17:12:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Backend Data</t>
+  </si>
+  <si>
+    <t>Verified</t>
+  </si>
+  <si>
+    <t>Tranx Fails</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 17:23:31 EST 2024</t>
+  </si>
+  <si>
+    <t>774</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 17:25:34 EST 2024</t>
+  </si>
+  <si>
+    <t>783</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 17:30:44 EST 2024</t>
+  </si>
+  <si>
+    <t>784</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 17:32:45 EST 2024</t>
+  </si>
+  <si>
+    <t>786</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 17:44:36 EST 2024</t>
+  </si>
+  <si>
+    <t>705</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 17:49:51 EST 2024</t>
+  </si>
+  <si>
+    <t>706</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 17:53:16 EST 2024</t>
+  </si>
+  <si>
+    <t>707</t>
+  </si>
+  <si>
+    <t>Month is 12 instead of 00</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 18:22:08 EST 2024</t>
+  </si>
+  <si>
+    <t>709</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 18:26:22 EST 2024</t>
+  </si>
+  <si>
+    <t>711</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 18:30:38 EST 2024</t>
+  </si>
+  <si>
+    <t>712</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 18:43:10 EST 2024</t>
+  </si>
+  <si>
+    <t>713</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 18:47:04 EST 2024</t>
+  </si>
+  <si>
+    <t>714</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 18:50:43 EST 2024</t>
+  </si>
+  <si>
+    <t>715</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 18:59:24 EST 2024</t>
+  </si>
+  <si>
+    <t>788</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 19:04:15 EST 2024</t>
+  </si>
+  <si>
+    <t>787</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 19:06:23 EST 2024</t>
+  </si>
+  <si>
+    <t>795</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 19:10:31 EST 2024</t>
+  </si>
+  <si>
+    <t>799</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 19:17:16 EST 2024</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 19:20:25 EST 2024</t>
+  </si>
+  <si>
+    <t>801</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 19:59:52 EST 2024</t>
+  </si>
+  <si>
+    <t>802</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 20:06:10 EST 2024</t>
+  </si>
+  <si>
+    <t>803</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 20:08:39 EST 2024</t>
+  </si>
+  <si>
+    <t>816</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 20:16:16 EST 2024</t>
+  </si>
+  <si>
+    <t>778</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 20:21:39 EST 2024</t>
+  </si>
+  <si>
+    <t>779</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 20:24:16 EST 2024</t>
+  </si>
+  <si>
+    <t>780</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 20:26:56 EST 2024</t>
+  </si>
+  <si>
+    <t>781</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 20:29:31 EST 2024</t>
+  </si>
+  <si>
+    <t>782</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 20:35:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 20:38:06 EST 2024</t>
+  </si>
+  <si>
+    <t>804</t>
+  </si>
+  <si>
+    <t>805</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 20:44:14 EST 2024</t>
+  </si>
+  <si>
+    <t>806</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:01:16 EST 2024</t>
+  </si>
+  <si>
+    <t>798</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:08:09 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:10:00 EST 2024</t>
+  </si>
+  <si>
+    <t>809</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:12:42 EST 2024</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:14:53 EST 2024</t>
+  </si>
+  <si>
+    <t>811</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:19:25 EST 2024</t>
+  </si>
+  <si>
+    <t>812</t>
+  </si>
+  <si>
+    <t>813</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:25:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:36:32 EST 2024</t>
+  </si>
+  <si>
+    <t>814</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:39:28 EST 2024</t>
+  </si>
+  <si>
+    <t>815</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:42:19 EST 2024</t>
+  </si>
+  <si>
+    <t>817</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:44:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:47:56 EST 2024</t>
+  </si>
+  <si>
+    <t>702</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:52:47 EST 2024</t>
+  </si>
+  <si>
+    <t>703</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 21:57:40 EST 2024</t>
+  </si>
+  <si>
+    <t>708</t>
   </si>
 </sst>
 </file>
@@ -721,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,10 +935,12 @@
     <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,13 +965,19 @@
       <c r="H1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -783,18 +989,24 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -806,18 +1018,24 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -829,7 +1047,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -837,13 +1055,19 @@
       <c r="H4" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -855,7 +1079,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>22</v>
@@ -863,13 +1087,19 @@
       <c r="H5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -881,7 +1111,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>23</v>
@@ -889,13 +1119,19 @@
       <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -907,13 +1143,19 @@
         <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -928,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,10 +1183,12 @@
     <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
     <col min="4" max="4" width="37.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -963,13 +1207,19 @@
       <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -980,13 +1230,19 @@
       <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -997,13 +1253,19 @@
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1014,13 +1276,19 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1034,13 +1302,19 @@
       <c r="F5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1054,13 +1328,19 @@
       <c r="F6" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1071,13 +1351,16 @@
       <c r="E7" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1088,13 +1371,16 @@
       <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1105,13 +1391,16 @@
       <c r="E9" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1122,13 +1411,16 @@
       <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1142,13 +1434,16 @@
       <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1162,8 +1457,17 @@
       <c r="F12" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>111</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
@@ -1171,10 +1475,13 @@
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1182,10 +1489,16 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1193,10 +1506,19 @@
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
@@ -1204,10 +1526,19 @@
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1215,13 +1546,22 @@
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1229,10 +1569,19 @@
         <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1240,10 +1589,19 @@
         <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1251,7 +1609,10 @@
         <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>96</v>
+        <v>70</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1454,10 +1815,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C55"/>
+      <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,10 +1830,12 @@
     <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
     <col min="7" max="7" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="9.140625" style="1" collapsed="1"/>
+    <col min="9" max="9" width="23.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1494,13 +1857,19 @@
       <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1514,13 +1883,16 @@
       <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1537,13 +1909,16 @@
       <c r="G3" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1560,13 +1935,16 @@
       <c r="G4" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1583,13 +1961,16 @@
       <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1606,13 +1987,16 @@
       <c r="G6" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1626,13 +2010,16 @@
       <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1649,13 +2036,16 @@
       <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1672,13 +2062,16 @@
       <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1695,13 +2088,16 @@
       <c r="G10" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1718,13 +2114,16 @@
       <c r="G11" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1738,13 +2137,16 @@
       <c r="F12" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1761,13 +2163,16 @@
       <c r="G13" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1784,13 +2189,16 @@
       <c r="G14" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1807,13 +2215,16 @@
       <c r="G15" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1830,8 +2241,17 @@
       <c r="G16" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1839,13 +2259,22 @@
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>139</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1858,8 +2287,17 @@
       <c r="F18" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>141</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1872,8 +2310,17 @@
       <c r="F19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>143</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1886,8 +2333,11 @@
       <c r="F20" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>32</v>
       </c>
@@ -1895,13 +2345,19 @@
         <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>144</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
@@ -1909,13 +2365,22 @@
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>146</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1923,13 +2388,22 @@
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>148</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1937,13 +2411,22 @@
         <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>150</v>
+      </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
       </c>
@@ -1956,8 +2439,17 @@
       <c r="F25" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>153</v>
+      </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1965,7 +2457,7 @@
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>18</v>
@@ -1973,13 +2465,16 @@
       <c r="G26" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>154</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -1988,18 +2483,21 @@
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2008,18 +2506,21 @@
         <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2033,8 +2534,17 @@
       <c r="F29" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>160</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
       </c>
@@ -2042,13 +2552,16 @@
         <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
@@ -2061,8 +2574,11 @@
       <c r="F31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>32</v>
       </c>
@@ -2075,8 +2591,11 @@
       <c r="F32" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>32</v>
       </c>
@@ -2089,8 +2608,11 @@
       <c r="F33" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>32</v>
       </c>
@@ -2098,13 +2620,13 @@
         <v>16</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>32</v>
       </c>
@@ -2112,13 +2634,16 @@
         <v>16</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>32</v>
       </c>
@@ -2126,13 +2651,16 @@
         <v>16</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>32</v>
       </c>
@@ -2140,13 +2668,16 @@
         <v>16</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>32</v>
       </c>
@@ -2159,8 +2690,11 @@
       <c r="F38" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>32</v>
       </c>
@@ -2168,7 +2702,7 @@
         <v>16</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>30</v>
@@ -2176,8 +2710,11 @@
       <c r="G39" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>32</v>
       </c>
@@ -2185,13 +2722,16 @@
         <v>16</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>32</v>
       </c>
@@ -2199,13 +2739,16 @@
         <v>16</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>32</v>
       </c>
@@ -2218,8 +2761,11 @@
       <c r="F42" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
         <v>32</v>
       </c>
@@ -2227,13 +2773,16 @@
         <v>16</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>32</v>
       </c>
@@ -2246,8 +2795,11 @@
       <c r="F44" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>32</v>
       </c>
@@ -2260,8 +2812,11 @@
       <c r="F45" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>32</v>
       </c>
@@ -2274,8 +2829,11 @@
       <c r="F46" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
         <v>32</v>
       </c>
@@ -2283,13 +2841,13 @@
         <v>16</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>32</v>
       </c>
@@ -2297,13 +2855,16 @@
         <v>16</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>32</v>
       </c>
@@ -2311,13 +2872,16 @@
         <v>16</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>32</v>
       </c>
@@ -2325,13 +2889,16 @@
         <v>16</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
         <v>32</v>
       </c>
@@ -2344,8 +2911,11 @@
       <c r="F51" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
         <v>32</v>
       </c>
@@ -2353,7 +2923,7 @@
         <v>16</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>31</v>
@@ -2361,8 +2931,11 @@
       <c r="G52" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>32</v>
       </c>
@@ -2370,13 +2943,16 @@
         <v>16</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
         <v>32</v>
       </c>
@@ -2384,13 +2960,16 @@
         <v>16</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
         <v>32</v>
       </c>
@@ -2402,6 +2981,9 @@
       </c>
       <c r="F55" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2462,7 +3044,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2542,10 +3124,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,10 +3137,12 @@
     <col min="3" max="3" width="15.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2577,13 +3161,19 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2595,10 +3185,13 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -2618,12 +3211,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2637,13 +3230,16 @@
       <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2657,13 +3253,16 @@
       <c r="F5" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2676,6 +3275,9 @@
       </c>
       <c r="F6" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2726,7 +3328,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2738,7 +3340,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2766,7 +3368,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2786,7 +3388,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2806,7 +3408,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2828,10 +3430,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,7 +3446,7 @@
     <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2860,13 +3462,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>165</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2876,6 +3481,9 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified RAD Phase 3 scripts and test data for Estate Tax.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7205EAE8-2027-44B4-8658-389E6F1849CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{7BC77991-A6A2-41DD-B0EC-EB4D825CD7A3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-26250" yWindow="3450" windowWidth="24525" windowHeight="14010" activeTab="5" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView activeTab="7" windowHeight="14010" windowWidth="24525" xWindow="1680" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="2580"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
-    <sheet name="Existing" sheetId="2" r:id="rId2"/>
-    <sheet name="Extension" sheetId="3" r:id="rId3"/>
-    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
-    <sheet name="Personal" sheetId="5" r:id="rId5"/>
-    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
-    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
-    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
+    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
+    <sheet name="Existing" r:id="rId2" sheetId="2"/>
+    <sheet name="Extension" r:id="rId3" sheetId="3"/>
+    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
+    <sheet name="Personal" r:id="rId5" sheetId="5"/>
+    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
+    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
+    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="260">
   <si>
     <t>Result</t>
   </si>
@@ -186,51 +186,6 @@
     <t>DoNotRun</t>
   </si>
   <si>
-    <t>Mon Dec 11 15:45:32 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:46:12 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:46:53 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:47:34 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:48:19 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:49:01 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:49:43 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:50:24 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 15:51:05 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:14:49 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:15:28 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:23:29 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:24:18 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:25:03 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:25:48 EST 2023</t>
-  </si>
-  <si>
     <t>2024</t>
   </si>
   <si>
@@ -270,12 +225,6 @@
     <t>773</t>
   </si>
   <si>
-    <t>Sat Jan 20 17:11:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 20 17:12:02 EST 2024</t>
-  </si>
-  <si>
     <t>Backend Data</t>
   </si>
   <si>
@@ -285,271 +234,602 @@
     <t>Tranx Fails</t>
   </si>
   <si>
-    <t>Sat Jan 20 17:23:31 EST 2024</t>
-  </si>
-  <si>
     <t>774</t>
   </si>
   <si>
-    <t>Sat Jan 20 17:25:34 EST 2024</t>
-  </si>
-  <si>
     <t>783</t>
   </si>
   <si>
-    <t>Sat Jan 20 17:30:44 EST 2024</t>
-  </si>
-  <si>
     <t>784</t>
   </si>
   <si>
-    <t>Sat Jan 20 17:32:45 EST 2024</t>
-  </si>
-  <si>
     <t>786</t>
   </si>
   <si>
-    <t>Sat Jan 20 17:44:36 EST 2024</t>
-  </si>
-  <si>
     <t>705</t>
   </si>
   <si>
-    <t>Sat Jan 20 17:49:51 EST 2024</t>
-  </si>
-  <si>
     <t>706</t>
   </si>
   <si>
-    <t>Sat Jan 20 17:53:16 EST 2024</t>
-  </si>
-  <si>
     <t>707</t>
   </si>
   <si>
     <t>Month is 12 instead of 00</t>
   </si>
   <si>
-    <t>Sat Jan 20 18:22:08 EST 2024</t>
-  </si>
-  <si>
     <t>709</t>
   </si>
   <si>
-    <t>Sat Jan 20 18:26:22 EST 2024</t>
-  </si>
-  <si>
     <t>711</t>
   </si>
   <si>
-    <t>Sat Jan 20 18:30:38 EST 2024</t>
-  </si>
-  <si>
     <t>712</t>
   </si>
   <si>
-    <t>Sat Jan 20 18:43:10 EST 2024</t>
-  </si>
-  <si>
     <t>713</t>
   </si>
   <si>
-    <t>Sat Jan 20 18:47:04 EST 2024</t>
-  </si>
-  <si>
     <t>714</t>
   </si>
   <si>
-    <t>Sat Jan 20 18:50:43 EST 2024</t>
-  </si>
-  <si>
     <t>715</t>
   </si>
   <si>
-    <t>Sat Jan 20 18:59:24 EST 2024</t>
-  </si>
-  <si>
     <t>788</t>
   </si>
   <si>
-    <t>Sat Jan 20 19:04:15 EST 2024</t>
-  </si>
-  <si>
     <t>787</t>
   </si>
   <si>
-    <t>Sat Jan 20 19:06:23 EST 2024</t>
-  </si>
-  <si>
     <t>795</t>
   </si>
   <si>
-    <t>Sat Jan 20 19:10:31 EST 2024</t>
-  </si>
-  <si>
     <t>799</t>
   </si>
   <si>
-    <t>Sat Jan 20 19:17:16 EST 2024</t>
-  </si>
-  <si>
     <t>800</t>
   </si>
   <si>
-    <t>Sat Jan 20 19:20:25 EST 2024</t>
-  </si>
-  <si>
     <t>801</t>
   </si>
   <si>
-    <t>Sat Jan 20 19:59:52 EST 2024</t>
-  </si>
-  <si>
     <t>802</t>
   </si>
   <si>
-    <t>Sat Jan 20 20:06:10 EST 2024</t>
-  </si>
-  <si>
     <t>803</t>
   </si>
   <si>
-    <t>Sat Jan 20 20:08:39 EST 2024</t>
-  </si>
-  <si>
     <t>816</t>
   </si>
   <si>
-    <t>Sat Jan 20 20:16:16 EST 2024</t>
-  </si>
-  <si>
     <t>778</t>
   </si>
   <si>
-    <t>Sat Jan 20 20:21:39 EST 2024</t>
-  </si>
-  <si>
     <t>779</t>
   </si>
   <si>
-    <t>Sat Jan 20 20:24:16 EST 2024</t>
-  </si>
-  <si>
     <t>780</t>
   </si>
   <si>
-    <t>Sat Jan 20 20:26:56 EST 2024</t>
-  </si>
-  <si>
     <t>781</t>
   </si>
   <si>
-    <t>Sat Jan 20 20:29:31 EST 2024</t>
-  </si>
-  <si>
     <t>782</t>
   </si>
   <si>
-    <t>Sat Jan 20 20:35:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 20 20:38:06 EST 2024</t>
-  </si>
-  <si>
     <t>804</t>
   </si>
   <si>
     <t>805</t>
   </si>
   <si>
-    <t>Sat Jan 20 20:44:14 EST 2024</t>
-  </si>
-  <si>
     <t>806</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:01:16 EST 2024</t>
-  </si>
-  <si>
     <t>798</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:08:09 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 20 21:10:00 EST 2024</t>
-  </si>
-  <si>
     <t>809</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:12:42 EST 2024</t>
-  </si>
-  <si>
     <t>810</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:14:53 EST 2024</t>
-  </si>
-  <si>
     <t>811</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:19:25 EST 2024</t>
-  </si>
-  <si>
     <t>812</t>
   </si>
   <si>
     <t>813</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:25:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 20 21:36:32 EST 2024</t>
-  </si>
-  <si>
     <t>814</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:39:28 EST 2024</t>
-  </si>
-  <si>
     <t>815</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:42:19 EST 2024</t>
-  </si>
-  <si>
     <t>817</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:44:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 20 21:47:56 EST 2024</t>
-  </si>
-  <si>
     <t>702</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:52:47 EST 2024</t>
-  </si>
-  <si>
     <t>703</t>
   </si>
   <si>
-    <t>Sat Jan 20 21:57:40 EST 2024</t>
-  </si>
-  <si>
     <t>708</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:45:34 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:46:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:47:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:48:19 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:49:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:50:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:51:06 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:52:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:52:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:53:51 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:54:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:55:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:56:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:57:36 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:58:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 18:59:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:00:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:01:22 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:03:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:04:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:05:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:06:41 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:07:36 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:08:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:09:29 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:10:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:11:19 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:12:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:13:09 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:14:06 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:15:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:15:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:16:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:17:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:18:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:19:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:20:34 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:21:29 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:22:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:23:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:24:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:25:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:26:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:28:34 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:29:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:30:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:31:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:32:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:33:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:34:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:34:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:35:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:36:49 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:37:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:38:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:41:07 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:42:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:42:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:43:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:44:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:45:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:46:40 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:47:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:48:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:49:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:50:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:51:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:53:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:54:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:55:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:56:27 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:57:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:58:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 19:59:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 20:00:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 20:01:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 20:01:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 20:02:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 20:03:42 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 20:04:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 20:05:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 20:06:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 20:07:27 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Jan 25 20:08:27 EST 2024</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:14:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:15:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:16:51 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:17:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:18:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:19:40 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:20:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:21:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:22:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:23:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:24:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:25:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:26:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:27:09 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:28:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:29:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:29:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:30:49 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:31:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:32:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:33:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:34:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:35:31 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:36:27 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:37:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:38:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:39:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:40:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:41:07 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:42:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:42:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:43:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:44:49 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:45:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:46:41 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:47:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:48:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:49:29 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:50:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:51:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:52:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:53:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:54:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:55:06 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:56:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:56:58 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:57:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:58:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 22:59:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:00:41 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:01:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:02:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:03:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:04:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:05:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:06:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:07:11 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:08:07 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:09:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:09:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:10:55 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:11:51 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:12:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:13:42 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:14:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:15:36 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:16:34 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:17:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Sat Jan 27 23:18:30 EST 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -598,19 +878,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -627,10 +907,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -665,7 +945,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -717,7 +997,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -828,21 +1108,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -859,7 +1139,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -911,15 +1191,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:J1"/>
@@ -927,17 +1207,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="32.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="32.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
+    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -966,10 +1246,10 @@
         <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -977,7 +1257,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -989,16 +1269,16 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1006,7 +1286,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1018,16 +1298,16 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1035,7 +1315,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1047,7 +1327,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -1056,10 +1336,10 @@
         <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1067,7 +1347,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1079,7 +1359,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>22</v>
@@ -1088,10 +1368,10 @@
         <v>32</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1099,7 +1379,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1111,7 +1391,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>23</v>
@@ -1120,10 +1400,10 @@
         <v>32</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1131,7 +1411,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1143,7 +1423,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
@@ -1152,16 +1432,16 @@
         <v>32</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1169,23 +1449,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="37.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1208,10 +1488,10 @@
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1219,7 +1499,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>191</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1231,10 +1511,10 @@
         <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1242,7 +1522,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1254,10 +1534,10 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1265,7 +1545,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>193</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1277,10 +1557,10 @@
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1288,7 +1568,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>194</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1303,10 +1583,10 @@
         <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1314,7 +1594,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>195</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1329,10 +1609,10 @@
         <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1340,7 +1620,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1352,7 +1632,7 @@
         <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1360,7 +1640,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1372,7 +1652,7 @@
         <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1380,7 +1660,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>198</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1392,7 +1672,7 @@
         <v>28</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1400,7 +1680,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>199</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1412,7 +1692,7 @@
         <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1420,7 +1700,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>200</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1435,7 +1715,7 @@
         <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1443,7 +1723,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>201</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1458,7 +1738,7 @@
         <v>32</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1466,7 +1746,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>202</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1475,13 +1755,19 @@
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>203</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1489,7 +1775,10 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1497,7 +1786,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>204</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1506,10 +1795,10 @@
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1517,7 +1806,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>205</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1526,10 +1815,13 @@
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1537,7 +1829,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1546,13 +1838,10 @@
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1560,7 +1849,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>207</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1569,10 +1858,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1580,7 +1869,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>208</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -1589,34 +1878,14 @@
         <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1624,8 +1893,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C7"/>
@@ -1633,15 +1902,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1806,7 +2075,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1814,25 +2083,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:I55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="1" collapsed="1"/>
-    <col min="9" max="9" width="23.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="8" max="8" style="1" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.140625" collapsed="true"/>
+    <col min="10" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1858,10 +2127,10 @@
         <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1869,7 +2138,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>209</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1884,7 +2153,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1892,7 +2161,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>210</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1910,7 +2179,7 @@
         <v>32</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1918,7 +2187,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>211</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1936,7 +2205,7 @@
         <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1944,7 +2213,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>212</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1962,7 +2231,7 @@
         <v>32</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1970,7 +2239,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>213</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1988,7 +2257,7 @@
         <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1996,7 +2265,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>214</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2011,7 +2280,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2019,7 +2288,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>215</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2037,7 +2306,7 @@
         <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2045,7 +2314,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>216</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2063,7 +2332,7 @@
         <v>32</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2071,7 +2340,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>217</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2089,7 +2358,7 @@
         <v>32</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2097,7 +2366,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>218</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2115,7 +2384,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2123,7 +2392,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>219</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2138,7 +2407,7 @@
         <v>31</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2146,7 +2415,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>220</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2164,7 +2433,7 @@
         <v>32</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2172,7 +2441,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>221</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2190,7 +2459,7 @@
         <v>32</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2198,7 +2467,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>222</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2216,7 +2485,7 @@
         <v>32</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2224,7 +2493,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>223</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2242,7 +2511,7 @@
         <v>32</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2250,7 +2519,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>224</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2259,13 +2528,13 @@
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2273,7 +2542,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>225</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2288,7 +2557,7 @@
         <v>18</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2296,7 +2565,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>226</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2311,7 +2580,7 @@
         <v>18</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>140</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2319,7 +2588,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>227</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2334,10 +2603,16 @@
         <v>18</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>228</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
       </c>
@@ -2345,18 +2620,21 @@
         <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H21" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>229</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2365,13 +2643,13 @@
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2379,7 +2657,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>230</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2388,13 +2666,13 @@
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2402,7 +2680,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>148</v>
+        <v>231</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2411,13 +2689,13 @@
         <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2425,7 +2703,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
+        <v>232</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2434,13 +2712,16 @@
         <v>16</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G25" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="H25" s="1" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2448,7 +2729,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>153</v>
+        <v>233</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2457,16 +2738,13 @@
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>152</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2474,7 +2752,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>154</v>
+        <v>234</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2483,13 +2761,13 @@
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2497,7 +2775,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>156</v>
+        <v>235</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2506,13 +2784,13 @@
         <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2520,7 +2798,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>158</v>
+        <v>236</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2529,13 +2807,13 @@
         <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2543,7 +2821,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>160</v>
+        <v>237</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2552,16 +2830,22 @@
         <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>238</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
@@ -2569,16 +2853,22 @@
         <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>239</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
       </c>
@@ -2586,16 +2876,22 @@
         <v>16</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>240</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
       </c>
@@ -2603,16 +2899,22 @@
         <v>16</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>241</v>
+      </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
       </c>
@@ -2620,13 +2922,22 @@
         <v>16</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>242</v>
+      </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
       </c>
@@ -2634,16 +2945,22 @@
         <v>16</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>243</v>
+      </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
       </c>
@@ -2651,16 +2968,22 @@
         <v>16</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>244</v>
+      </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
       </c>
@@ -2668,16 +2991,25 @@
         <v>16</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="G37" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="H37" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>245</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
       </c>
@@ -2685,16 +3017,22 @@
         <v>16</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" t="s">
+        <v>246</v>
+      </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
       </c>
@@ -2702,19 +3040,22 @@
         <v>16</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="H39" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>247</v>
+      </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
       </c>
@@ -2722,16 +3063,22 @@
         <v>16</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" t="s">
+        <v>248</v>
+      </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
       </c>
@@ -2739,16 +3086,22 @@
         <v>16</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" t="s">
+        <v>249</v>
+      </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
       </c>
@@ -2756,16 +3109,22 @@
         <v>16</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" t="s">
+        <v>250</v>
+      </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
       </c>
@@ -2773,16 +3132,22 @@
         <v>16</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" t="s">
+        <v>251</v>
+      </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
       </c>
@@ -2790,16 +3155,22 @@
         <v>16</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" t="s">
+        <v>252</v>
+      </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
       </c>
@@ -2807,16 +3178,22 @@
         <v>16</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" t="s">
+        <v>253</v>
+      </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
       </c>
@@ -2824,16 +3201,22 @@
         <v>16</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" t="s">
+        <v>254</v>
+      </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
       </c>
@@ -2841,13 +3224,22 @@
         <v>16</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" t="s">
+        <v>255</v>
+      </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
       </c>
@@ -2855,16 +3247,22 @@
         <v>16</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" t="s">
+        <v>256</v>
+      </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
       </c>
@@ -2872,16 +3270,25 @@
         <v>16</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="G49" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="H49" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" t="s">
+        <v>257</v>
+      </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
       </c>
@@ -2889,16 +3296,22 @@
         <v>16</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" t="s">
+        <v>258</v>
+      </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
       </c>
@@ -2906,16 +3319,22 @@
         <v>16</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" t="s">
+        <v>259</v>
+      </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
       </c>
@@ -2923,72 +3342,18 @@
         <v>16</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="H52" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C53" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C54" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C55" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>159</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2996,8 +3361,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3005,15 +3370,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3044,7 +3409,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3115,7 +3480,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3123,23 +3488,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3162,10 +3527,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3173,7 +3538,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3185,10 +3550,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>162</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3216,7 +3581,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3231,7 +3596,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>164</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3239,7 +3604,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>184</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3254,7 +3619,7 @@
         <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>164</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3262,7 +3627,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>185</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3277,30 +3642,256 @@
         <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>164</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F7" sqref="F7:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3320,7 +3911,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3328,165 +3919,30 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>181</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Executed RAD UI Test Cases.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="344">
   <si>
     <t>Result</t>
   </si>
@@ -823,6 +823,258 @@
   </si>
   <si>
     <t>Sat Jan 27 23:18:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:39:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:40:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:41:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:42:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:43:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:43:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:44:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:45:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:46:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:47:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:48:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:48:55 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:49:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:50:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:51:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:52:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:53:06 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:53:55 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:54:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:55:34 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:57:06 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:57:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:58:46 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 22:59:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:00:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:01:14 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:02:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:02:52 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:03:40 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:04:29 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:05:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:06:07 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:06:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:07:46 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:08:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:09:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:10:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:11:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:11:51 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:12:40 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:13:29 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:14:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:15:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:15:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:16:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:17:34 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:18:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:19:11 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:20:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:20:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:21:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:22:27 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:23:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:24:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:24:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:25:42 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:26:31 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:27:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:28:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:28:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:29:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:30:34 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:31:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:32:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:33:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:33:49 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:34:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:35:27 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:36:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:37:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:37:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:38:42 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:39:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:40:19 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:41:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:41:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:42:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:43:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:44:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:45:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:45:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:46:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:47:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Jan 30 23:48:29 EST 2024</t>
   </si>
 </sst>
 </file>
@@ -1257,7 +1509,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>260</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1286,7 +1538,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>261</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1315,7 +1567,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>262</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1347,7 +1599,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1379,7 +1631,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>264</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1411,7 +1663,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>265</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1499,7 +1751,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>266</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1522,7 +1774,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>267</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1545,7 +1797,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>268</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1568,7 +1820,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>194</v>
+        <v>269</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1594,7 +1846,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>195</v>
+        <v>270</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1620,7 +1872,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>271</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1640,7 +1892,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>272</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1660,7 +1912,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>273</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1680,7 +1932,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>199</v>
+        <v>274</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1700,7 +1952,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>275</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1723,7 +1975,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>201</v>
+        <v>276</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1746,7 +1998,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>202</v>
+        <v>277</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1766,7 +2018,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>203</v>
+        <v>278</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1783,10 +2035,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>204</v>
+        <v>279</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1806,7 +2058,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>205</v>
+        <v>280</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1829,7 +2081,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>206</v>
+        <v>281</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1849,7 +2101,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>207</v>
+        <v>282</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1869,7 +2121,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>283</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2138,7 +2390,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>284</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2161,7 +2413,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>285</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2187,7 +2439,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>286</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2213,7 +2465,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>287</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2239,7 +2491,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>288</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2265,7 +2517,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>289</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2288,7 +2540,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>290</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2314,7 +2566,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>216</v>
+        <v>291</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2340,7 +2592,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>292</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2366,7 +2618,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>218</v>
+        <v>293</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2392,7 +2644,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>219</v>
+        <v>294</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2415,7 +2667,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2441,7 +2693,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>221</v>
+        <v>296</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2467,7 +2719,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>297</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2493,7 +2745,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>223</v>
+        <v>298</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2519,7 +2771,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>224</v>
+        <v>299</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2542,7 +2794,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2565,7 +2817,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>226</v>
+        <v>301</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2588,7 +2840,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>227</v>
+        <v>302</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2611,7 +2863,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>228</v>
+        <v>303</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2634,7 +2886,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2657,7 +2909,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>230</v>
+        <v>305</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2680,7 +2932,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2703,7 +2955,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>232</v>
+        <v>307</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2729,7 +2981,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>233</v>
+        <v>308</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2752,7 +3004,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2775,7 +3027,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>235</v>
+        <v>310</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2798,7 +3050,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>236</v>
+        <v>311</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2821,7 +3073,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>237</v>
+        <v>312</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2844,7 +3096,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>238</v>
+        <v>313</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2867,7 +3119,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>239</v>
+        <v>314</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2890,7 +3142,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>240</v>
+        <v>315</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2913,7 +3165,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>241</v>
+        <v>316</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2936,7 +3188,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>242</v>
+        <v>317</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -2959,7 +3211,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>243</v>
+        <v>318</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -2982,7 +3234,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>244</v>
+        <v>319</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3008,7 +3260,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>245</v>
+        <v>320</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3031,7 +3283,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>246</v>
+        <v>321</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3054,7 +3306,7 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>247</v>
+        <v>322</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3077,7 +3329,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>248</v>
+        <v>323</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3100,7 +3352,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>249</v>
+        <v>324</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3123,7 +3375,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>250</v>
+        <v>325</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3146,7 +3398,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>251</v>
+        <v>326</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3169,7 +3421,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>252</v>
+        <v>327</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3192,7 +3444,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>253</v>
+        <v>328</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3215,7 +3467,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>254</v>
+        <v>329</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3238,7 +3490,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>255</v>
+        <v>330</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3261,7 +3513,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>256</v>
+        <v>331</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3287,7 +3539,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>257</v>
+        <v>332</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3310,7 +3562,7 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>258</v>
+        <v>333</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3333,7 +3585,7 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>259</v>
+        <v>334</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3538,7 +3790,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>336</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3581,7 +3833,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>337</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3604,7 +3856,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>338</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3627,7 +3879,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>339</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3731,7 +3983,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>340</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3774,7 +4026,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>341</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3797,7 +4049,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>342</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3820,7 +4072,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>343</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3919,7 +4171,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>335</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Updated RAD Phase 3 Test Cases and test data for Estate Tax.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{7BC77991-A6A2-41DD-B0EC-EB4D825CD7A3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1C3E15-37AB-48B6-BE0F-56D68D73D6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="7" windowHeight="14010" windowWidth="24525" xWindow="1680" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="2580"/>
+    <workbookView xWindow="2220" yWindow="2325" windowWidth="24525" windowHeight="14010" activeTab="7" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
-    <sheet name="Existing" r:id="rId2" sheetId="2"/>
-    <sheet name="Extension" r:id="rId3" sheetId="3"/>
-    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
-    <sheet name="Personal" r:id="rId5" sheetId="5"/>
-    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
-    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
-    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
+    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
+    <sheet name="Existing" sheetId="2" r:id="rId2"/>
+    <sheet name="Extension" sheetId="3" r:id="rId3"/>
+    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
+    <sheet name="Personal" sheetId="5" r:id="rId5"/>
+    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
+    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
+    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="192">
   <si>
     <t>Result</t>
   </si>
@@ -363,468 +363,6 @@
     <t>708</t>
   </si>
   <si>
-    <t>Thu Jan 25 18:45:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:46:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:47:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:48:19 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:49:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:50:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:51:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:52:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:52:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:53:51 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:54:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:55:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:56:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:57:36 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:58:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 18:59:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:00:24 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:01:22 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:03:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:04:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:05:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:06:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:07:36 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:08:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:09:29 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:10:24 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:11:19 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:12:13 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:13:09 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:14:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:15:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:15:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:16:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:17:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:18:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:19:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:20:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:21:29 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:22:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:23:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:24:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:25:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:26:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:28:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:29:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:30:21 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:31:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:32:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:33:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:34:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:34:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:35:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:36:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:37:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:38:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:41:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:42:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:42:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:43:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:44:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:45:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:46:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:47:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:48:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:49:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:50:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:51:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:53:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:54:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:55:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:56:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:57:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:58:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 19:59:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 20:00:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 20:01:02 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 20:01:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 20:02:50 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 20:03:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 20:04:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 20:05:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 20:06:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 20:07:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Jan 25 20:08:27 EST 2024</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:14:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:15:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:16:51 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:17:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:18:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:19:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:20:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:21:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:22:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:23:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:24:21 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:25:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:26:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:27:09 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:28:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:29:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:29:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:30:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:31:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:32:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:33:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:34:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:35:31 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:36:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:37:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:38:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:39:13 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:40:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:41:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:42:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:42:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:43:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:44:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:45:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:46:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:47:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:48:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:49:29 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:50:24 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:51:21 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:52:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:53:13 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:54:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:55:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:56:02 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:56:58 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:57:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:58:50 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 22:59:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:00:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:01:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:02:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:03:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:04:24 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:05:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:06:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:07:11 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:08:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:09:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:09:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:10:55 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:11:51 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:12:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:13:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:14:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:15:36 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:16:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:17:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Jan 27 23:18:30 EST 2024</t>
-  </si>
-  <si>
     <t>Tue Jan 30 22:39:43 EST 2024</t>
   </si>
   <si>
@@ -1050,15 +588,6 @@
     <t>Tue Jan 30 23:41:08 EST 2024</t>
   </si>
   <si>
-    <t>Tue Jan 30 23:41:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:42:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:43:32 EST 2024</t>
-  </si>
-  <si>
     <t>Tue Jan 30 23:44:18 EST 2024</t>
   </si>
   <si>
@@ -1075,13 +604,27 @@
   </si>
   <si>
     <t>Tue Jan 30 23:48:29 EST 2024</t>
+  </si>
+  <si>
+    <t>Fri Feb 02 15:32:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Fri Feb 02 15:33:42 EST 2024</t>
+  </si>
+  <si>
+    <t>Fri Feb 02 16:05:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Fri Feb 02 16:06:36 EST 2024</t>
+  </si>
+  <si>
+    <t>Fri Feb 02 16:07:25 EST 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1130,19 +673,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1159,10 +702,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1197,7 +740,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1249,7 +792,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1360,21 +903,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1391,7 +934,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1443,15 +986,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:J1"/>
@@ -1459,17 +1002,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
-    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1509,7 +1052,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1538,7 +1081,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1567,7 +1110,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>262</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1599,7 +1142,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>263</v>
+        <v>109</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1631,7 +1174,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>264</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1663,7 +1206,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>265</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1692,8 +1235,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1701,8 +1244,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
@@ -1710,14 +1253,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="37.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1751,7 +1294,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1774,7 +1317,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>113</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1797,7 +1340,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>114</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1820,7 +1363,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>115</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1846,7 +1389,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>116</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1872,7 +1415,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1892,7 +1435,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>272</v>
+        <v>118</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1912,7 +1455,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>273</v>
+        <v>119</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1932,7 +1475,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>274</v>
+        <v>120</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1952,7 +1495,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>121</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1975,7 +1518,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>276</v>
+        <v>122</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1998,7 +1541,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>277</v>
+        <v>123</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2018,7 +1561,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>278</v>
+        <v>124</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2038,7 +1581,7 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>279</v>
+        <v>125</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2058,7 +1601,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>280</v>
+        <v>126</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2081,7 +1624,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>281</v>
+        <v>127</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2101,7 +1644,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>282</v>
+        <v>128</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2121,7 +1664,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>283</v>
+        <v>129</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2137,7 +1680,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2145,8 +1688,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C7"/>
@@ -2154,15 +1697,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2327,7 +1870,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2335,25 +1878,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:J52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="8" max="8" style="1" width="9.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.140625" collapsed="true"/>
-    <col min="10" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.140625" style="1" collapsed="1"/>
+    <col min="9" max="9" width="23.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2390,7 +1933,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>284</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2413,7 +1956,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>285</v>
+        <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2439,7 +1982,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>286</v>
+        <v>132</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2465,7 +2008,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>287</v>
+        <v>133</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2491,7 +2034,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>288</v>
+        <v>134</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2517,7 +2060,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>289</v>
+        <v>135</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2540,7 +2083,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>290</v>
+        <v>136</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2566,7 +2109,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>291</v>
+        <v>137</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2592,7 +2135,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>292</v>
+        <v>138</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2618,7 +2161,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>293</v>
+        <v>139</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2644,7 +2187,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>294</v>
+        <v>140</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2667,7 +2210,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>295</v>
+        <v>141</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2693,7 +2236,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>296</v>
+        <v>142</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2719,7 +2262,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>297</v>
+        <v>143</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2745,7 +2288,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>298</v>
+        <v>144</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2771,7 +2314,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>299</v>
+        <v>145</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2794,7 +2337,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>300</v>
+        <v>146</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2817,7 +2360,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>301</v>
+        <v>147</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2840,7 +2383,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>302</v>
+        <v>148</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2863,7 +2406,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>303</v>
+        <v>149</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2886,7 +2429,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>304</v>
+        <v>150</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2909,7 +2452,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>305</v>
+        <v>151</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2932,7 +2475,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>306</v>
+        <v>152</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2955,7 +2498,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>307</v>
+        <v>153</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2981,7 +2524,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>308</v>
+        <v>154</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -3004,7 +2547,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>309</v>
+        <v>155</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -3027,7 +2570,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>310</v>
+        <v>156</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -3050,7 +2593,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>311</v>
+        <v>157</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -3073,7 +2616,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>312</v>
+        <v>158</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -3096,7 +2639,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>313</v>
+        <v>159</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -3119,7 +2662,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>314</v>
+        <v>160</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -3142,7 +2685,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>315</v>
+        <v>161</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -3165,7 +2708,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>316</v>
+        <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -3188,7 +2731,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>317</v>
+        <v>163</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -3211,7 +2754,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>318</v>
+        <v>164</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -3234,7 +2777,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>319</v>
+        <v>165</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3260,7 +2803,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>320</v>
+        <v>166</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3283,7 +2826,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>321</v>
+        <v>167</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3306,7 +2849,7 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>322</v>
+        <v>168</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3329,7 +2872,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>323</v>
+        <v>169</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3352,7 +2895,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>324</v>
+        <v>170</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3375,7 +2918,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>325</v>
+        <v>171</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3398,7 +2941,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>326</v>
+        <v>172</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3421,7 +2964,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>327</v>
+        <v>173</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3444,7 +2987,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>328</v>
+        <v>174</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3467,7 +3010,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>329</v>
+        <v>175</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3490,7 +3033,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>330</v>
+        <v>176</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3513,7 +3056,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>331</v>
+        <v>177</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3539,7 +3082,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>332</v>
+        <v>178</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3562,7 +3105,7 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>333</v>
+        <v>179</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3585,7 +3128,7 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>334</v>
+        <v>180</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3605,7 +3148,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3613,8 +3156,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3622,15 +3165,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3732,7 +3275,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3740,23 +3283,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F9"/>
+      <selection activeCell="C4" sqref="C4:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3790,7 +3333,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>336</v>
+        <v>189</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3833,7 +3376,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>337</v>
+        <v>190</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3856,7 +3399,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>338</v>
+        <v>181</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3879,7 +3422,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>339</v>
+        <v>182</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3898,6 +3441,15 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
@@ -3909,6 +3461,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3920,6 +3475,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3931,28 +3489,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F9"/>
+      <selection activeCell="A7" sqref="A7:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3983,7 +3541,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
+        <v>183</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4026,7 +3584,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>341</v>
+        <v>184</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -4049,7 +3607,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>342</v>
+        <v>185</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4072,7 +3630,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>343</v>
+        <v>186</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4090,60 +3648,27 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4171,7 +3696,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>335</v>
+        <v>187</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4187,6 +3712,15 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
@@ -4195,6 +3729,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Executed RAD in QA2.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="369">
   <si>
     <t>Result</t>
   </si>
@@ -886,6 +886,270 @@
   </si>
   <si>
     <t>Fri Feb 02 23:37:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:19:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:20:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:21:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:22:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:23:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:24:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:25:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:26:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:27:06 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:27:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:28:52 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:29:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:30:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:31:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:32:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:33:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:34:22 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:35:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:36:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:37:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:38:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:38:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:39:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:40:41 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:41:36 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:42:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:43:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:44:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:45:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:46:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:46:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:47:46 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:48:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:49:31 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:50:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:51:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:52:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:53:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:53:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:54:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:55:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:56:31 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:57:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:58:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 16:59:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:00:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:00:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:01:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:02:40 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:03:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:04:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:05:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:06:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:07:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:07:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:08:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:09:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:10:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:11:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:12:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:13:11 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:14:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:14:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:15:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:16:40 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:17:34 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:18:27 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:19:19 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:20:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:21:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:21:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:22:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:23:42 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:24:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:25:27 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:26:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:27:11 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:28:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:28:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:29:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:30:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:31:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:32:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:33:14 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:34:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:35:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:35:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Feb 06 17:36:54 EST 2024</t>
   </si>
 </sst>
 </file>
@@ -1320,7 +1584,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>281</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1349,7 +1613,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>282</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1378,7 +1642,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>283</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1410,7 +1674,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>284</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1442,7 +1706,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>285</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1474,7 +1738,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>286</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1562,7 +1826,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>287</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1585,7 +1849,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>288</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1608,7 +1872,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>201</v>
+        <v>289</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1631,7 +1895,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>202</v>
+        <v>290</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1657,7 +1921,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>203</v>
+        <v>291</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1683,7 +1947,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>292</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1703,7 +1967,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
+        <v>293</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1723,7 +1987,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
+        <v>294</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1743,7 +2007,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>295</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1763,7 +2027,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>296</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1786,7 +2050,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>209</v>
+        <v>297</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1809,7 +2073,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>298</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1829,7 +2093,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>211</v>
+        <v>299</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1849,7 +2113,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>300</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1869,7 +2133,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>301</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1892,7 +2156,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>214</v>
+        <v>302</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1912,7 +2176,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>303</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1932,7 +2196,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>216</v>
+        <v>304</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2201,7 +2465,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>305</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2224,7 +2488,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>218</v>
+        <v>306</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2250,7 +2514,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>307</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2276,7 +2540,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>308</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2302,7 +2566,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>309</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2328,7 +2592,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>310</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2351,7 +2615,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>223</v>
+        <v>311</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2377,7 +2641,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>224</v>
+        <v>312</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2403,7 +2667,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>313</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2429,7 +2693,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>226</v>
+        <v>314</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2455,7 +2719,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>227</v>
+        <v>315</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2478,7 +2742,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>228</v>
+        <v>316</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2504,7 +2768,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>229</v>
+        <v>317</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2530,7 +2794,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2556,7 +2820,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>231</v>
+        <v>319</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2582,7 +2846,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>232</v>
+        <v>320</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2605,7 +2869,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>233</v>
+        <v>321</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2628,7 +2892,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>234</v>
+        <v>322</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2651,7 +2915,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>235</v>
+        <v>323</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2674,7 +2938,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>236</v>
+        <v>324</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2697,7 +2961,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>237</v>
+        <v>325</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2720,7 +2984,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>238</v>
+        <v>326</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2743,7 +3007,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>239</v>
+        <v>327</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2766,7 +3030,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>240</v>
+        <v>328</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2792,7 +3056,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>241</v>
+        <v>329</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2815,7 +3079,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>242</v>
+        <v>330</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2838,7 +3102,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>243</v>
+        <v>331</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2861,7 +3125,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>244</v>
+        <v>332</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2884,7 +3148,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>245</v>
+        <v>333</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2907,7 +3171,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>246</v>
+        <v>334</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2930,7 +3194,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>247</v>
+        <v>335</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2953,7 +3217,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>336</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2976,7 +3240,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>249</v>
+        <v>337</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2999,7 +3263,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>250</v>
+        <v>338</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -3022,7 +3286,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -3045,7 +3309,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>252</v>
+        <v>340</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3071,7 +3335,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>253</v>
+        <v>341</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3094,7 +3358,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>254</v>
+        <v>342</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3117,7 +3381,7 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>255</v>
+        <v>343</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3140,7 +3404,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>256</v>
+        <v>344</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3163,7 +3427,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>257</v>
+        <v>345</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3186,7 +3450,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>258</v>
+        <v>346</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3209,7 +3473,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>259</v>
+        <v>347</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3232,7 +3496,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>260</v>
+        <v>348</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3255,7 +3519,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>261</v>
+        <v>349</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3278,7 +3542,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>262</v>
+        <v>350</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3301,7 +3565,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>263</v>
+        <v>351</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3324,7 +3588,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>264</v>
+        <v>352</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3350,7 +3614,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>265</v>
+        <v>353</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3373,7 +3637,7 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>266</v>
+        <v>354</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3396,7 +3660,7 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>267</v>
+        <v>355</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3601,7 +3865,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>358</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3644,7 +3908,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3667,7 +3931,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>272</v>
+        <v>360</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3690,7 +3954,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>273</v>
+        <v>361</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3713,7 +3977,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>274</v>
+        <v>362</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -3733,7 +3997,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>275</v>
+        <v>363</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -3753,7 +4017,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>276</v>
+        <v>364</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -3821,7 +4085,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>365</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3864,7 +4128,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>278</v>
+        <v>366</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3887,7 +4151,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>279</v>
+        <v>367</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3910,7 +4174,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>280</v>
+        <v>368</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3976,7 +4240,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>356</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3996,7 +4260,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>357</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Added VSP and VT test cases for No CC and No ACH.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="457">
   <si>
     <t>Result</t>
   </si>
@@ -1150,6 +1150,270 @@
   </si>
   <si>
     <t>Tue Feb 06 17:36:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:33:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:33:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:34:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:35:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:35:49 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:36:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:37:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:37:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:38:29 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:39:11 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:39:51 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:40:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:41:19 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:41:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:42:40 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:43:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:43:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:44:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:45:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:46:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:46:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:47:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:47:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:48:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:49:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:49:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:50:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:51:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:51:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:52:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:53:14 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:53:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:54:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:55:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:55:51 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:56:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:57:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:57:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:58:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:59:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:59:46 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:00:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:01:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:01:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:02:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:03:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:03:41 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:04:19 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:04:58 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:05:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:06:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:06:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:07:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:08:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:08:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:09:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:10:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:10:52 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:11:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:12:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:13:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:13:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:14:22 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:15:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:15:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:16:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:17:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:17:42 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:18:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:19:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:19:46 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:20:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:21:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:21:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:22:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:23:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:23:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:24:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:25:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:25:49 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:26:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:27:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:27:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:28:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:28:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:29:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:30:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:31:23 EST 2024</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1848,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>369</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1613,7 +1877,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>370</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1642,7 +1906,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>283</v>
+        <v>371</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1674,7 +1938,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>284</v>
+        <v>372</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1706,7 +1970,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1738,7 +2002,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>374</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1826,7 +2090,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>287</v>
+        <v>375</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1849,7 +2113,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>376</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1872,7 +2136,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>289</v>
+        <v>377</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1895,7 +2159,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>290</v>
+        <v>378</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1921,7 +2185,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>291</v>
+        <v>379</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1947,7 +2211,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>292</v>
+        <v>380</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1967,7 +2231,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>293</v>
+        <v>381</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1987,7 +2251,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>294</v>
+        <v>382</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2007,7 +2271,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>295</v>
+        <v>383</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2027,7 +2291,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>296</v>
+        <v>384</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2050,7 +2314,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>297</v>
+        <v>385</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2073,7 +2337,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>298</v>
+        <v>386</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2093,7 +2357,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>299</v>
+        <v>387</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2113,7 +2377,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>300</v>
+        <v>388</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2133,7 +2397,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>301</v>
+        <v>389</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2156,7 +2420,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>302</v>
+        <v>390</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2176,7 +2440,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>303</v>
+        <v>391</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2196,7 +2460,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>304</v>
+        <v>392</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2465,7 +2729,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>305</v>
+        <v>393</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2488,7 +2752,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>306</v>
+        <v>394</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2514,7 +2778,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>307</v>
+        <v>395</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2540,7 +2804,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>308</v>
+        <v>396</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2566,7 +2830,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>309</v>
+        <v>397</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2592,7 +2856,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>310</v>
+        <v>398</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2615,7 +2879,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>311</v>
+        <v>399</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2641,7 +2905,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>312</v>
+        <v>400</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2667,7 +2931,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>313</v>
+        <v>401</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2693,7 +2957,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>314</v>
+        <v>402</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2719,7 +2983,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>315</v>
+        <v>403</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2742,7 +3006,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>316</v>
+        <v>404</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2768,7 +3032,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>317</v>
+        <v>405</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2794,7 +3058,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2820,7 +3084,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>319</v>
+        <v>407</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2846,7 +3110,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>320</v>
+        <v>408</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2869,7 +3133,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>321</v>
+        <v>409</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2892,7 +3156,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>322</v>
+        <v>410</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2915,7 +3179,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>323</v>
+        <v>411</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2938,7 +3202,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>324</v>
+        <v>412</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2961,7 +3225,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>325</v>
+        <v>413</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2984,7 +3248,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>326</v>
+        <v>414</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -3007,7 +3271,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>327</v>
+        <v>415</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -3030,7 +3294,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>328</v>
+        <v>416</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -3056,7 +3320,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>329</v>
+        <v>417</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -3079,7 +3343,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>330</v>
+        <v>418</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -3102,7 +3366,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>331</v>
+        <v>419</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -3125,7 +3389,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>332</v>
+        <v>420</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -3148,7 +3412,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>333</v>
+        <v>421</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -3171,7 +3435,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>334</v>
+        <v>422</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -3194,7 +3458,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>335</v>
+        <v>423</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -3217,7 +3481,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>336</v>
+        <v>424</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -3240,7 +3504,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>337</v>
+        <v>425</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -3263,7 +3527,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>338</v>
+        <v>426</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -3286,7 +3550,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>339</v>
+        <v>427</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -3309,7 +3573,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>340</v>
+        <v>428</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3335,7 +3599,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>341</v>
+        <v>429</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3358,7 +3622,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>342</v>
+        <v>430</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3381,7 +3645,7 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>343</v>
+        <v>431</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3404,7 +3668,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>344</v>
+        <v>432</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3427,7 +3691,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>345</v>
+        <v>433</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3450,7 +3714,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>346</v>
+        <v>434</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3473,7 +3737,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>347</v>
+        <v>435</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3496,7 +3760,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>348</v>
+        <v>436</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3519,7 +3783,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>349</v>
+        <v>437</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3542,7 +3806,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>350</v>
+        <v>438</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3565,7 +3829,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>351</v>
+        <v>439</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3588,7 +3852,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>352</v>
+        <v>440</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3614,7 +3878,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>353</v>
+        <v>441</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3637,7 +3901,7 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>354</v>
+        <v>442</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3660,7 +3924,7 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>355</v>
+        <v>443</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3865,7 +4129,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3908,7 +4172,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>359</v>
+        <v>447</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3931,7 +4195,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3954,7 +4218,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>361</v>
+        <v>449</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3977,7 +4241,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>362</v>
+        <v>450</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -3997,7 +4261,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>363</v>
+        <v>451</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -4017,7 +4281,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>364</v>
+        <v>452</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -4085,7 +4349,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>453</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4128,7 +4392,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>366</v>
+        <v>454</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -4151,7 +4415,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>367</v>
+        <v>455</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4174,7 +4438,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>368</v>
+        <v>456</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4240,7 +4504,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>356</v>
+        <v>444</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4260,7 +4524,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>357</v>
+        <v>445</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Updated RAD Test Cases for Filing Year drop down and MD CRN changes.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{9D1C3E15-37AB-48B6-BE0F-56D68D73D6D9}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{8E109D1F-1318-4B89-8487-7D4E57AC6BB5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="7" windowHeight="14010" windowWidth="24525" xWindow="2220" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="2325"/>
+    <workbookView activeTab="3" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" r:id="rId1" sheetId="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="247">
   <si>
     <t>Result</t>
   </si>
@@ -363,1057 +363,427 @@
     <t>708</t>
   </si>
   <si>
-    <t>Tue Jan 30 22:39:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:40:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:41:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:42:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:43:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:43:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:44:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:45:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:46:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:47:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:48:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:48:55 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:49:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:50:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:51:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:52:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:53:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:53:55 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:54:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:55:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:57:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:57:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:58:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 22:59:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:00:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:01:14 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:02:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:02:52 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:03:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:04:29 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:05:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:06:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:06:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:07:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:08:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:09:24 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:10:13 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:11:02 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:11:51 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:12:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:13:29 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:14:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:15:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:15:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:16:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:17:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:18:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:19:11 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:20:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:20:50 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:21:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:22:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:23:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:24:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:24:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:25:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:26:31 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:27:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:28:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:28:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:29:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:30:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:31:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:32:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:33:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:33:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:34:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:35:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:36:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:37:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:37:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:38:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:39:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:40:19 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:41:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:44:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:45:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:45:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:46:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:47:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Jan 30 23:48:29 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 15:32:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 15:33:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 16:05:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 16:06:36 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 16:07:25 EST 2024</t>
+    <t>Wed Feb 07 23:33:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:33:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:34:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:35:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:35:49 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:36:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:37:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:37:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:38:29 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:39:11 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:39:51 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:40:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:41:19 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:41:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:42:40 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:43:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:43:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:44:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:45:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:46:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:46:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:47:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:47:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:48:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:49:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:49:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:50:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:51:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:51:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:52:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:53:14 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:53:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:54:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:55:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:55:51 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:56:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:57:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:57:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:58:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:59:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Wed Feb 07 23:59:46 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:00:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:01:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:01:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:02:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:03:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:03:41 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:04:19 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:04:58 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:05:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:06:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:06:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:07:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:08:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:08:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:09:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:10:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:10:52 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:11:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:12:18 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:13:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:13:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:14:22 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:15:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:15:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:16:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:17:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:17:42 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:18:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:19:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:19:46 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:20:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:21:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:21:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:22:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:23:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:23:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:24:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:25:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:25:49 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:26:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:27:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:27:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:28:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:28:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:29:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:30:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Thu Feb 08 00:31:23 EST 2024</t>
+  </si>
+  <si>
+    <t>CRN</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Fri Feb 02 22:26:11 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:27:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:27:50 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:28:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:29:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:30:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:31:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:31:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:32:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:33:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:34:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:35:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:36:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:36:58 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:37:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:38:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:39:29 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:40:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:41:09 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:41:58 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:42:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:43:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:44:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:45:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:46:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:46:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:47:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:48:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:49:24 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:50:13 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:51:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:51:52 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:52:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:53:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:54:19 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:55:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:55:58 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:56:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:57:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:58:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 22:59:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:00:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:00:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:01:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:02:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:03:22 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:04:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:05:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:05:50 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:06:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:07:29 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:08:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:09:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:09:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:10:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:11:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:12:24 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:13:13 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:14:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:14:52 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:15:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:16:31 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:17:21 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:18:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:18:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:19:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:20:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:21:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:22:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:23:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:23:55 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:24:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:25:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:26:22 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:27:11 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:28:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:28:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:29:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:30:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:31:13 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:32:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:32:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:33:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:34:22 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:35:11 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:36:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:36:58 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Feb 02 23:37:50 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:19:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:20:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:21:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:22:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:23:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:24:24 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:25:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:26:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:27:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:27:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:28:52 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:29:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:30:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:31:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:32:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:33:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:34:22 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:35:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:36:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:37:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:38:02 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:38:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:39:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:40:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:41:36 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:42:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:43:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:44:13 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:45:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:46:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:46:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:47:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:48:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:49:31 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:50:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:51:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:52:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:53:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:53:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:54:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:55:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:56:31 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:57:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:58:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 16:59:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:00:02 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:00:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:01:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:02:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:03:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:04:24 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:05:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:06:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:07:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:07:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:08:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:09:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:10:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:11:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:12:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:13:11 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:14:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:14:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:15:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:16:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:17:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:18:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:19:19 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:20:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:21:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:21:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:22:50 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:23:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:24:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:25:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:26:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:27:11 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:28:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:28:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:29:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:30:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:31:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:32:24 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:33:14 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:34:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:35:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:35:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Feb 06 17:36:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:33:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:33:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:34:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:35:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:35:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:36:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:37:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:37:50 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:38:29 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:39:11 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:39:51 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:40:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:41:19 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:41:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:42:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:43:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:43:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:44:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:45:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:46:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:46:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:47:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:47:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:48:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:49:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:49:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:50:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:51:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:51:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:52:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:53:14 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:53:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:54:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:55:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:55:51 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:56:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:57:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:57:50 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:58:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:59:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:59:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:00:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:01:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:01:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:02:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:03:02 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:03:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:04:19 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:04:58 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:05:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:06:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:06:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:07:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:08:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:08:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:09:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:10:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:10:52 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:11:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:12:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:13:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:13:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:14:22 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:15:02 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:15:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:16:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:17:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:17:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:18:21 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:19:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:19:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:20:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:21:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:21:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:22:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:23:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:23:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:24:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:25:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:25:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:26:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:27:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:27:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:28:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:28:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:29:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:30:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:31:23 EST 2024</t>
+    <t>Sun Feb 18 22:43:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:44:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:45:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:46:29 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:47:22 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:48:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:49:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:49:55 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:50:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:51:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:52:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:53:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:54:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:55:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:55:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:56:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:57:41 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:58:34 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 22:59:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:00:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:01:09 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:02:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:02:55 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:03:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:04:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:05:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:06:22 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:07:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:08:07 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:09:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:09:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:10:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:11:36 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:12:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:13:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:14:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:15:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:15:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:16:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:17:43 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:18:36 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:19:29 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:20:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:21:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:22:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:22:58 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:23:49 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:24:42 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:25:34 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:26:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Sun Feb 18 23:27:59 EST 2024</t>
   </si>
 </sst>
 </file>
@@ -1848,7 +1218,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1877,7 +1247,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>370</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1906,7 +1276,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>371</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1938,7 +1308,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>372</v>
+        <v>109</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1970,7 +1340,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>373</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2002,7 +1372,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>374</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2090,7 +1460,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>375</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2113,7 +1483,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>376</v>
+        <v>113</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2136,7 +1506,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>377</v>
+        <v>114</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2159,7 +1529,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>378</v>
+        <v>115</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2185,7 +1555,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>379</v>
+        <v>116</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2211,7 +1581,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>380</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2231,7 +1601,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>381</v>
+        <v>118</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2251,7 +1621,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>382</v>
+        <v>119</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2271,7 +1641,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>383</v>
+        <v>120</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2291,7 +1661,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>384</v>
+        <v>121</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2314,7 +1684,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>385</v>
+        <v>122</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2337,7 +1707,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>386</v>
+        <v>123</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2357,7 +1727,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>387</v>
+        <v>124</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2377,7 +1747,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>388</v>
+        <v>125</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2397,7 +1767,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>389</v>
+        <v>126</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2420,7 +1790,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>390</v>
+        <v>127</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2440,7 +1810,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>391</v>
+        <v>128</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2460,7 +1830,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>392</v>
+        <v>129</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2675,10 +2045,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,12 +2060,13 @@
     <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
     <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="8" max="8" style="1" width="9.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.140625" collapsed="true"/>
-    <col min="10" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="23.140625" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2718,18 +2089,21 @@
         <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>393</v>
+        <v>196</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2743,16 +2117,16 @@
       <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>394</v>
+        <v>197</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2769,16 +2143,16 @@
       <c r="G3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>395</v>
+        <v>198</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2795,16 +2169,16 @@
       <c r="G4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>396</v>
+        <v>199</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2821,16 +2195,16 @@
       <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>397</v>
+        <v>200</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2847,16 +2221,16 @@
       <c r="G6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>398</v>
+        <v>201</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2870,16 +2244,16 @@
       <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>399</v>
+        <v>202</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2896,16 +2270,16 @@
       <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>400</v>
+        <v>203</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2922,16 +2296,16 @@
       <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>401</v>
+        <v>204</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2948,16 +2322,16 @@
       <c r="G10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>402</v>
+        <v>205</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2974,16 +2348,16 @@
       <c r="G11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>403</v>
+        <v>206</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2997,16 +2371,16 @@
       <c r="F12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>404</v>
+        <v>207</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -3023,16 +2397,16 @@
       <c r="G13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>405</v>
+        <v>208</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -3049,16 +2423,16 @@
       <c r="G14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>406</v>
+        <v>209</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -3075,16 +2449,16 @@
       <c r="G15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>407</v>
+        <v>210</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -3101,16 +2475,16 @@
       <c r="G16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>408</v>
+        <v>211</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -3122,18 +2496,21 @@
         <v>48</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>409</v>
+        <v>212</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -3145,18 +2522,21 @@
         <v>29</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>410</v>
+        <v>213</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -3168,18 +2548,18 @@
         <v>25</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>411</v>
+        <v>214</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -3193,16 +2573,16 @@
       <c r="F20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>412</v>
+        <v>215</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -3214,18 +2594,18 @@
         <v>50</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>413</v>
+        <v>216</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -3237,18 +2617,21 @@
         <v>56</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="H22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>414</v>
+        <v>217</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -3260,18 +2643,18 @@
         <v>51</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>415</v>
+        <v>218</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -3283,18 +2666,18 @@
         <v>27</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>416</v>
+        <v>219</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -3306,21 +2689,21 @@
         <v>52</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -3332,18 +2715,18 @@
         <v>53</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>418</v>
+        <v>221</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -3357,16 +2740,16 @@
       <c r="F27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>419</v>
+        <v>222</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -3378,18 +2761,21 @@
         <v>28</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>420</v>
+        <v>223</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -3401,18 +2787,21 @@
         <v>48</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>421</v>
+        <v>224</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -3424,18 +2813,21 @@
         <v>29</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="H30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>422</v>
+        <v>225</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -3447,18 +2839,18 @@
         <v>25</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>423</v>
+        <v>226</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -3472,16 +2864,16 @@
       <c r="F32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>424</v>
+        <v>227</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -3493,18 +2885,18 @@
         <v>50</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>425</v>
+        <v>228</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -3516,18 +2908,21 @@
         <v>56</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>426</v>
+        <v>229</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -3539,18 +2934,18 @@
         <v>51</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>427</v>
+        <v>230</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -3562,18 +2957,18 @@
         <v>27</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>428</v>
+        <v>231</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3585,21 +2980,21 @@
         <v>52</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>429</v>
+        <v>232</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3611,18 +3006,18 @@
         <v>53</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>430</v>
+        <v>233</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3636,16 +3031,16 @@
       <c r="F39" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>431</v>
+        <v>234</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3657,18 +3052,21 @@
         <v>28</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>432</v>
+        <v>235</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3680,18 +3078,21 @@
         <v>48</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>433</v>
+        <v>236</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3703,18 +3104,21 @@
         <v>29</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>434</v>
+        <v>237</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3726,18 +3130,18 @@
         <v>25</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>435</v>
+        <v>238</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3751,16 +3155,16 @@
       <c r="F44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>436</v>
+        <v>239</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3772,18 +3176,18 @@
         <v>50</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>437</v>
+        <v>240</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3795,18 +3199,21 @@
         <v>56</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>438</v>
+        <v>241</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3818,18 +3225,18 @@
         <v>51</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>439</v>
+        <v>242</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3841,18 +3248,18 @@
         <v>27</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>440</v>
+        <v>243</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3864,21 +3271,21 @@
         <v>52</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>441</v>
+        <v>244</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3890,18 +3297,18 @@
         <v>53</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>442</v>
+        <v>245</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3915,16 +3322,16 @@
       <c r="F51" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>443</v>
+        <v>246</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3936,9 +3343,12 @@
         <v>28</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4083,7 +3493,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4129,7 +3539,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>446</v>
+        <v>183</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4172,7 +3582,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>447</v>
+        <v>184</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -4195,7 +3605,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>448</v>
+        <v>185</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4218,7 +3628,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>449</v>
+        <v>186</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4241,7 +3651,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>450</v>
+        <v>187</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -4253,7 +3663,7 @@
         <v>49</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4261,7 +3671,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>451</v>
+        <v>188</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -4273,7 +3683,7 @@
         <v>49</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4281,7 +3691,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>452</v>
+        <v>189</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -4293,7 +3703,7 @@
         <v>49</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -4349,7 +3759,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>453</v>
+        <v>190</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4392,7 +3802,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>454</v>
+        <v>191</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -4415,7 +3825,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>455</v>
+        <v>192</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4438,7 +3848,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>456</v>
+        <v>193</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4465,7 +3875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -4504,7 +3914,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>444</v>
+        <v>181</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4524,7 +3934,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>445</v>
+        <v>182</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Updated RAD Test Cases and Test Data for Month and CRN.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{8E109D1F-1318-4B89-8487-7D4E57AC6BB5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEF5A62-AED8-4806-BA0E-47F021F2D258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="-120"/>
+    <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
-    <sheet name="Existing" r:id="rId2" sheetId="2"/>
-    <sheet name="Extension" r:id="rId3" sheetId="3"/>
-    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
-    <sheet name="Personal" r:id="rId5" sheetId="5"/>
-    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
-    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
-    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
+    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
+    <sheet name="Existing" sheetId="2" r:id="rId2"/>
+    <sheet name="Extension" sheetId="3" r:id="rId3"/>
+    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
+    <sheet name="Personal" sheetId="5" r:id="rId5"/>
+    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
+    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
+    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="195">
   <si>
     <t>Result</t>
   </si>
@@ -435,159 +435,6 @@
     <t>Wed Feb 07 23:48:37 EST 2024</t>
   </si>
   <si>
-    <t>Wed Feb 07 23:49:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:49:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:50:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:51:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:51:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:52:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:53:14 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:53:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:54:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:55:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:55:51 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:56:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:57:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:57:50 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:58:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:59:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 07 23:59:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:00:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:01:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:01:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:02:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:03:02 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:03:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:04:19 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:04:58 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:05:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:06:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:06:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:07:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:08:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:08:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:09:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:10:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:10:52 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:11:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:12:18 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:13:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:13:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:14:22 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:15:02 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:15:43 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:16:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:17:03 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:17:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:18:21 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:19:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:19:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:20:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:21:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:21:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Thu Feb 08 00:22:23 EST 2024</t>
-  </si>
-  <si>
     <t>Thu Feb 08 00:23:03 EST 2024</t>
   </si>
   <si>
@@ -628,9 +475,6 @@
   </si>
   <si>
     <t>CRN</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Sun Feb 18 22:43:48 EST 2024</t>
@@ -790,7 +634,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -839,19 +682,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -868,10 +711,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -906,7 +749,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -958,7 +801,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1069,21 +912,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1100,7 +943,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1152,15 +995,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:J1"/>
@@ -1168,17 +1011,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
-    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1401,8 +1244,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1410,8 +1253,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
@@ -1419,14 +1262,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="37.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1846,7 +1689,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1854,8 +1697,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C7"/>
@@ -1863,15 +1706,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2036,7 +1879,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2044,26 +1887,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:K52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="23.140625" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="8" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="23.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2089,7 +1931,7 @@
         <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>57</v>
@@ -2103,7 +1945,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2126,7 +1968,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>145</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2152,7 +1994,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2178,7 +2020,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>147</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2204,7 +2046,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>148</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2230,7 +2072,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>149</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2253,7 +2095,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2279,7 +2121,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>151</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2305,7 +2147,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>152</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2331,7 +2173,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>153</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2357,7 +2199,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>154</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2380,7 +2222,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>155</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2406,7 +2248,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>156</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2432,7 +2274,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>157</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2458,7 +2300,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>158</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2484,7 +2326,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>159</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2510,7 +2352,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2536,7 +2378,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>161</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2559,7 +2401,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>214</v>
+        <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2582,7 +2424,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>215</v>
+        <v>163</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2596,6 +2438,9 @@
       <c r="F21" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="H21" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I21" s="1" t="s">
         <v>95</v>
       </c>
@@ -2605,7 +2450,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>216</v>
+        <v>164</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2631,7 +2476,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>217</v>
+        <v>165</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2654,7 +2499,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>218</v>
+        <v>166</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2668,6 +2513,9 @@
       <c r="F24" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="H24" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>98</v>
       </c>
@@ -2677,7 +2525,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>219</v>
+        <v>167</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2694,6 +2542,9 @@
       <c r="G25" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="H25" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I25" s="1" t="s">
         <v>99</v>
       </c>
@@ -2703,7 +2554,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>220</v>
+        <v>168</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2717,6 +2568,9 @@
       <c r="F26" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="H26" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I26" s="1" t="s">
         <v>100</v>
       </c>
@@ -2726,7 +2580,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>221</v>
+        <v>169</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2738,7 +2592,7 @@
         <v>54</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>101</v>
@@ -2749,7 +2603,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>170</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2775,7 +2629,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>223</v>
+        <v>171</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2801,7 +2655,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>224</v>
+        <v>172</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2827,7 +2681,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>225</v>
+        <v>173</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2850,7 +2704,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>226</v>
+        <v>174</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2873,7 +2727,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>227</v>
+        <v>175</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2887,6 +2741,9 @@
       <c r="F33" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H33" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I33" s="1" t="s">
         <v>95</v>
       </c>
@@ -2896,7 +2753,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>228</v>
+        <v>176</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2922,7 +2779,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>229</v>
+        <v>177</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -2945,7 +2802,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>230</v>
+        <v>178</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -2959,6 +2816,9 @@
       <c r="F36" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H36" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I36" s="1" t="s">
         <v>98</v>
       </c>
@@ -2968,7 +2828,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>231</v>
+        <v>179</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -2985,6 +2845,9 @@
       <c r="G37" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="H37" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I37" s="1" t="s">
         <v>99</v>
       </c>
@@ -2994,7 +2857,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>232</v>
+        <v>180</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3008,6 +2871,9 @@
       <c r="F38" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H38" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I38" s="1" t="s">
         <v>100</v>
       </c>
@@ -3017,7 +2883,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>233</v>
+        <v>181</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3029,7 +2895,7 @@
         <v>54</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>101</v>
@@ -3040,7 +2906,7 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>234</v>
+        <v>182</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3066,7 +2932,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>235</v>
+        <v>183</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3092,7 +2958,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>236</v>
+        <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3118,7 +2984,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>237</v>
+        <v>185</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3141,7 +3007,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>238</v>
+        <v>186</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3164,7 +3030,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3178,6 +3044,9 @@
       <c r="F45" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="H45" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I45" s="1" t="s">
         <v>95</v>
       </c>
@@ -3187,7 +3056,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>240</v>
+        <v>188</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3213,7 +3082,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>241</v>
+        <v>189</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3236,7 +3105,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>242</v>
+        <v>190</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3250,6 +3119,9 @@
       <c r="F48" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="H48" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I48" s="1" t="s">
         <v>98</v>
       </c>
@@ -3259,7 +3131,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>243</v>
+        <v>191</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3276,6 +3148,9 @@
       <c r="G49" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="H49" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I49" s="1" t="s">
         <v>99</v>
       </c>
@@ -3285,7 +3160,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>244</v>
+        <v>192</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3298,6 +3173,9 @@
       </c>
       <c r="F50" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>100</v>
@@ -3308,7 +3186,7 @@
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>245</v>
+        <v>193</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3320,7 +3198,7 @@
         <v>54</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>101</v>
@@ -3331,7 +3209,7 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>246</v>
+        <v>194</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3354,7 +3232,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3362,8 +3240,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3371,15 +3249,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3481,7 +3359,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3489,8 +3367,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -3498,14 +3376,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3539,7 +3417,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3582,7 +3460,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>133</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3605,7 +3483,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3628,7 +3506,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>135</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3651,7 +3529,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>136</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -3671,7 +3549,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -3691,7 +3569,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -3707,13 +3585,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD9"/>
@@ -3721,14 +3599,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3759,7 +3637,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3802,7 +3680,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>140</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3825,7 +3703,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3848,7 +3726,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>142</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3867,13 +3745,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -3881,12 +3759,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3914,7 +3792,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3934,7 +3812,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3947,6 +3825,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RAD Test Cases for Bay Restoration and Transportation for Month drop down.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{F4DD97DF-D619-4971-8F43-31D91C6C6A99}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{CB12AA62-7A2A-48FC-97DC-F33FFD7606A1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView activeTab="3" windowHeight="14010" windowWidth="24525" xWindow="-24870" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="3000"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="253">
   <si>
     <t>Result</t>
   </si>
@@ -522,27 +522,18 @@
     <t>Tue Mar 05 00:17:25 EST 2024</t>
   </si>
   <si>
-    <t>Tue Mar 05 00:18:17 EST 2024</t>
-  </si>
-  <si>
     <t>Tue Mar 05 00:19:51 EST 2024</t>
   </si>
   <si>
     <t>Tue Mar 05 00:21:25 EST 2024</t>
   </si>
   <si>
-    <t>Tue Mar 05 00:22:58 EST 2024</t>
-  </si>
-  <si>
     <t>Tue Mar 05 00:23:50 EST 2024</t>
   </si>
   <si>
     <t>Tue Mar 05 00:25:24 EST 2024</t>
   </si>
   <si>
-    <t>Tue Mar 05 00:26:57 EST 2024</t>
-  </si>
-  <si>
     <t>Tue Mar 05 00:27:49 EST 2024</t>
   </si>
   <si>
@@ -648,16 +639,169 @@
     <t>June</t>
   </si>
   <si>
+    <t>Tue Mar 05 22:14:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 22:15:01 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 22:15:56 EST 2024</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Tue Mar 05 22:14:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Mar 05 22:15:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Mar 05 22:15:56 EST 2024</t>
+    <t>Tue Mar 05 22:58:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 22:59:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:00:07 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:00:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:01:46 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:02:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:03:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:04:14 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:05:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:05:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:06:42 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:07:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:08:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:09:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:09:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:10:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:11:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:12:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:13:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:14:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:15:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:15:51 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:16:41 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:17:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:18:22 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:19:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:20:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:20:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:21:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:22:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:23:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:24:14 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:25:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:25:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:26:46 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:27:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:28:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:29:19 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:30:09 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:31:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:31:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:32:41 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:33:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:34:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:35:11 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:36:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:36:52 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:37:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:38:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:39:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 23:40:17 EST 2024</t>
   </si>
 </sst>
 </file>
@@ -1921,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,8 +2077,7 @@
     <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
     <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
     <col min="10" max="10" style="1" width="9.140625" collapsed="true"/>
     <col min="11" max="11" customWidth="true" style="1" width="23.140625" collapsed="true"/>
     <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
@@ -1980,7 +2123,10 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>202</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -2000,7 +2146,10 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>203</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -2023,7 +2172,10 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>204</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -2046,7 +2198,10 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>205</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -2069,7 +2224,10 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>206</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -2092,7 +2250,10 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>207</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
@@ -2112,7 +2273,10 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>208</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -2135,7 +2299,10 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>209</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -2158,7 +2325,10 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>210</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
@@ -2181,7 +2351,10 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>211</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -2204,7 +2377,10 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>212</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
@@ -2224,7 +2400,10 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>213</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -2247,7 +2426,10 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>214</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -2270,7 +2452,10 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>215</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>
@@ -2293,7 +2478,10 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>216</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>16</v>
@@ -2316,7 +2504,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2334,7 +2522,7 @@
         <v>32</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>91</v>
@@ -2342,10 +2530,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>218</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -2368,10 +2559,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>219</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>16</v>
@@ -2397,7 +2591,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2417,10 +2611,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>221</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>16</v>
@@ -2435,7 +2632,7 @@
         <v>32</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>95</v>
@@ -2443,10 +2640,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>164</v>
+        <v>222</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -2461,7 +2661,7 @@
         <v>32</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>96</v>
@@ -2472,7 +2672,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2495,10 +2695,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>166</v>
+        <v>224</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>16</v>
@@ -2513,7 +2716,7 @@
         <v>32</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>98</v>
@@ -2521,10 +2724,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>167</v>
+        <v>225</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>16</v>
@@ -2542,7 +2748,7 @@
         <v>32</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>99</v>
@@ -2550,10 +2756,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>226</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>16</v>
@@ -2568,7 +2777,7 @@
         <v>32</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>100</v>
@@ -2576,10 +2785,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>227</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>16</v>
@@ -2602,10 +2814,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
+        <v>228</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>16</v>
@@ -2628,10 +2843,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>171</v>
+        <v>229</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>16</v>
@@ -2646,7 +2864,7 @@
         <v>32</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>91</v>
@@ -2654,10 +2872,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>172</v>
+        <v>230</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>16</v>
@@ -2680,10 +2901,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>173</v>
+        <v>231</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>16</v>
@@ -2709,7 +2933,10 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
+        <v>232</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>16</v>
@@ -2726,10 +2953,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>175</v>
+        <v>233</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>16</v>
@@ -2744,7 +2974,7 @@
         <v>32</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>95</v>
@@ -2752,10 +2982,13 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>176</v>
+        <v>234</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>16</v>
@@ -2770,7 +3003,7 @@
         <v>32</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>96</v>
@@ -2781,7 +3014,10 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>177</v>
+        <v>235</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>16</v>
@@ -2801,10 +3037,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>178</v>
+        <v>236</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>16</v>
@@ -2819,7 +3058,7 @@
         <v>32</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>98</v>
@@ -2827,10 +3066,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>179</v>
+        <v>237</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>16</v>
@@ -2848,7 +3090,7 @@
         <v>32</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>99</v>
@@ -2856,10 +3098,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>180</v>
+        <v>238</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>16</v>
@@ -2874,7 +3119,7 @@
         <v>32</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>100</v>
@@ -2882,10 +3127,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>181</v>
+        <v>239</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>16</v>
@@ -2908,10 +3156,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>182</v>
+        <v>240</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>16</v>
@@ -2934,10 +3185,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>183</v>
+        <v>241</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>16</v>
@@ -2952,7 +3206,7 @@
         <v>32</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>91</v>
@@ -2960,10 +3214,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>184</v>
+        <v>242</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>16</v>
@@ -2986,10 +3243,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>185</v>
+        <v>243</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>16</v>
@@ -3015,7 +3275,10 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>186</v>
+        <v>244</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>16</v>
@@ -3032,10 +3295,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>245</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>16</v>
@@ -3050,7 +3316,7 @@
         <v>32</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>95</v>
@@ -3058,10 +3324,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>188</v>
+        <v>246</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -3076,7 +3345,7 @@
         <v>32</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>96</v>
@@ -3087,7 +3356,10 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>189</v>
+        <v>247</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>16</v>
@@ -3107,10 +3379,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
+        <v>248</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -3125,7 +3400,7 @@
         <v>32</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>98</v>
@@ -3133,10 +3408,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>191</v>
+        <v>249</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>16</v>
@@ -3154,7 +3432,7 @@
         <v>32</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>99</v>
@@ -3162,10 +3440,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>192</v>
+        <v>250</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>16</v>
@@ -3180,7 +3461,7 @@
         <v>32</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>100</v>
@@ -3188,10 +3469,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>193</v>
+        <v>251</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>16</v>
@@ -3214,10 +3498,13 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>194</v>
+        <v>252</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Updates to execute RAD Extension Payment Type.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63161B30-D4FD-4C35-92A3-D618B937BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A1FC403C-D099-40AA-877A-0FE0305701CC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="30810" yWindow="990" windowWidth="24525" windowHeight="14010" activeTab="7" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView activeTab="6" windowHeight="14010" windowWidth="24525" xWindow="2610" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="1665"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
-    <sheet name="Existing" sheetId="2" r:id="rId2"/>
-    <sheet name="Extension" sheetId="3" r:id="rId3"/>
-    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
-    <sheet name="Personal" sheetId="5" r:id="rId5"/>
-    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
-    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
-    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
+    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
+    <sheet name="Existing" r:id="rId2" sheetId="2"/>
+    <sheet name="Extension" r:id="rId3" sheetId="3"/>
+    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
+    <sheet name="Personal" r:id="rId5" sheetId="5"/>
+    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
+    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
+    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="209">
   <si>
     <t>Result</t>
   </si>
@@ -171,15 +171,6 @@
     <t>Tue Oct 31 16:46:19 EDT 2023</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 22:41:41 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 22:46:40 EST 2023</t>
-  </si>
-  <si>
     <t>DoNotRun</t>
   </si>
   <si>
@@ -643,12 +634,49 @@
   </si>
   <si>
     <t>Sat Mar 09 00:40:51 EST 2024</t>
+  </si>
+  <si>
+    <t>704</t>
+  </si>
+  <si>
+    <t>AppID</t>
+  </si>
+  <si>
+    <t>739</t>
+  </si>
+  <si>
+    <t>789</t>
+  </si>
+  <si>
+    <t>790</t>
+  </si>
+  <si>
+    <t>775</t>
+  </si>
+  <si>
+    <t>776</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>Thu Mar 21 11:21:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Mar 21 11:22:56 EDT 2024</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Thu Mar 21 11:24:46 EDT 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -697,19 +725,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -726,10 +754,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -764,7 +792,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -816,7 +844,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -927,21 +955,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -958,7 +986,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1010,15 +1038,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:J1"/>
@@ -1026,17 +1054,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="32.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="32.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
+    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1065,10 +1093,10 @@
         <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1076,7 +1104,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1088,16 +1116,16 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1105,7 +1133,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1117,16 +1145,16 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1134,7 +1162,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1146,7 +1174,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -1155,10 +1183,10 @@
         <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1166,7 +1194,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1178,7 +1206,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>22</v>
@@ -1187,10 +1215,10 @@
         <v>32</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1198,7 +1226,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1210,7 +1238,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>23</v>
@@ -1219,10 +1247,10 @@
         <v>32</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1230,7 +1258,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1242,7 +1270,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
@@ -1251,16 +1279,16 @@
         <v>32</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1268,8 +1296,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
@@ -1277,14 +1305,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="37.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1307,10 +1335,10 @@
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1318,7 +1346,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1330,10 +1358,10 @@
         <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1341,7 +1369,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1353,10 +1381,10 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1364,7 +1392,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1376,10 +1404,10 @@
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1387,7 +1415,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1402,10 +1430,10 @@
         <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1413,7 +1441,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1428,10 +1456,10 @@
         <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1439,7 +1467,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1451,7 +1479,7 @@
         <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1459,7 +1487,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1471,7 +1499,7 @@
         <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1479,7 +1507,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1491,7 +1519,7 @@
         <v>28</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1499,7 +1527,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1511,7 +1539,7 @@
         <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1519,7 +1547,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1534,7 +1562,7 @@
         <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1542,7 +1570,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1557,7 +1585,7 @@
         <v>32</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1565,7 +1593,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1574,10 +1602,10 @@
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1585,7 +1613,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1594,10 +1622,10 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1605,7 +1633,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1614,10 +1642,10 @@
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1625,7 +1653,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1634,13 +1662,13 @@
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1648,7 +1676,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1657,10 +1685,10 @@
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1668,7 +1696,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1677,10 +1705,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1688,7 +1716,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -1697,14 +1725,14 @@
         <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1712,27 +1740,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1757,8 +1785,11 @@
       <c r="H1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1780,8 +1811,11 @@
       <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1800,8 +1834,11 @@
       <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1823,8 +1860,11 @@
       <c r="H4" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1846,8 +1886,11 @@
       <c r="H5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1869,8 +1912,11 @@
       <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1892,10 +1938,13 @@
       <c r="H7" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>204</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1903,8 +1952,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:K52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C52"/>
@@ -1912,16 +1961,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="9" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.140625" style="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="10" max="10" style="1" width="9.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="23.140625" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1947,16 +1996,16 @@
         <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1964,7 +2013,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1979,7 +2028,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1987,7 +2036,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2005,7 +2054,7 @@
         <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2013,7 +2062,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2031,7 +2080,7 @@
         <v>32</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2039,7 +2088,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2057,7 +2106,7 @@
         <v>32</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2065,7 +2114,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2083,7 +2132,7 @@
         <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2091,7 +2140,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2106,7 +2155,7 @@
         <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2114,7 +2163,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2132,7 +2181,7 @@
         <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2140,7 +2189,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2158,7 +2207,7 @@
         <v>32</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2166,7 +2215,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2184,7 +2233,7 @@
         <v>32</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2192,7 +2241,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2210,7 +2259,7 @@
         <v>32</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2218,7 +2267,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2233,7 +2282,7 @@
         <v>31</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2241,7 +2290,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2259,7 +2308,7 @@
         <v>32</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2267,7 +2316,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2285,7 +2334,7 @@
         <v>32</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2293,7 +2342,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2311,7 +2360,7 @@
         <v>32</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2319,7 +2368,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2337,7 +2386,7 @@
         <v>32</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2345,7 +2394,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2354,19 +2403,19 @@
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2374,7 +2423,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2386,7 +2435,7 @@
         <v>29</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>32</v>
@@ -2395,7 +2444,7 @@
         <v>23</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2403,7 +2452,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2415,7 +2464,7 @@
         <v>25</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>32</v>
@@ -2424,7 +2473,7 @@
         <v>19</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2432,7 +2481,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2447,7 +2496,7 @@
         <v>18</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2455,7 +2504,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2464,19 +2513,19 @@
         <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2484,7 +2533,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2493,19 +2542,19 @@
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2513,7 +2562,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2522,16 +2571,16 @@
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2539,7 +2588,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2551,16 +2600,16 @@
         <v>27</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2568,7 +2617,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2577,10 +2626,10 @@
         <v>16</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>32</v>
@@ -2589,10 +2638,10 @@
         <v>32</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2600,7 +2649,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2609,19 +2658,19 @@
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2629,7 +2678,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2638,10 +2687,10 @@
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>32</v>
@@ -2650,7 +2699,7 @@
         <v>21</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2658,7 +2707,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2670,7 +2719,7 @@
         <v>28</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>32</v>
@@ -2679,7 +2728,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2687,7 +2736,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2696,7 +2745,7 @@
         <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>18</v>
@@ -2705,10 +2754,10 @@
         <v>32</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2716,7 +2765,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2728,7 +2777,7 @@
         <v>29</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>32</v>
@@ -2737,7 +2786,7 @@
         <v>23</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2745,7 +2794,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2766,7 +2815,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2774,7 +2823,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2789,7 +2838,7 @@
         <v>30</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2797,7 +2846,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2806,7 +2855,7 @@
         <v>16</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>18</v>
@@ -2815,10 +2864,10 @@
         <v>32</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2826,7 +2875,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2835,7 +2884,7 @@
         <v>16</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>18</v>
@@ -2844,10 +2893,10 @@
         <v>32</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2855,7 +2904,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -2864,7 +2913,7 @@
         <v>16</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>18</v>
@@ -2873,7 +2922,7 @@
         <v>32</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2881,7 +2930,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -2899,10 +2948,10 @@
         <v>32</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2910,7 +2959,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -2919,7 +2968,7 @@
         <v>16</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>18</v>
@@ -2931,10 +2980,10 @@
         <v>32</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2942,7 +2991,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -2951,7 +3000,7 @@
         <v>16</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>18</v>
@@ -2960,10 +3009,10 @@
         <v>32</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2971,7 +3020,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -2980,7 +3029,7 @@
         <v>16</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>18</v>
@@ -2992,7 +3041,7 @@
         <v>21</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -3000,7 +3049,7 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3021,7 +3070,7 @@
         <v>20</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3029,7 +3078,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3038,7 +3087,7 @@
         <v>16</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>30</v>
@@ -3047,10 +3096,10 @@
         <v>32</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -3058,7 +3107,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3079,7 +3128,7 @@
         <v>23</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3087,7 +3136,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3108,7 +3157,7 @@
         <v>19</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -3116,7 +3165,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3131,7 +3180,7 @@
         <v>31</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3139,7 +3188,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3148,7 +3197,7 @@
         <v>16</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>30</v>
@@ -3157,10 +3206,10 @@
         <v>32</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3168,7 +3217,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3177,7 +3226,7 @@
         <v>16</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>30</v>
@@ -3186,10 +3235,10 @@
         <v>32</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -3197,7 +3246,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3206,7 +3255,7 @@
         <v>16</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>30</v>
@@ -3215,7 +3264,7 @@
         <v>32</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3223,7 +3272,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3241,10 +3290,10 @@
         <v>32</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -3252,7 +3301,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3261,7 +3310,7 @@
         <v>16</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>30</v>
@@ -3273,10 +3322,10 @@
         <v>32</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -3284,7 +3333,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3293,7 +3342,7 @@
         <v>16</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>30</v>
@@ -3302,10 +3351,10 @@
         <v>32</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3313,7 +3362,7 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3322,7 +3371,7 @@
         <v>16</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>30</v>
@@ -3334,7 +3383,7 @@
         <v>21</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3342,7 +3391,7 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3363,12 +3412,12 @@
         <v>20</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3376,8 +3425,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3385,15 +3434,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3424,7 +3473,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3440,7 +3489,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
@@ -3495,7 +3544,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3503,23 +3552,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3542,10 +3591,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3553,10 +3602,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>186</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -3565,18 +3611,18 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>205</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3590,16 +3636,16 @@
       <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -3611,7 +3657,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3619,10 +3665,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>188</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -3634,7 +3677,7 @@
         <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3642,10 +3685,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>189</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -3657,7 +3697,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3665,16 +3705,13 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>190</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>18</v>
@@ -3685,16 +3722,13 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>30</v>
@@ -3705,44 +3739,41 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3765,7 +3796,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3773,10 +3804,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>193</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -3785,18 +3813,18 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>208</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3808,10 +3836,10 @@
         <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3819,10 +3847,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -3834,7 +3859,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3842,10 +3867,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>195</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -3857,7 +3879,7 @@
         <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3865,10 +3887,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>199</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>196</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -3880,30 +3899,30 @@
         <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3923,7 +3942,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3931,7 +3950,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3943,7 +3962,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3951,7 +3970,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3960,10 +3979,10 @@
         <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RAD Test Scripts and Test Data for Existing Liability.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{A1FC403C-D099-40AA-877A-0FE0305701CC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ABDBF5-644B-4ADA-8389-9FC1534148D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="6" windowHeight="14010" windowWidth="24525" xWindow="2610" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="1665"/>
+    <workbookView xWindow="1965" yWindow="1155" windowWidth="24525" windowHeight="14010" activeTab="7" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
-    <sheet name="Existing" r:id="rId2" sheetId="2"/>
-    <sheet name="Extension" r:id="rId3" sheetId="3"/>
-    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
-    <sheet name="Personal" r:id="rId5" sheetId="5"/>
-    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
-    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
-    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
+    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
+    <sheet name="Existing" sheetId="2" r:id="rId2"/>
+    <sheet name="Extension" sheetId="3" r:id="rId3"/>
+    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
+    <sheet name="Personal" sheetId="5" r:id="rId5"/>
+    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
+    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
+    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="208">
   <si>
     <t>Result</t>
   </si>
@@ -663,20 +663,16 @@
     <t>Thu Mar 21 11:21:29 EDT 2024</t>
   </si>
   <si>
-    <t>Thu Mar 21 11:22:56 EDT 2024</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>Thu Mar 21 11:24:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Existing Liability with Notice/Invoice Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -725,19 +721,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -754,10 +750,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -792,7 +788,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -844,7 +840,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -955,21 +951,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -986,7 +982,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1038,15 +1034,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:J1"/>
@@ -1054,17 +1050,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
-    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1287,8 +1283,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1296,23 +1292,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="D2" sqref="D2:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="52" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1352,7 +1348,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>25</v>
@@ -1375,7 +1371,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -1398,7 +1394,7 @@
         <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -1421,7 +1417,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
@@ -1447,7 +1443,7 @@
         <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -1473,7 +1469,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>26</v>
@@ -1493,7 +1489,7 @@
         <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>27</v>
@@ -1513,7 +1509,7 @@
         <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1533,7 +1529,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>29</v>
@@ -1553,7 +1549,7 @@
         <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
@@ -1576,7 +1572,7 @@
         <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
@@ -1599,7 +1595,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>44</v>
@@ -1619,7 +1615,7 @@
         <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>46</v>
@@ -1639,7 +1635,7 @@
         <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>47</v>
@@ -1659,7 +1655,7 @@
         <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>48</v>
@@ -1682,7 +1678,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>49</v>
@@ -1702,7 +1698,7 @@
         <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>50</v>
@@ -1722,7 +1718,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>51</v>
@@ -1732,7 +1728,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1740,8 +1736,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -1749,15 +1745,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1944,7 +1940,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1952,25 +1948,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:L52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="10" max="10" style="1" width="9.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="23.140625" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="9" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.140625" style="1" collapsed="1"/>
+    <col min="11" max="11" width="23.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -3417,7 +3413,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3425,8 +3421,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3434,15 +3430,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3544,7 +3540,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3552,23 +3548,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3604,6 +3600,9 @@
       <c r="B2" t="s">
         <v>186</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
@@ -3647,6 +3646,9 @@
       <c r="B4" t="s">
         <v>187</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
@@ -3667,6 +3669,9 @@
       <c r="B5" t="s">
         <v>188</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
@@ -3687,6 +3692,9 @@
       <c r="B6" t="s">
         <v>189</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
@@ -3707,6 +3715,9 @@
       <c r="B7" t="s">
         <v>190</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
@@ -3724,6 +3735,9 @@
       <c r="B8" t="s">
         <v>191</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3741,6 +3755,9 @@
       <c r="B9" t="s">
         <v>192</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3752,28 +3769,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3806,6 +3823,9 @@
       <c r="B2" t="s">
         <v>193</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
@@ -3824,7 +3844,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3849,6 +3869,9 @@
       <c r="B4" t="s">
         <v>194</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
@@ -3869,6 +3892,9 @@
       <c r="B5" t="s">
         <v>195</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
@@ -3889,6 +3915,9 @@
       <c r="B6" t="s">
         <v>196</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
@@ -3903,26 +3932,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3956,7 +3985,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
@@ -3976,13 +4005,13 @@
         <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RAD Test Data for Existing Liability MD CRN.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ABDBF5-644B-4ADA-8389-9FC1534148D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B02703-3A42-4E6D-A560-95EAE739B25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="1155" windowWidth="24525" windowHeight="14010" activeTab="7" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView xWindow="29595" yWindow="1470" windowWidth="24525" windowHeight="14010" activeTab="1" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="208">
   <si>
     <t>Result</t>
   </si>
@@ -1293,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,12 +1306,14 @@
     <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
     <col min="4" max="4" width="52" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="1" collapsed="1"/>
+    <col min="9" max="9" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1331,13 +1333,16 @@
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1353,14 +1358,14 @@
       <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1376,14 +1381,14 @@
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1399,14 +1404,14 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1425,14 +1430,14 @@
       <c r="F5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1451,14 +1456,14 @@
       <c r="F6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1475,10 +1480,13 @@
         <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1495,10 +1503,13 @@
         <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1515,10 +1526,13 @@
         <v>28</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1535,10 +1549,13 @@
         <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1557,11 +1574,11 @@
       <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1580,11 +1597,11 @@
       <c r="F12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1601,10 +1618,13 @@
         <v>44</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1621,10 +1641,13 @@
         <v>46</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1640,11 +1663,11 @@
       <c r="E15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1664,10 +1687,13 @@
         <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1684,10 +1710,13 @@
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1703,11 +1732,11 @@
       <c r="E18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1723,7 +1752,7 @@
       <c r="E19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3940,7 +3969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made updates for RAD Motor Fuel Lic Num.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B02703-3A42-4E6D-A560-95EAE739B25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F013C0-2881-45EA-A19A-EB8CF1187CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29595" yWindow="1470" windowWidth="24525" windowHeight="14010" activeTab="1" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="209">
   <si>
     <t>Result</t>
   </si>
@@ -501,12 +501,6 @@
     <t>Sat Mar 09 00:01:14 EST 2024</t>
   </si>
   <si>
-    <t>Sat Mar 09 00:02:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:02:59 EST 2024</t>
-  </si>
-  <si>
     <t>Sat Mar 09 00:03:52 EST 2024</t>
   </si>
   <si>
@@ -667,6 +661,15 @@
   </si>
   <si>
     <t>Existing Liability with Notice/Invoice Number</t>
+  </si>
+  <si>
+    <t>MFLicNum</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 15:27:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 15:28:20 EDT 2024</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -1306,9 +1309,7 @@
     <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
     <col min="4" max="4" width="52" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="1" collapsed="1"/>
+    <col min="6" max="8" width="9.140625" style="1" collapsed="1"/>
     <col min="9" max="9" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="10" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
@@ -1353,7 +1354,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>25</v>
@@ -1376,7 +1377,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -1399,7 +1400,7 @@
         <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -1422,7 +1423,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
@@ -1448,7 +1449,7 @@
         <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -1474,7 +1475,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>26</v>
@@ -1497,7 +1498,7 @@
         <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>27</v>
@@ -1520,7 +1521,7 @@
         <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1543,7 +1544,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>29</v>
@@ -1566,7 +1567,7 @@
         <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
@@ -1589,7 +1590,7 @@
         <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
@@ -1612,7 +1613,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>44</v>
@@ -1635,7 +1636,7 @@
         <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>46</v>
@@ -1658,7 +1659,7 @@
         <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>47</v>
@@ -1678,7 +1679,7 @@
         <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>48</v>
@@ -1704,7 +1705,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>49</v>
@@ -1727,7 +1728,7 @@
         <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>50</v>
@@ -1747,7 +1748,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>51</v>
@@ -1811,7 +1812,7 @@
         <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1837,7 +1838,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1860,7 +1861,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1886,7 +1887,7 @@
         <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1912,7 +1913,7 @@
         <v>32</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1938,7 +1939,7 @@
         <v>32</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1964,7 +1965,7 @@
         <v>32</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1978,7 +1979,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C52"/>
@@ -1992,13 +1993,13 @@
     <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="9" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.140625" style="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="10" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" style="1" collapsed="1"/>
+    <col min="12" max="12" width="23.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2027,13 +2028,16 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2052,11 +2056,11 @@
       <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2078,11 +2082,11 @@
       <c r="G3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -2104,11 +2108,11 @@
       <c r="G4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2130,11 +2134,11 @@
       <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2156,11 +2160,11 @@
       <c r="G6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -2179,11 +2183,11 @@
       <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2205,11 +2209,11 @@
       <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2231,11 +2235,11 @@
       <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2257,11 +2261,11 @@
       <c r="G10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2283,11 +2287,11 @@
       <c r="G11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2306,11 +2310,11 @@
       <c r="F12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2332,11 +2336,11 @@
       <c r="G13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2358,11 +2362,11 @@
       <c r="G14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2384,11 +2388,11 @@
       <c r="G15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -2410,11 +2414,11 @@
       <c r="G16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2439,11 +2443,11 @@
       <c r="I17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2468,11 +2472,11 @@
       <c r="I18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2497,11 +2501,11 @@
       <c r="I19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2520,16 +2524,16 @@
       <c r="F20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>207</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2543,22 +2547,22 @@
       <c r="F21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="I21" s="1" t="s">
         <v>104</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>208</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2578,16 +2582,16 @@
       <c r="I22" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2604,16 +2608,16 @@
       <c r="H23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2633,16 +2637,16 @@
       <c r="I24" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2665,16 +2669,16 @@
       <c r="I25" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2694,16 +2698,16 @@
       <c r="I26" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2723,16 +2727,16 @@
       <c r="I27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2752,16 +2756,16 @@
       <c r="I28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2781,16 +2785,16 @@
       <c r="I29" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2810,16 +2814,16 @@
       <c r="I30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2839,16 +2843,16 @@
       <c r="I31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2862,16 +2866,16 @@
       <c r="F32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2885,22 +2889,22 @@
       <c r="F33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="I33" s="1" t="s">
         <v>104</v>
       </c>
       <c r="J33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2920,16 +2924,16 @@
       <c r="I34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -2946,16 +2950,16 @@
       <c r="H35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -2975,16 +2979,16 @@
       <c r="I36" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3007,16 +3011,16 @@
       <c r="I37" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3036,16 +3040,16 @@
       <c r="I38" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3065,16 +3069,16 @@
       <c r="I39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3094,16 +3098,16 @@
       <c r="I40" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3123,16 +3127,16 @@
       <c r="I41" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3152,16 +3156,16 @@
       <c r="I42" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3181,16 +3185,16 @@
       <c r="I43" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3204,16 +3208,16 @@
       <c r="F44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3227,22 +3231,22 @@
       <c r="F45" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="I45" s="1" t="s">
         <v>104</v>
       </c>
       <c r="J45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3262,16 +3266,16 @@
       <c r="I46" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3288,16 +3292,16 @@
       <c r="H47" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3317,16 +3321,16 @@
       <c r="I48" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="K48" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3349,16 +3353,16 @@
       <c r="I49" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3378,16 +3382,16 @@
       <c r="I50" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3407,16 +3411,16 @@
       <c r="I51" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3436,7 +3440,7 @@
       <c r="I52" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3627,7 +3631,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3650,7 +3654,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3665,7 +3669,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3673,7 +3677,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3696,7 +3700,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3719,7 +3723,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3742,7 +3746,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -3762,7 +3766,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -3782,7 +3786,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -3806,8 +3810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3850,7 +3854,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3873,7 +3877,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3888,7 +3892,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3896,7 +3900,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3919,7 +3923,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3942,7 +3946,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4008,13 +4012,13 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
@@ -4028,13 +4032,13 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Updated RAD EL-Motor Fuel Tax.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F013C0-2881-45EA-A19A-EB8CF1187CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2BAF82-5EFE-4E92-BFA7-0C9AA2704DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="209">
   <si>
     <t>Result</t>
   </si>
@@ -153,24 +153,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Tue Oct 31 16:41:50 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:42:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:43:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:44:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:45:26 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Oct 31 16:46:19 EDT 2023</t>
-  </si>
-  <si>
     <t>DoNotRun</t>
   </si>
   <si>
@@ -372,264 +354,6 @@
     <t>June</t>
   </si>
   <si>
-    <t>Fri Mar 08 23:24:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:25:23 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:26:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:27:08 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:28:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:28:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:29:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:30:38 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:31:30 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:32:22 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:33:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:34:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:35:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:35:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:36:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:37:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:38:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:39:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:40:19 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:41:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:42:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:42:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:43:49 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:44:42 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:45:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:46:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:47:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:48:09 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:49:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:49:52 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:50:44 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:51:36 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:52:28 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:53:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:54:13 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:55:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:55:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:56:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:57:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:58:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 08 23:59:26 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:00:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:01:14 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:03:52 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:04:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:05:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:06:33 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:07:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:08:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:09:13 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:10:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:11:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:11:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:12:46 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:13:39 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:14:32 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:15:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:16:19 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:17:12 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:18:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:18:59 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:19:53 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:20:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:21:40 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:22:34 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:23:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:24:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:25:14 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:26:07 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:27:01 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:27:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:28:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:29:41 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:30:35 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:31:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:32:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:33:06 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:33:56 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:34:45 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:35:36 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:36:25 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:37:15 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:38:05 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:39:00 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:39:55 EST 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 09 00:40:51 EST 2024</t>
-  </si>
-  <si>
     <t>704</t>
   </si>
   <si>
@@ -654,22 +378,298 @@
     <t>777</t>
   </si>
   <si>
-    <t>Thu Mar 21 11:21:29 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Mar 21 11:24:46 EDT 2024</t>
-  </si>
-  <si>
     <t>Existing Liability with Notice/Invoice Number</t>
   </si>
   <si>
     <t>MFLicNum</t>
   </si>
   <si>
-    <t>Mon Apr 08 15:27:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 15:28:20 EDT 2024</t>
+    <t>Mon Apr 08 19:07:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:08:13 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:09:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:09:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:10:51 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:11:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:12:40 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:13:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:14:25 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:15:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:16:13 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:17:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:18:00 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:18:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:19:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:20:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:21:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:22:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:23:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:24:16 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:25:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:26:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:26:56 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:27:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:28:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:29:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:30:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:31:21 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:32:13 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:33:07 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:34:01 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:34:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:35:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:36:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:37:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:38:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:39:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:40:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:41:04 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:41:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:42:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:43:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:44:37 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:45:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:46:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:47:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:48:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:49:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:49:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:50:52 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:51:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:52:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:53:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:54:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:55:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:56:20 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:57:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:58:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:59:02 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 19:59:56 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:00:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:01:43 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:02:37 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:03:31 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:04:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:05:20 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:06:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:07:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:08:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:08:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:09:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:10:45 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:11:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:12:31 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:13:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:14:21 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:15:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:16:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:17:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:17:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:18:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:19:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:20:38 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:21:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:22:20 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:23:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:23:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:24:51 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:25:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:26:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:27:21 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:28:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:29:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:30:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:31:01 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Apr 08 20:31:57 EDT 2024</t>
   </si>
 </sst>
 </file>
@@ -1092,10 +1092,10 @@
         <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1103,7 +1103,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1115,16 +1115,16 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1144,16 +1144,16 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1161,7 +1161,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1173,7 +1173,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -1182,10 +1182,10 @@
         <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1193,7 +1193,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1205,7 +1205,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>22</v>
@@ -1214,10 +1214,10 @@
         <v>32</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1237,7 +1237,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>23</v>
@@ -1246,10 +1246,10 @@
         <v>32</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1269,7 +1269,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
@@ -1278,10 +1278,10 @@
         <v>32</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1298,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,13 +1334,13 @@
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1348,22 +1348,22 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1371,22 +1371,22 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1394,22 +1394,22 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1417,13 +1417,13 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
@@ -1432,10 +1432,10 @@
         <v>32</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1443,13 +1443,13 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -1458,10 +1458,10 @@
         <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1469,13 +1469,13 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>26</v>
@@ -1484,7 +1484,7 @@
         <v>32</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1492,13 +1492,13 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>27</v>
@@ -1507,7 +1507,7 @@
         <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1515,13 +1515,13 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1530,7 +1530,7 @@
         <v>32</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1538,13 +1538,13 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>29</v>
@@ -1553,7 +1553,7 @@
         <v>32</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1561,13 +1561,13 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
@@ -1576,7 +1576,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1584,13 +1584,13 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
@@ -1599,7 +1599,7 @@
         <v>32</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1607,22 +1607,22 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1630,22 +1630,19 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1653,19 +1650,19 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1673,16 +1670,16 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>32</v>
@@ -1691,7 +1688,7 @@
         <v>32</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1699,22 +1696,22 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1722,19 +1719,19 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1742,19 +1739,19 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1812,7 +1809,7 @@
         <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>196</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1820,7 +1817,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1838,7 +1835,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>197</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1846,7 +1843,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1861,7 +1858,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>198</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1869,7 +1866,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1887,7 +1884,7 @@
         <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1895,7 +1892,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1913,7 +1910,7 @@
         <v>32</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>200</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1921,7 +1918,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>141</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1939,7 +1936,7 @@
         <v>32</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>201</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1947,7 +1944,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1965,7 +1962,7 @@
         <v>32</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>202</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2022,19 +2019,19 @@
         <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>206</v>
+        <v>112</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2042,7 +2039,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2057,7 +2054,7 @@
         <v>18</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2065,7 +2062,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2083,7 +2080,7 @@
         <v>32</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2091,7 +2088,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2109,7 +2106,7 @@
         <v>32</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2117,7 +2114,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2135,7 +2132,7 @@
         <v>32</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2143,7 +2140,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2161,7 +2158,7 @@
         <v>32</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2169,7 +2166,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2184,7 +2181,7 @@
         <v>30</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2192,7 +2189,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2210,7 +2207,7 @@
         <v>32</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2218,7 +2215,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2236,7 +2233,7 @@
         <v>32</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2244,7 +2241,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2262,7 +2259,7 @@
         <v>32</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2270,7 +2267,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2288,7 +2285,7 @@
         <v>32</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2296,7 +2293,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2311,7 +2308,7 @@
         <v>31</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2319,7 +2316,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2337,7 +2334,7 @@
         <v>32</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2345,7 +2342,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2363,7 +2360,7 @@
         <v>32</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2371,7 +2368,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2389,7 +2386,7 @@
         <v>32</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2397,7 +2394,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2415,7 +2412,7 @@
         <v>32</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2423,7 +2420,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2432,19 +2429,19 @@
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2452,7 +2449,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2464,7 +2461,7 @@
         <v>29</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>32</v>
@@ -2473,7 +2470,7 @@
         <v>23</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2481,7 +2478,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2493,7 +2490,7 @@
         <v>25</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>32</v>
@@ -2502,7 +2499,7 @@
         <v>19</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2510,7 +2507,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2525,7 +2522,7 @@
         <v>18</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2533,7 +2530,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2542,19 +2539,19 @@
         <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2562,7 +2559,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>208</v>
+        <v>163</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2571,19 +2568,19 @@
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2591,7 +2588,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2600,16 +2597,16 @@
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2617,7 +2614,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2629,16 +2626,16 @@
         <v>27</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2646,7 +2643,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2655,10 +2652,10 @@
         <v>16</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>32</v>
@@ -2667,10 +2664,10 @@
         <v>32</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2678,7 +2675,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2687,19 +2684,19 @@
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2707,7 +2704,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2716,10 +2713,10 @@
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>32</v>
@@ -2728,7 +2725,7 @@
         <v>21</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2736,7 +2733,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2748,7 +2745,7 @@
         <v>28</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>32</v>
@@ -2757,7 +2754,7 @@
         <v>20</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2765,7 +2762,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2774,7 +2771,7 @@
         <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>18</v>
@@ -2783,10 +2780,10 @@
         <v>32</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2794,7 +2791,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2806,7 +2803,7 @@
         <v>29</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>32</v>
@@ -2815,7 +2812,7 @@
         <v>23</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2823,7 +2820,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2844,7 +2841,7 @@
         <v>19</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2852,7 +2849,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2867,7 +2864,7 @@
         <v>30</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2875,7 +2872,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2884,19 +2881,19 @@
         <v>16</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2904,7 +2901,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2913,7 +2910,7 @@
         <v>16</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>18</v>
@@ -2922,10 +2919,10 @@
         <v>32</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2933,7 +2930,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -2942,7 +2939,7 @@
         <v>16</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>18</v>
@@ -2951,7 +2948,7 @@
         <v>32</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2959,7 +2956,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -2977,10 +2974,10 @@
         <v>32</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2988,7 +2985,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -2997,7 +2994,7 @@
         <v>16</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>18</v>
@@ -3009,10 +3006,10 @@
         <v>32</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -3020,7 +3017,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3029,7 +3026,7 @@
         <v>16</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>18</v>
@@ -3038,10 +3035,10 @@
         <v>32</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -3049,7 +3046,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3058,7 +3055,7 @@
         <v>16</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>18</v>
@@ -3070,7 +3067,7 @@
         <v>21</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3078,7 +3075,7 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3099,7 +3096,7 @@
         <v>20</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -3107,7 +3104,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3116,7 +3113,7 @@
         <v>16</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>30</v>
@@ -3125,10 +3122,10 @@
         <v>32</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3136,7 +3133,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3157,7 +3154,7 @@
         <v>23</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -3165,7 +3162,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3186,7 +3183,7 @@
         <v>19</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -3194,7 +3191,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3209,7 +3206,7 @@
         <v>31</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -3217,7 +3214,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3226,19 +3223,19 @@
         <v>16</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>32</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -3246,7 +3243,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3255,7 +3252,7 @@
         <v>16</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>30</v>
@@ -3264,10 +3261,10 @@
         <v>32</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -3275,7 +3272,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3284,7 +3281,7 @@
         <v>16</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>30</v>
@@ -3293,7 +3290,7 @@
         <v>32</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -3301,7 +3298,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3319,10 +3316,10 @@
         <v>32</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3330,7 +3327,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3339,7 +3336,7 @@
         <v>16</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>30</v>
@@ -3351,10 +3348,10 @@
         <v>32</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3362,7 +3359,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3371,7 +3368,7 @@
         <v>16</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>30</v>
@@ -3380,10 +3377,10 @@
         <v>32</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3391,7 +3388,7 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3400,7 +3397,7 @@
         <v>16</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>30</v>
@@ -3412,7 +3409,7 @@
         <v>21</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3420,7 +3417,7 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3441,7 +3438,7 @@
         <v>20</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3502,7 +3499,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3518,7 +3515,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
@@ -3620,10 +3617,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3631,7 +3628,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3643,10 +3640,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3654,7 +3651,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3669,7 +3666,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>195</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3677,7 +3674,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3692,7 +3689,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3700,7 +3697,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3715,7 +3712,7 @@
         <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3723,7 +3720,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3738,7 +3735,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3746,7 +3743,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -3755,7 +3752,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>18</v>
@@ -3766,7 +3763,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -3775,7 +3772,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>30</v>
@@ -3786,7 +3783,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -3795,7 +3792,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>31</v>
@@ -3810,7 +3807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
@@ -3846,7 +3843,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3854,7 +3851,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3866,10 +3863,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3877,7 +3874,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3892,7 +3889,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>195</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3900,7 +3897,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3915,7 +3912,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3923,7 +3920,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3938,7 +3935,7 @@
         <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3946,7 +3943,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3961,7 +3958,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -4004,7 +4001,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4012,19 +4009,19 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4032,16 +4029,16 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated RAD test cases for Existing Liability - Motor Fuel Tax
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2BAF82-5EFE-4E92-BFA7-0C9AA2704DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5CA702-696E-489F-A061-7C4C6410696D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView xWindow="32145" yWindow="2340" windowWidth="25710" windowHeight="12690" activeTab="1" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="209">
   <si>
     <t>Result</t>
   </si>
@@ -438,9 +438,6 @@
     <t>Mon Apr 08 19:22:28 EDT 2024</t>
   </si>
   <si>
-    <t>Mon Apr 08 19:23:22 EDT 2024</t>
-  </si>
-  <si>
     <t>Mon Apr 08 19:24:16 EDT 2024</t>
   </si>
   <si>
@@ -670,6 +667,9 @@
   </si>
   <si>
     <t>Mon Apr 08 20:31:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Oct 14 22:23:38 EDT 2024</t>
   </si>
 </sst>
 </file>
@@ -749,9 +749,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -789,7 +789,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -895,7 +895,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1037,7 +1037,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1296,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C2" sqref="C2:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,12 +1309,14 @@
     <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
     <col min="4" max="4" width="52" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="9.140625" style="1" collapsed="1"/>
-    <col min="9" max="9" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1337,13 +1339,16 @@
         <v>96</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1359,14 +1364,14 @@
       <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1382,14 +1387,14 @@
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1405,14 +1410,14 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1431,14 +1436,14 @@
       <c r="F5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1457,14 +1462,14 @@
       <c r="F6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1483,11 +1488,11 @@
       <c r="G7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1506,11 +1511,11 @@
       <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1529,11 +1534,11 @@
       <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1552,11 +1557,11 @@
       <c r="G10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1575,11 +1580,11 @@
       <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1598,11 +1603,11 @@
       <c r="F12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1621,16 +1626,16 @@
       <c r="G13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>208</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1642,15 +1647,18 @@
         <v>40</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1661,16 +1669,16 @@
       <c r="E15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1687,16 +1695,16 @@
       <c r="G16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1710,16 +1718,16 @@
       <c r="G17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1730,16 +1738,16 @@
       <c r="E18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -1750,7 +1758,7 @@
       <c r="E19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1817,7 +1825,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1843,7 +1851,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1866,7 +1874,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1892,7 +1900,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1918,7 +1926,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1944,7 +1952,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1979,7 +1987,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C52"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,7 +2047,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2062,7 +2070,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2088,7 +2096,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2114,7 +2122,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2140,7 +2148,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2166,7 +2174,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2189,7 +2197,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2215,7 +2223,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2241,7 +2249,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2267,7 +2275,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2293,7 +2301,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2316,7 +2324,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2342,7 +2350,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2368,7 +2376,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2394,7 +2402,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2420,7 +2428,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2449,7 +2457,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2478,7 +2486,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2507,7 +2515,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2530,7 +2538,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2559,7 +2567,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2588,7 +2596,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2614,7 +2622,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2643,7 +2651,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2675,7 +2683,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2704,7 +2712,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2733,7 +2741,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2762,7 +2770,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2791,7 +2799,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2820,7 +2828,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2849,7 +2857,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2872,7 +2880,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2901,7 +2909,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2930,7 +2938,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -2956,7 +2964,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -2985,7 +2993,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3017,7 +3025,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3046,7 +3054,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3075,7 +3083,7 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3104,7 +3112,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3133,7 +3141,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3162,7 +3170,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3191,7 +3199,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3214,7 +3222,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3243,7 +3251,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3272,7 +3280,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3298,7 +3306,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3327,7 +3335,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3359,7 +3367,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3388,7 +3396,7 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3417,7 +3425,7 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3628,7 +3636,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3651,7 +3659,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3674,7 +3682,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3697,7 +3705,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3720,7 +3728,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3743,7 +3751,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -3763,7 +3771,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -3783,7 +3791,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -3851,7 +3859,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3874,7 +3882,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3897,7 +3905,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3920,7 +3928,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3943,7 +3951,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4009,7 +4017,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4029,7 +4037,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Updated RAD MRF test case for new Motor Fuel Tax Error message
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5CA702-696E-489F-A061-7C4C6410696D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9B5CA702-696E-489F-A061-7C4C6410696D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="32145" yWindow="2340" windowWidth="25710" windowHeight="12690" activeTab="1" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView activeTab="1" windowHeight="12690" windowWidth="25710" xWindow="32145" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="2340"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
-    <sheet name="Existing" sheetId="2" r:id="rId2"/>
-    <sheet name="Extension" sheetId="3" r:id="rId3"/>
-    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
-    <sheet name="Personal" sheetId="5" r:id="rId5"/>
-    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
-    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
-    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
+    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
+    <sheet name="Existing" r:id="rId2" sheetId="2"/>
+    <sheet name="Extension" r:id="rId3" sheetId="3"/>
+    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
+    <sheet name="Personal" r:id="rId5" sheetId="5"/>
+    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
+    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
+    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="306">
   <si>
     <t>Result</t>
   </si>
@@ -670,12 +670,304 @@
   </si>
   <si>
     <t>Mon Oct 14 22:23:38 EDT 2024</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:07:25 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:08:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:09:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:10:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:11:01 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:11:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:14:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:15:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:16:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:17:02 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:17:56 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:18:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:19:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:20:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:21:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:22:23 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:23:17 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:24:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:25:04 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:25:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:26:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:27:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:28:37 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 20:29:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:27:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:28:43 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:29:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:30:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:31:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:32:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:33:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:33:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:34:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:35:37 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:36:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:37:20 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:38:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:39:04 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:39:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:40:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:41:38 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:42:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:43:21 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:44:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:45:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:45:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:46:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:47:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:48:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:49:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:50:18 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:51:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:52:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:52:56 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:53:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:54:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:55:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:56:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:57:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:58:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 21:59:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:00:00 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:00:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:01:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:02:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:03:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:04:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:05:20 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:06:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:07:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:07:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:08:51 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:09:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:10:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:11:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:12:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:13:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:14:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:15:01 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:15:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:16:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:17:40 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:18:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:19:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:20:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:21:00 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:21:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:22:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:23:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:24:17 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:25:07 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:25:56 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:26:51 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:27:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:28:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 16 22:29:38 EDT 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -724,19 +1016,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -753,10 +1045,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -791,7 +1083,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -843,7 +1135,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -954,21 +1246,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -985,7 +1277,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1037,15 +1329,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office 2013 - 2022 Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:J1"/>
@@ -1053,17 +1345,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="32.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="32.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
+    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1103,7 +1395,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>210</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1132,7 +1424,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>211</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1161,7 +1453,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>212</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1193,7 +1485,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>213</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1225,7 +1517,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>214</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1257,7 +1549,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>215</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1286,8 +1578,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1295,8 +1587,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C19"/>
@@ -1304,16 +1596,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="52" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
-    <col min="10" max="10" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="52.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1353,7 +1645,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1376,7 +1668,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>217</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1399,7 +1691,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>218</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1422,7 +1714,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>219</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1448,7 +1740,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>220</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1474,7 +1766,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>221</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1497,7 +1789,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1520,7 +1812,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>223</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1543,7 +1835,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>224</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1566,7 +1858,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1589,7 +1881,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>226</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1612,7 +1904,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1635,7 +1927,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1658,7 +1950,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>229</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1678,7 +1970,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>230</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1704,7 +1996,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>231</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1727,7 +2019,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>232</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1747,7 +2039,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>233</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -1763,7 +2055,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1771,8 +2063,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -1780,15 +2072,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1825,7 +2117,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>234</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1851,7 +2143,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>235</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1874,7 +2166,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>236</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1900,7 +2192,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>237</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1926,7 +2218,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>238</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1952,7 +2244,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>239</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1975,7 +2267,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1983,8 +2275,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:L52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -1992,16 +2284,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="10" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.140625" style="1" collapsed="1"/>
-    <col min="12" max="12" width="23.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="10" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="11" max="11" style="1" width="9.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="23.140625" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2047,7 +2339,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>240</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2070,7 +2362,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>241</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2096,7 +2388,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>242</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2122,7 +2414,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>243</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2148,7 +2440,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>244</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2174,7 +2466,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>245</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2197,7 +2489,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>246</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2223,7 +2515,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>247</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2249,7 +2541,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2275,7 +2567,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>249</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2301,7 +2593,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>250</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2324,7 +2616,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>251</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2350,7 +2642,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>252</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2376,7 +2668,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>253</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2402,7 +2694,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>254</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2428,7 +2720,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>255</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2457,7 +2749,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>256</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2486,7 +2778,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>257</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2515,7 +2807,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>258</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2538,7 +2830,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>259</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2567,7 +2859,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>162</v>
+        <v>260</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2596,7 +2888,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>261</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2622,7 +2914,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>164</v>
+        <v>262</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2651,7 +2943,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>165</v>
+        <v>263</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2683,7 +2975,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>166</v>
+        <v>264</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2712,7 +3004,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>167</v>
+        <v>265</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2741,7 +3033,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>168</v>
+        <v>266</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2770,7 +3062,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>169</v>
+        <v>267</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2799,7 +3091,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>170</v>
+        <v>268</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2828,7 +3120,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
+        <v>269</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2857,7 +3149,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>172</v>
+        <v>270</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2880,7 +3172,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>173</v>
+        <v>271</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2909,7 +3201,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>174</v>
+        <v>272</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2938,7 +3230,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>175</v>
+        <v>273</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -2964,7 +3256,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>176</v>
+        <v>274</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -2993,7 +3285,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>177</v>
+        <v>275</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3025,7 +3317,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>178</v>
+        <v>276</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3054,7 +3346,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>179</v>
+        <v>277</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3083,7 +3375,7 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>278</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3112,7 +3404,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>181</v>
+        <v>279</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3141,7 +3433,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>182</v>
+        <v>280</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3170,7 +3462,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>183</v>
+        <v>281</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3199,7 +3491,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>184</v>
+        <v>282</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3222,7 +3514,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>185</v>
+        <v>283</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3251,7 +3543,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>186</v>
+        <v>284</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3280,7 +3572,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>187</v>
+        <v>285</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3306,7 +3598,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>188</v>
+        <v>286</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3335,7 +3627,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>189</v>
+        <v>287</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3367,7 +3659,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>190</v>
+        <v>288</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3396,7 +3688,7 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>191</v>
+        <v>289</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3425,7 +3717,7 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>192</v>
+        <v>290</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3451,7 +3743,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3459,8 +3751,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3468,15 +3760,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3578,7 +3870,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3586,8 +3878,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C9"/>
@@ -3595,14 +3887,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3636,7 +3928,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>293</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3659,7 +3951,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>294</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3682,7 +3974,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>295</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3705,7 +3997,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>296</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3728,7 +4020,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>199</v>
+        <v>297</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3751,7 +4043,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>298</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -3771,7 +4063,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>201</v>
+        <v>299</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -3791,7 +4083,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -3807,13 +4099,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
@@ -3821,14 +4113,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3859,7 +4151,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>301</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3882,7 +4174,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>302</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3905,7 +4197,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>303</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3928,7 +4220,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>304</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3951,7 +4243,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>305</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3970,13 +4262,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -3984,12 +4276,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4017,7 +4309,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>291</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4037,7 +4329,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>292</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -4050,6 +4342,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Existing MRF TC
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2424" uniqueCount="603">
   <si>
     <t>Result</t>
   </si>
@@ -961,6 +961,897 @@
   </si>
   <si>
     <t>Wed Oct 16 22:29:38 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Thu Oct 17 23:54:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 17 23:56:16 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 17 23:58:02 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 17 23:59:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:01:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:03:21 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:05:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:06:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:08:43 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:10:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:12:18 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:14:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:15:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:17:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:19:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:21:18 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:23:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:24:51 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:26:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:28:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:30:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:31:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:33:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:35:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:37:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:39:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:40:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:42:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:44:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:46:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:47:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:49:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:51:33 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:53:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:55:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:56:52 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 00:58:38 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:00:25 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:02:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:03:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:05:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:07:31 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:09:17 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:11:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:12:51 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:14:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:16:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:18:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:20:02 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:21:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:23:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:25:23 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:27:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:28:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:30:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:32:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:34:21 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:36:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:37:56 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:39:45 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:41:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:43:18 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:45:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:46:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:48:40 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:50:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:52:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:54:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:55:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:57:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 01:59:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:01:16 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:03:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:04:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:06:37 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:08:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:10:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:12:00 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:13:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:15:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:17:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:19:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:20:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:22:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:24:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:26:13 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:27:58 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:29:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:31:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:33:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:34:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:36:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:38:33 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:40:23 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:42:13 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 18 02:44:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:54:37 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:55:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:56:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:57:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:58:07 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:58:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:59:52 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:00:45 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:01:37 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:02:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:03:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:04:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:05:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:06:02 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:06:56 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:07:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:08:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:09:33 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:10:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:11:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:12:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:13:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:13:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:14:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:15:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:16:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:17:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:18:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:19:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:20:02 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:20:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:21:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:22:38 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:23:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:24:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:25:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:26:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:26:58 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:27:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:28:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:29:38 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:30:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:31:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:32:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:33:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:33:58 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:34:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:35:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:36:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:37:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:38:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:39:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:40:07 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:41:00 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:41:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:42:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:43:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:44:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:45:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:46:17 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:47:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:48:02 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:48:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:49:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:50:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:51:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:52:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:53:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:54:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:55:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:56:01 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:56:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:57:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:58:40 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:59:33 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:00:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:01:20 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:02:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:03:07 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:04:01 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:04:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:05:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:06:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:07:31 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:08:25 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:09:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:10:04 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:10:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:11:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:12:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:13:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:14:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:15:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:16:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:17:00 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:17:56 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:07:01 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:08:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:10:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:12:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:14:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:16:02 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:17:52 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:19:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:21:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:23:17 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:25:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:26:52 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:28:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:30:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:32:18 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:34:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:35:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:37:43 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:39:33 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:41:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:43:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:44:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:46:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:48:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:50:23 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:52:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:53:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:55:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:57:31 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 13:59:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:01:07 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:02:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:04:40 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:06:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:08:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:10:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:11:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:13:37 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:15:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:17:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:18:58 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:20:45 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:22:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:24:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:26:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:27:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:29:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:31:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:33:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:35:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:36:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:38:45 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:40:33 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:42:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:44:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:45:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:47:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:49:37 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:51:25 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:53:13 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:55:01 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:56:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 14:58:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:00:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:02:16 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:04:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:05:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:07:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:09:31 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:11:20 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:13:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:14:58 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:16:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:18:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:20:23 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:22:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:23:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:25:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:27:37 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:29:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:31:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:33:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:34:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:36:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:38:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:40:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:41:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:43:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:45:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:47:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:48:58 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:50:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:52:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:54:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:56:18 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 15:58:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Oct 26 21:31:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Oct 26 21:32:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Oct 26 21:33:20 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Oct 26 21:34:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Oct 26 21:34:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Oct 26 21:35:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Oct 26 21:36:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Oct 26 21:37:27 EDT 2024</t>
   </si>
 </sst>
 </file>
@@ -1392,10 +2283,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>499</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1421,10 +2312,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>500</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1450,10 +2341,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>501</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1482,10 +2373,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>502</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1514,10 +2405,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>503</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1546,10 +2437,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>504</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1642,10 +2533,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>505</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1665,10 +2556,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>506</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1688,10 +2579,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B4" t="s">
-        <v>218</v>
+        <v>507</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1711,10 +2602,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>508</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1737,10 +2628,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>509</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1763,10 +2654,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>510</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1786,10 +2677,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>511</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1809,10 +2700,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>512</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1832,10 +2723,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B10" t="s">
-        <v>224</v>
+        <v>513</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1855,10 +2746,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B11" t="s">
-        <v>225</v>
+        <v>514</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1878,10 +2769,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>515</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1901,10 +2792,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B13" t="s">
-        <v>227</v>
+        <v>516</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1924,10 +2815,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>517</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1947,10 +2838,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B15" t="s">
-        <v>229</v>
+        <v>518</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1967,10 +2858,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B16" t="s">
-        <v>230</v>
+        <v>519</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1993,10 +2884,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B17" t="s">
-        <v>231</v>
+        <v>520</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2016,10 +2907,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B18" t="s">
-        <v>232</v>
+        <v>521</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2036,10 +2927,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B19" t="s">
-        <v>233</v>
+        <v>522</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2114,10 +3005,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B2" t="s">
-        <v>234</v>
+        <v>523</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2140,10 +3031,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>524</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2163,10 +3054,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B4" t="s">
-        <v>236</v>
+        <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2189,10 +3080,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B5" t="s">
-        <v>237</v>
+        <v>526</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2215,10 +3106,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>527</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2241,10 +3132,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>528</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2336,10 +3227,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>529</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2359,10 +3250,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B3" t="s">
-        <v>241</v>
+        <v>530</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2385,10 +3276,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>531</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2411,10 +3302,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>532</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2437,10 +3328,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>533</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2463,10 +3354,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>534</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2486,10 +3377,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B8" t="s">
-        <v>246</v>
+        <v>535</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2512,10 +3403,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B9" t="s">
-        <v>247</v>
+        <v>536</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2538,10 +3429,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B10" t="s">
-        <v>248</v>
+        <v>537</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2564,10 +3455,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B11" t="s">
-        <v>249</v>
+        <v>538</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2590,10 +3481,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B12" t="s">
-        <v>250</v>
+        <v>539</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2613,10 +3504,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B13" t="s">
-        <v>251</v>
+        <v>540</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2639,10 +3530,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B14" t="s">
-        <v>252</v>
+        <v>541</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2665,10 +3556,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B15" t="s">
-        <v>253</v>
+        <v>542</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2691,10 +3582,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B16" t="s">
-        <v>254</v>
+        <v>543</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2717,10 +3608,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B17" t="s">
-        <v>255</v>
+        <v>544</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2746,10 +3637,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B18" t="s">
-        <v>256</v>
+        <v>545</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2775,10 +3666,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B19" t="s">
-        <v>257</v>
+        <v>546</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2804,10 +3695,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B20" t="s">
-        <v>258</v>
+        <v>547</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2827,10 +3718,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B21" t="s">
-        <v>259</v>
+        <v>548</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2856,10 +3747,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B22" t="s">
-        <v>260</v>
+        <v>549</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2885,10 +3776,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B23" t="s">
-        <v>261</v>
+        <v>550</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2911,10 +3802,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B24" t="s">
-        <v>262</v>
+        <v>551</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2940,10 +3831,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B25" t="s">
-        <v>263</v>
+        <v>552</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2972,10 +3863,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B26" t="s">
-        <v>264</v>
+        <v>553</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -3001,10 +3892,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B27" t="s">
-        <v>265</v>
+        <v>554</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -3030,10 +3921,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B28" t="s">
-        <v>266</v>
+        <v>555</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -3059,10 +3950,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B29" t="s">
-        <v>267</v>
+        <v>556</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -3088,10 +3979,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B30" t="s">
-        <v>268</v>
+        <v>557</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -3117,10 +4008,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B31" t="s">
-        <v>269</v>
+        <v>558</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -3146,10 +4037,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B32" t="s">
-        <v>270</v>
+        <v>559</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -3169,10 +4060,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B33" t="s">
-        <v>271</v>
+        <v>560</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -3198,10 +4089,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B34" t="s">
-        <v>272</v>
+        <v>561</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -3227,10 +4118,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B35" t="s">
-        <v>273</v>
+        <v>562</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -3253,10 +4144,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B36" t="s">
-        <v>274</v>
+        <v>563</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -3282,10 +4173,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B37" t="s">
-        <v>275</v>
+        <v>564</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3314,10 +4205,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B38" t="s">
-        <v>276</v>
+        <v>565</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3343,10 +4234,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B39" t="s">
-        <v>277</v>
+        <v>566</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3372,10 +4263,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B40" t="s">
-        <v>278</v>
+        <v>567</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3401,10 +4292,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B41" t="s">
-        <v>279</v>
+        <v>568</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3430,10 +4321,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B42" t="s">
-        <v>280</v>
+        <v>569</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3459,10 +4350,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B43" t="s">
-        <v>281</v>
+        <v>570</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3488,10 +4379,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B44" t="s">
-        <v>282</v>
+        <v>571</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3511,10 +4402,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B45" t="s">
-        <v>283</v>
+        <v>572</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3540,10 +4431,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B46" t="s">
-        <v>284</v>
+        <v>573</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3569,10 +4460,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B47" t="s">
-        <v>285</v>
+        <v>574</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3595,10 +4486,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B48" t="s">
-        <v>286</v>
+        <v>575</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3624,10 +4515,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B49" t="s">
-        <v>287</v>
+        <v>576</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3656,10 +4547,10 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B50" t="s">
-        <v>288</v>
+        <v>577</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3685,10 +4576,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B51" t="s">
-        <v>289</v>
+        <v>578</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3714,10 +4605,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B52" t="s">
-        <v>290</v>
+        <v>579</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3928,7 +4819,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>595</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3951,7 +4842,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>596</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3974,7 +4865,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>295</v>
+        <v>597</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3997,7 +4888,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>598</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4020,7 +4911,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>297</v>
+        <v>599</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4043,7 +4934,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>298</v>
+        <v>600</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -4063,7 +4954,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>299</v>
+        <v>601</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -4083,7 +4974,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>300</v>
+        <v>602</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -4148,10 +5039,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B2" t="s">
-        <v>301</v>
+        <v>590</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4171,10 +5062,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B3" t="s">
-        <v>302</v>
+        <v>591</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -4194,10 +5085,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B4" t="s">
-        <v>303</v>
+        <v>592</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -4217,10 +5108,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B5" t="s">
-        <v>304</v>
+        <v>593</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4240,10 +5131,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B6" t="s">
-        <v>305</v>
+        <v>594</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4306,10 +5197,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B2" t="s">
-        <v>291</v>
+        <v>580</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4326,10 +5217,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>581</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Updated RAD Scripts to remove Estate Tax and executed in Production
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{9B5CA702-696E-489F-A061-7C4C6410696D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2189DDCF-0C02-4BFA-88E2-F2D72DFF818E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12690" windowWidth="25710" xWindow="32145" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="2340"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" activeTab="7" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
-    <sheet name="Existing" r:id="rId2" sheetId="2"/>
-    <sheet name="Extension" r:id="rId3" sheetId="3"/>
-    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
-    <sheet name="Personal" r:id="rId5" sheetId="5"/>
-    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
-    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
-    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
+    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
+    <sheet name="Existing" sheetId="2" r:id="rId2"/>
+    <sheet name="Extension" sheetId="3" r:id="rId3"/>
+    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
+    <sheet name="Personal" sheetId="5" r:id="rId5"/>
+    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
+    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
+    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2424" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="210">
   <si>
     <t>Result</t>
   </si>
@@ -384,1164 +384,9 @@
     <t>MFLicNum</t>
   </si>
   <si>
-    <t>Mon Apr 08 19:07:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:08:13 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:09:06 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:09:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:10:51 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:11:46 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:12:40 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:13:32 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:14:25 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:15:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:16:13 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:17:06 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:18:00 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:18:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:19:48 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:20:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:21:35 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:22:28 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:24:16 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:25:09 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:26:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:26:56 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:27:50 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:28:44 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:29:36 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:30:29 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:31:21 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:32:13 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:33:07 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:34:01 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:34:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:35:48 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:36:41 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:37:34 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:38:26 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:39:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:40:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:41:04 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:41:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:42:50 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:43:44 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:44:37 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:45:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:46:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:47:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:48:10 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:49:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:49:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:50:52 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:51:47 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:52:41 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:53:35 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:54:29 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:55:24 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:56:20 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:57:14 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:58:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:59:02 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 19:59:56 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:00:50 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:01:43 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:02:37 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:03:31 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:04:24 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:05:20 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:06:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:07:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:08:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:08:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:09:50 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:10:45 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:11:39 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:12:31 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:13:26 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:14:21 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:15:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:16:10 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:17:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:17:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:18:53 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:19:46 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:20:38 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:21:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:22:20 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:23:09 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:23:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:24:51 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:25:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:26:32 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:27:21 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:28:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:29:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:30:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:31:01 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Apr 08 20:31:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Oct 14 22:23:38 EDT 2024</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:07:25 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:08:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:09:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:10:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:11:01 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:11:53 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:14:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:15:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:16:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:17:02 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:17:56 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:18:48 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:19:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:20:36 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:21:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:22:23 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:23:17 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:24:10 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:25:04 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:25:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:26:50 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:27:44 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:28:37 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 20:29:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:27:47 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:28:43 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:29:36 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:30:28 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:31:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:32:11 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:33:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:33:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:34:46 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:35:37 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:36:29 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:37:20 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:38:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:39:04 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:39:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:40:47 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:41:38 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:42:29 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:43:21 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:44:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:45:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:45:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:46:48 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:47:41 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:48:34 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:49:26 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:50:18 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:51:11 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:52:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:52:56 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:53:49 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:54:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:55:35 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:56:29 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:57:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:58:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 21:59:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:00:00 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:00:53 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:01:47 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:02:39 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:03:32 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:04:26 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:05:20 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:06:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:07:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:07:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:08:51 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:09:44 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:10:36 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:11:29 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:12:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:13:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:14:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:15:01 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:15:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:16:47 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:17:40 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:18:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:19:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:20:11 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:21:00 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:21:49 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:22:39 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:23:28 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:24:17 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:25:07 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:25:56 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:26:51 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:27:47 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:28:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 16 22:29:38 EDT 2024</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>Thu Oct 17 23:54:28 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 17 23:56:16 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 17 23:58:02 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 17 23:59:49 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:01:35 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:03:21 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:05:09 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:06:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:08:43 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:10:32 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:12:18 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:14:06 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:15:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:17:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:19:29 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:21:18 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:23:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:24:51 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:26:39 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:28:26 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:30:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:31:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:33:47 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:35:34 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:37:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:39:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:40:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:42:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:44:27 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:46:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:47:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:49:46 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:51:33 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:53:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:55:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:56:52 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 00:58:38 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:00:25 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:02:11 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:03:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:05:44 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:07:31 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:09:17 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:11:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:12:51 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:14:39 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:16:26 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:18:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:20:02 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:21:48 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:23:35 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:25:23 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:27:11 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:28:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:30:46 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:32:34 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:34:21 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:36:09 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:37:56 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:39:45 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:41:32 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:43:18 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:45:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:46:53 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:48:40 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:50:28 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:52:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:54:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:55:53 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:57:41 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 01:59:29 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:01:16 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:03:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:04:49 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:06:37 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:08:24 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:10:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:12:00 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:13:47 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:15:35 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:17:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:19:11 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:20:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:22:44 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:24:28 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:26:13 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:27:58 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:29:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:31:27 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:33:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:34:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:36:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:38:33 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:40:23 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:42:13 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 18 02:44:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 22:54:37 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 22:55:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 22:56:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 22:57:14 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 22:58:07 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 22:58:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 22:59:52 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:00:45 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:01:37 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:02:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:03:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:04:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:05:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:06:02 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:06:56 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:07:49 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:08:41 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:09:33 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:10:26 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:11:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:12:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:13:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:13:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:14:49 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:15:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:16:34 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:17:26 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:18:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:19:11 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:20:02 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:20:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:21:46 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:22:38 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:23:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:24:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:25:14 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:26:06 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:26:58 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:27:50 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:28:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:29:38 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:30:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:31:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:32:14 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:33:06 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:33:58 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:34:50 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:35:44 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:36:36 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:37:29 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:38:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:39:14 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:40:07 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:41:00 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:41:53 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:42:46 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:43:39 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:44:32 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:45:24 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:46:17 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:47:11 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:48:02 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:48:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:49:49 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:50:41 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:51:34 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:52:28 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:53:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:54:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:55:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:56:01 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:56:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:57:47 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:58:40 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Oct 24 23:59:33 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:00:27 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:01:20 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:02:14 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:03:07 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:04:01 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:04:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:05:48 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:06:39 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:07:31 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:08:25 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:09:14 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:10:04 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:10:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:11:44 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:12:34 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:13:24 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:14:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:15:10 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:16:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:17:00 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 00:17:56 EDT 2024</t>
-  </si>
-  <si>
     <t>Fri Oct 25 13:07:01 EDT 2024</t>
   </si>
   <si>
@@ -1789,30 +634,6 @@
   </si>
   <si>
     <t>Fri Oct 25 15:34:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 15:36:41 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 15:38:27 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 15:40:11 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 15:41:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 15:43:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 15:45:27 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 15:47:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 15:48:58 EDT 2024</t>
   </si>
   <si>
     <t>Fri Oct 25 15:50:44 EDT 2024</t>
@@ -1858,7 +679,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1907,19 +727,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1936,10 +756,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1974,7 +794,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2026,7 +846,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2137,21 +957,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2168,7 +988,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2220,15 +1040,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office 2013 - 2022 Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:J1"/>
@@ -2236,17 +1056,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
-    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2283,10 +1103,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>499</v>
+        <v>114</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2312,10 +1132,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>500</v>
+        <v>115</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2341,10 +1161,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>501</v>
+        <v>116</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2373,10 +1193,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>502</v>
+        <v>117</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2405,10 +1225,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>503</v>
+        <v>118</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2437,10 +1257,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>504</v>
+        <v>119</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2469,8 +1289,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2478,25 +1298,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:K19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="52.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="52" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2533,10 +1353,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>505</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2556,10 +1376,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>506</v>
+        <v>121</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2579,10 +1399,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>507</v>
+        <v>122</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2602,10 +1422,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>508</v>
+        <v>123</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2628,10 +1448,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>509</v>
+        <v>124</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2654,10 +1474,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>510</v>
+        <v>125</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2677,10 +1497,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>511</v>
+        <v>126</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2700,10 +1520,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>512</v>
+        <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2723,10 +1543,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>513</v>
+        <v>128</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2746,10 +1566,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>514</v>
+        <v>129</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2769,10 +1589,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
-        <v>515</v>
+        <v>130</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2792,10 +1612,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>516</v>
+        <v>131</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2815,10 +1635,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>517</v>
+        <v>132</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2838,10 +1658,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>518</v>
+        <v>133</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2858,10 +1678,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>519</v>
+        <v>134</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2884,10 +1704,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
-        <v>520</v>
+        <v>135</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2907,10 +1727,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>521</v>
+        <v>136</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2927,10 +1747,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>522</v>
+        <v>137</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2946,7 +1766,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2954,8 +1774,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -2963,15 +1783,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3005,10 +1825,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>523</v>
+        <v>138</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3031,10 +1851,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>524</v>
+        <v>139</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3054,10 +1874,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>525</v>
+        <v>140</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3080,10 +1900,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>526</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3106,10 +1926,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>527</v>
+        <v>142</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3132,10 +1952,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>528</v>
+        <v>143</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -3158,7 +1978,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3166,25 +1986,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:M52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="10" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="11" max="11" style="1" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="23.140625" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="10" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" style="1" collapsed="1"/>
+    <col min="12" max="12" width="23.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3227,10 +2047,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>529</v>
+        <v>144</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3250,10 +2070,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>530</v>
+        <v>145</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3276,10 +2096,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>531</v>
+        <v>146</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3302,10 +2122,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>532</v>
+        <v>147</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3328,10 +2148,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>533</v>
+        <v>148</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3354,10 +2174,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>534</v>
+        <v>149</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -3377,10 +2197,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>535</v>
+        <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -3403,10 +2223,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>536</v>
+        <v>151</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -3429,10 +2249,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>537</v>
+        <v>152</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -3455,10 +2275,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>538</v>
+        <v>153</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -3481,10 +2301,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
-        <v>539</v>
+        <v>154</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -3504,10 +2324,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>540</v>
+        <v>155</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -3530,10 +2350,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>541</v>
+        <v>156</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -3556,10 +2376,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>542</v>
+        <v>157</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -3582,10 +2402,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>543</v>
+        <v>158</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -3608,10 +2428,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
-        <v>544</v>
+        <v>159</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -3637,10 +2457,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>545</v>
+        <v>160</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -3666,10 +2486,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>546</v>
+        <v>161</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -3695,10 +2515,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>547</v>
+        <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -3718,10 +2538,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
-        <v>548</v>
+        <v>163</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -3747,10 +2567,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>549</v>
+        <v>164</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -3776,10 +2596,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>550</v>
+        <v>165</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -3802,10 +2622,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B24" t="s">
-        <v>551</v>
+        <v>166</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -3831,10 +2651,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>552</v>
+        <v>167</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -3863,10 +2683,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B26" t="s">
-        <v>553</v>
+        <v>168</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -3892,10 +2712,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>554</v>
+        <v>169</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -3921,10 +2741,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>555</v>
+        <v>170</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -3950,10 +2770,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
-        <v>556</v>
+        <v>171</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -3979,10 +2799,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>557</v>
+        <v>172</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -4008,10 +2828,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B31" t="s">
-        <v>558</v>
+        <v>173</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -4037,10 +2857,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B32" t="s">
-        <v>559</v>
+        <v>174</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -4060,10 +2880,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B33" t="s">
-        <v>560</v>
+        <v>175</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -4089,10 +2909,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B34" t="s">
-        <v>561</v>
+        <v>176</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -4118,10 +2938,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>562</v>
+        <v>177</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -4144,10 +2964,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B36" t="s">
-        <v>563</v>
+        <v>178</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -4173,10 +2993,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B37" t="s">
-        <v>564</v>
+        <v>179</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -4205,10 +3025,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>565</v>
+        <v>180</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -4234,10 +3054,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B39" t="s">
-        <v>566</v>
+        <v>181</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -4263,10 +3083,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>567</v>
+        <v>182</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -4292,10 +3112,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>568</v>
+        <v>183</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -4321,10 +3141,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B42" t="s">
-        <v>569</v>
+        <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -4350,10 +3170,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B43" t="s">
-        <v>570</v>
+        <v>185</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -4379,10 +3199,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
-        <v>571</v>
+        <v>186</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -4402,10 +3222,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>572</v>
+        <v>187</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -4431,10 +3251,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>573</v>
+        <v>188</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -4460,10 +3280,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B47" t="s">
-        <v>574</v>
+        <v>189</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -4486,10 +3306,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>575</v>
+        <v>190</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -4515,10 +3335,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B49" t="s">
-        <v>576</v>
+        <v>191</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -4547,10 +3367,10 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B50" t="s">
-        <v>577</v>
+        <v>192</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -4576,10 +3396,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B51" t="s">
-        <v>578</v>
+        <v>193</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -4605,10 +3425,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B52" t="s">
-        <v>579</v>
+        <v>194</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -4634,7 +3454,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4642,8 +3462,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -4651,15 +3471,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4761,7 +3581,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4769,23 +3589,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+      <selection activeCell="C7" sqref="C7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4819,7 +3639,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>595</v>
+        <v>202</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4842,7 +3662,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>596</v>
+        <v>203</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -4865,7 +3685,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>597</v>
+        <v>204</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -4888,7 +3708,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>598</v>
+        <v>205</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4911,7 +3731,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>599</v>
+        <v>206</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4934,10 +3754,10 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>600</v>
+        <v>207</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
@@ -4954,10 +3774,10 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>601</v>
+        <v>208</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -4974,10 +3794,10 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>602</v>
+        <v>209</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -4990,13 +3810,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
@@ -5004,14 +3824,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5039,10 +3859,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>590</v>
+        <v>197</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -5062,10 +3882,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>591</v>
+        <v>198</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -5085,10 +3905,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>592</v>
+        <v>199</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -5108,10 +3928,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>593</v>
+        <v>200</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -5131,10 +3951,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>594</v>
+        <v>201</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -5153,26 +3973,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5197,10 +4017,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>580</v>
+        <v>195</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -5217,13 +4037,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>581</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>111</v>
@@ -5233,6 +4053,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RAD Test Cases for Year dropdown
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2189DDCF-0C02-4BFA-88E2-F2D72DFF818E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{7277DB49-CE81-4C06-9F80-FA3F48F216DD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" activeTab="7" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
+    <workbookView activeTab="6" windowHeight="16920" windowWidth="30960" xWindow="-120" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
-    <sheet name="Existing" sheetId="2" r:id="rId2"/>
-    <sheet name="Extension" sheetId="3" r:id="rId3"/>
-    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
-    <sheet name="Personal" sheetId="5" r:id="rId5"/>
-    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
-    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
-    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
+    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
+    <sheet name="Existing" r:id="rId2" sheetId="2"/>
+    <sheet name="Extension" r:id="rId3" sheetId="3"/>
+    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
+    <sheet name="Personal" r:id="rId5" sheetId="5"/>
+    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
+    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
+    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="304">
   <si>
     <t>Result</t>
   </si>
@@ -673,12 +673,295 @@
   </si>
   <si>
     <t>Sat Oct 26 21:37:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:14:59 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:15:52 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:16:44 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:17:36 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:18:28 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:19:20 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:20:13 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:21:05 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:21:57 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:22:50 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:23:42 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:24:35 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:25:28 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:26:21 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:27:14 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:28:07 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:29:00 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:29:52 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:30:45 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:31:38 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:32:31 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:33:24 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:34:17 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:35:52 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:37:26 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:38:19 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:39:11 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:40:02 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:40:54 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:41:47 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:42:39 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:43:32 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:44:24 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:45:17 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:46:09 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:47:01 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:47:53 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:48:45 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:49:37 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:50:29 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:51:21 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:52:13 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:53:05 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:53:57 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:54:50 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:55:42 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:56:35 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:57:28 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:58:22 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 28 23:59:14 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:00:07 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:01:00 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:01:52 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:02:46 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:03:41 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:04:34 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:06:09 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:07:07 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:08:00 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:08:55 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:09:48 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:10:40 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:11:34 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:12:28 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:13:21 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:14:15 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:15:08 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:16:02 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:17:37 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:18:34 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:19:27 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:20:21 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:21:14 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:22:05 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:22:58 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:23:52 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:24:44 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:25:38 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:26:31 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:27:24 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:28:59 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:29:57 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:30:50 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:31:40 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:32:30 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:33:20 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:34:09 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:35:01 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:35:56 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:36:52 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:37:47 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 00:38:42 EST 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -727,19 +1010,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -756,10 +1039,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -794,7 +1077,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -846,7 +1129,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -957,21 +1240,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -988,7 +1271,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1040,33 +1323,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office 2013 - 2022 Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="32.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="32.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
+    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1103,10 +1386,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1118,7 +1401,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
+        <v>210</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>19</v>
@@ -1132,10 +1415,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1147,7 +1430,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>210</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>20</v>
@@ -1161,10 +1444,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>214</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1176,7 +1459,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>37</v>
+        <v>210</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -1193,10 +1476,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>215</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1208,7 +1491,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>210</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>22</v>
@@ -1225,10 +1508,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>216</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1240,7 +1523,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>210</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>23</v>
@@ -1257,10 +1540,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>217</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1272,7 +1555,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>210</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
@@ -1289,8 +1572,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1298,8 +1581,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C19"/>
@@ -1307,16 +1590,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="52" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
-    <col min="10" max="10" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="52.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1353,10 +1636,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>218</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1376,10 +1659,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>219</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1399,10 +1682,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>220</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1422,10 +1705,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>221</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1448,10 +1731,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>222</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1474,10 +1757,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>223</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1497,10 +1780,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>224</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1520,10 +1803,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1543,10 +1826,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>226</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1566,10 +1849,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>227</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1589,10 +1872,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>228</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1612,10 +1895,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>229</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1635,10 +1918,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>230</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1658,10 +1941,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>231</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1678,10 +1961,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>232</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1704,10 +1987,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>233</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1730,7 +2013,7 @@
         <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>136</v>
+        <v>234</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1750,7 +2033,7 @@
         <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>235</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -1766,7 +2049,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1774,24 +2057,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1825,10 +2108,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>236</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1840,7 +2123,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>22</v>
@@ -1851,10 +2134,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>237</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1866,7 +2149,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>106</v>
@@ -1874,10 +2157,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>238</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1889,7 +2172,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>32</v>
@@ -1900,10 +2183,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>239</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1915,7 +2198,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>32</v>
@@ -1926,10 +2209,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>240</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1941,7 +2224,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>32</v>
@@ -1952,10 +2235,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>241</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1967,7 +2250,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>32</v>
@@ -1978,7 +2261,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1986,25 +2269,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:L52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="10" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.140625" style="1" collapsed="1"/>
-    <col min="12" max="12" width="23.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="10" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="11" max="11" style="1" width="9.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="23.140625" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2047,10 +2330,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>242</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2061,8 +2344,8 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
+      <c r="F2" s="1">
+        <v>2024</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>76</v>
@@ -2070,10 +2353,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>243</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2084,8 +2367,8 @@
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
+      <c r="F3" s="1">
+        <v>2024</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>32</v>
@@ -2096,10 +2379,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>244</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2110,8 +2393,8 @@
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
+      <c r="F4" s="1">
+        <v>2024</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>32</v>
@@ -2122,10 +2405,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>245</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2136,8 +2419,8 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
+      <c r="F5" s="1">
+        <v>2024</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
@@ -2148,10 +2431,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>246</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2162,8 +2445,8 @@
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
+      <c r="F6" s="1">
+        <v>2024</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>32</v>
@@ -2174,10 +2457,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>247</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2188,8 +2471,8 @@
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
+      <c r="F7" s="1">
+        <v>2023</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>76</v>
@@ -2197,10 +2480,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2211,8 +2494,8 @@
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>30</v>
+      <c r="F8" s="1">
+        <v>2023</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>32</v>
@@ -2223,10 +2506,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>249</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2237,8 +2520,8 @@
       <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
+      <c r="F9" s="1">
+        <v>2023</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>32</v>
@@ -2249,10 +2532,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>250</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2263,8 +2546,8 @@
       <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
+      <c r="F10" s="1">
+        <v>2023</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>32</v>
@@ -2275,10 +2558,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>251</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2289,8 +2572,8 @@
       <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>30</v>
+      <c r="F11" s="1">
+        <v>2023</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>32</v>
@@ -2301,10 +2584,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>252</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2315,8 +2598,8 @@
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>31</v>
+      <c r="F12" s="1">
+        <v>2022</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>76</v>
@@ -2324,10 +2607,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>253</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2338,8 +2621,8 @@
       <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>31</v>
+      <c r="F13" s="1">
+        <v>2022</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>32</v>
@@ -2350,10 +2633,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>254</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2364,8 +2647,8 @@
       <c r="E14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>31</v>
+      <c r="F14" s="1">
+        <v>2022</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>32</v>
@@ -2376,10 +2659,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>255</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2390,8 +2673,8 @@
       <c r="E15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>31</v>
+      <c r="F15" s="1">
+        <v>2022</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>32</v>
@@ -2402,10 +2685,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>256</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2416,8 +2699,8 @@
       <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>31</v>
+      <c r="F16" s="1">
+        <v>2022</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>32</v>
@@ -2428,10 +2711,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>257</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2442,8 +2725,8 @@
       <c r="E17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>37</v>
+      <c r="F17" s="1">
+        <v>2025</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>32</v>
@@ -2457,10 +2740,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>258</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2471,8 +2754,8 @@
       <c r="E18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>37</v>
+      <c r="F18" s="1">
+        <v>2025</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>32</v>
@@ -2486,10 +2769,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>259</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2500,8 +2783,8 @@
       <c r="E19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>37</v>
+      <c r="F19" s="1">
+        <v>2025</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>32</v>
@@ -2515,10 +2798,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>162</v>
+        <v>260</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2529,8 +2812,8 @@
       <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>18</v>
+      <c r="F20" s="1">
+        <v>2024</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>84</v>
@@ -2538,10 +2821,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>261</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2552,8 +2835,8 @@
       <c r="E21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>37</v>
+      <c r="F21" s="1">
+        <v>2025</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>98</v>
@@ -2567,10 +2850,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>164</v>
+        <v>262</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2581,8 +2864,8 @@
       <c r="E22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>37</v>
+      <c r="F22" s="1">
+        <v>2025</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>32</v>
@@ -2596,10 +2879,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>263</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2610,8 +2893,8 @@
       <c r="E23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>37</v>
+      <c r="F23" s="1">
+        <v>2025</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>32</v>
@@ -2622,10 +2905,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>166</v>
+        <v>264</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2636,8 +2919,8 @@
       <c r="E24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>37</v>
+      <c r="F24" s="1">
+        <v>2025</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
@@ -2651,10 +2934,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>167</v>
+        <v>265</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2665,8 +2948,8 @@
       <c r="E25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>37</v>
+      <c r="F25" s="1">
+        <v>2025</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>32</v>
@@ -2683,10 +2966,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>266</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2697,8 +2980,8 @@
       <c r="E26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>37</v>
+      <c r="F26" s="1">
+        <v>2025</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>32</v>
@@ -2715,7 +2998,7 @@
         <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>267</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2726,8 +3009,8 @@
       <c r="E27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>37</v>
+      <c r="F27" s="1">
+        <v>2025</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>32</v>
@@ -2744,7 +3027,7 @@
         <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
+        <v>268</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2755,8 +3038,8 @@
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>37</v>
+      <c r="F28" s="1">
+        <v>2025</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>32</v>
@@ -2770,10 +3053,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>171</v>
+        <v>269</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2784,8 +3067,8 @@
       <c r="E29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>18</v>
+      <c r="F29" s="1">
+        <v>2024</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>32</v>
@@ -2799,10 +3082,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>172</v>
+        <v>270</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2813,8 +3096,8 @@
       <c r="E30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>37</v>
+      <c r="F30" s="1">
+        <v>2025</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>32</v>
@@ -2828,10 +3111,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>173</v>
+        <v>271</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -2842,8 +3125,8 @@
       <c r="E31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>18</v>
+      <c r="F31" s="1">
+        <v>2024</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>
@@ -2857,10 +3140,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
+        <v>272</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2871,8 +3154,8 @@
       <c r="E32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>30</v>
+      <c r="F32" s="1">
+        <v>2023</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>84</v>
@@ -2880,10 +3163,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>175</v>
+        <v>273</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2894,8 +3177,8 @@
       <c r="E33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>18</v>
+      <c r="F33" s="1">
+        <v>2024</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>98</v>
@@ -2909,10 +3192,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>176</v>
+        <v>274</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2923,8 +3206,8 @@
       <c r="E34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>18</v>
+      <c r="F34" s="1">
+        <v>2024</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>32</v>
@@ -2938,10 +3221,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>177</v>
+        <v>275</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -2952,8 +3235,8 @@
       <c r="E35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>18</v>
+      <c r="F35" s="1">
+        <v>2024</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>32</v>
@@ -2964,10 +3247,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>178</v>
+        <v>276</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -2978,8 +3261,8 @@
       <c r="E36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>18</v>
+      <c r="F36" s="1">
+        <v>2024</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>32</v>
@@ -2993,10 +3276,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>179</v>
+        <v>277</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3007,8 +3290,8 @@
       <c r="E37" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>18</v>
+      <c r="F37" s="1">
+        <v>2024</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>32</v>
@@ -3025,10 +3308,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>180</v>
+        <v>278</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3039,8 +3322,8 @@
       <c r="E38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>18</v>
+      <c r="F38" s="1">
+        <v>2024</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>32</v>
@@ -3057,7 +3340,7 @@
         <v>113</v>
       </c>
       <c r="B39" t="s">
-        <v>181</v>
+        <v>279</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3068,8 +3351,8 @@
       <c r="E39" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>18</v>
+      <c r="F39" s="1">
+        <v>2024</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>32</v>
@@ -3086,7 +3369,7 @@
         <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>182</v>
+        <v>280</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3097,8 +3380,8 @@
       <c r="E40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>18</v>
+      <c r="F40" s="1">
+        <v>2024</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>32</v>
@@ -3112,10 +3395,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>183</v>
+        <v>281</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3126,8 +3409,8 @@
       <c r="E41" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>30</v>
+      <c r="F41" s="1">
+        <v>2023</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>32</v>
@@ -3141,10 +3424,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>184</v>
+        <v>282</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3155,8 +3438,8 @@
       <c r="E42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>30</v>
+      <c r="F42" s="1">
+        <v>2023</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>32</v>
@@ -3170,10 +3453,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>185</v>
+        <v>283</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3184,8 +3467,8 @@
       <c r="E43" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>30</v>
+      <c r="F43" s="1">
+        <v>2023</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>32</v>
@@ -3199,10 +3482,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>186</v>
+        <v>284</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3213,8 +3496,8 @@
       <c r="E44" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>31</v>
+      <c r="F44" s="1">
+        <v>2022</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>84</v>
@@ -3222,10 +3505,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>285</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3236,8 +3519,8 @@
       <c r="E45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>30</v>
+      <c r="F45" s="1">
+        <v>2023</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>98</v>
@@ -3251,10 +3534,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>188</v>
+        <v>286</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3265,8 +3548,8 @@
       <c r="E46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>30</v>
+      <c r="F46" s="1">
+        <v>2023</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>32</v>
@@ -3280,10 +3563,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>189</v>
+        <v>287</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3294,8 +3577,8 @@
       <c r="E47" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>30</v>
+      <c r="F47" s="1">
+        <v>2023</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>32</v>
@@ -3306,10 +3589,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
+        <v>288</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3320,8 +3603,8 @@
       <c r="E48" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>30</v>
+      <c r="F48" s="1">
+        <v>2023</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>32</v>
@@ -3335,10 +3618,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>191</v>
+        <v>289</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3349,8 +3632,8 @@
       <c r="E49" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>30</v>
+      <c r="F49" s="1">
+        <v>2023</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>32</v>
@@ -3367,10 +3650,10 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>192</v>
+        <v>290</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3381,8 +3664,8 @@
       <c r="E50" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>30</v>
+      <c r="F50" s="1">
+        <v>2023</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>32</v>
@@ -3399,7 +3682,7 @@
         <v>113</v>
       </c>
       <c r="B51" t="s">
-        <v>193</v>
+        <v>291</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3410,8 +3693,8 @@
       <c r="E51" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>30</v>
+      <c r="F51" s="1">
+        <v>2023</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>32</v>
@@ -3428,7 +3711,7 @@
         <v>113</v>
       </c>
       <c r="B52" t="s">
-        <v>194</v>
+        <v>292</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3439,8 +3722,8 @@
       <c r="E52" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>30</v>
+      <c r="F52" s="1">
+        <v>2023</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>32</v>
@@ -3454,7 +3737,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3462,8 +3745,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3471,15 +3754,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3581,7 +3864,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3589,23 +3872,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C9"/>
+      <selection activeCell="F7" sqref="F7:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3639,7 +3922,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>294</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3651,7 +3934,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
+        <v>210</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>93</v>
@@ -3662,7 +3945,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3674,7 +3957,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>103</v>
@@ -3685,7 +3968,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>296</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3697,7 +3980,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>94</v>
@@ -3708,7 +3991,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>297</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3720,7 +4003,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>94</v>
@@ -3731,7 +4014,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>298</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3743,7 +4026,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>94</v>
@@ -3766,7 +4049,7 @@
         <v>39</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3786,7 +4069,7 @@
         <v>39</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3806,32 +4089,32 @@
         <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3859,10 +4142,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>299</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -3874,7 +4157,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
+        <v>210</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>93</v>
@@ -3882,10 +4165,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>300</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -3897,7 +4180,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>103</v>
@@ -3905,10 +4188,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>301</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -3920,7 +4203,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>94</v>
@@ -3928,10 +4211,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>302</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -3943,7 +4226,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>94</v>
@@ -3951,10 +4234,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>303</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3966,33 +4249,33 @@
         <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4017,10 +4300,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>293</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4053,6 +4336,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RAD Summary Test Cases to include isRequiredTextPresent
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{9DACB5EB-97F7-43E2-81EF-9582CC15E659}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BFA2E8-9715-42BD-884A-2291E3EA6A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="7" windowHeight="16920" windowWidth="30960" xWindow="30600" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="-120"/>
+    <workbookView xWindow="30600" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
-    <sheet name="Existing" r:id="rId2" sheetId="2"/>
-    <sheet name="Extension" r:id="rId3" sheetId="3"/>
-    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
-    <sheet name="Personal" r:id="rId5" sheetId="5"/>
-    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
-    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
-    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
+    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
+    <sheet name="Existing" sheetId="2" r:id="rId2"/>
+    <sheet name="Extension" sheetId="3" r:id="rId3"/>
+    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
+    <sheet name="Personal" sheetId="5" r:id="rId5"/>
+    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
+    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
+    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">NewTaxReturn!$E$1:$E$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">NewTaxReturn!$E$1:$E$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="225">
   <si>
     <t>Result</t>
   </si>
@@ -393,629 +393,340 @@
     <t>2025</t>
   </si>
   <si>
-    <t>Tue Jan 28 23:14:59 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:15:52 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:16:44 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:17:36 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:18:28 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:19:20 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:20:13 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:21:05 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:21:57 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:22:50 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:23:42 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:24:35 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:25:28 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:26:21 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:27:14 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:28:07 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:29:00 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:29:52 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:30:45 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:31:38 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:32:31 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:33:24 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:37:26 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:38:19 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:39:11 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:40:02 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:40:54 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:41:47 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:42:39 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:43:32 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:44:24 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:45:17 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:46:09 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:47:01 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:47:53 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:48:45 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:49:37 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:50:29 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:51:21 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:52:13 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:53:05 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:53:57 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:54:50 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:55:42 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:56:35 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:57:28 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:58:22 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Jan 28 23:59:14 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:00:07 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:01:00 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:01:52 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:02:46 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:03:41 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:07:07 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:08:00 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:08:55 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:09:48 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:10:40 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:11:34 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:12:28 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:13:21 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:14:15 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:15:08 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:18:34 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:19:27 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:20:21 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:21:14 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:22:05 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:22:58 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:23:52 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:24:44 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:25:38 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:26:31 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:35:01 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:35:56 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:36:52 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:37:47 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Jan 29 00:38:42 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:15:39 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:16:31 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:19:37 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:20:35 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:21:38 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:22:36 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:23:35 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:24:26 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:25:18 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:26:07 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:26:57 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:27:46 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:28:34 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:29:24 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:30:12 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 17:31:01 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 18:07:14 EST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 18:08:19 EST 2025</t>
-  </si>
-  <si>
     <t>PTE Composite</t>
   </si>
   <si>
     <t>Digital Advertising Gross Revenues</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:07:53 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:08:46 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:09:37 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:10:29 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:11:21 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:12:13 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:13:05 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:13:58 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:14:49 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:15:40 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:16:32 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:17:24 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:18:16 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:19:10 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:20:02 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:20:55 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:21:46 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:22:38 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:23:31 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:24:24 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:25:15 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:26:08 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:27:00 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:27:52 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:28:44 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:29:37 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:30:29 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:31:20 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:32:12 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:33:03 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:33:54 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:34:46 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:35:38 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:36:29 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:37:21 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:38:12 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:39:04 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:39:56 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:40:47 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:41:39 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:42:31 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:43:22 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:44:14 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:45:06 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:45:57 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:46:48 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:47:40 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:48:31 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:49:24 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:50:18 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:51:10 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:52:03 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:52:56 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:53:48 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:54:40 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:55:33 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:56:26 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:57:19 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:58:17 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 11 23:59:15 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:00:08 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:01:00 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:01:52 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:02:44 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:03:37 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:04:30 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:05:24 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:06:17 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:07:09 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:08:02 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:09:00 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:09:57 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:10:51 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:11:44 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:12:37 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:13:31 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:14:23 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:15:16 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:16:09 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:17:03 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:17:55 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:18:48 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:19:46 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:20:43 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:21:39 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:22:35 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:23:31 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:24:27 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:25:23 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:26:19 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:27:15 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:28:11 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:29:08 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:29:59 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:30:50 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:31:38 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:32:27 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:33:17 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:34:05 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:34:54 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:35:43 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:36:33 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:37:22 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:38:18 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:39:12 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:40:07 EST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 12 00:41:01 EST 2025</t>
+    <t>Mon Feb 17 18:05:00 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:05:57 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:06:49 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:07:41 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:08:33 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:09:25 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:10:17 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:12:12 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:14:06 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:16:00 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:16:51 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:17:43 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:19:37 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:21:33 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:23:28 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:25:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:26:15 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:27:06 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:29:00 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:30:56 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:32:50 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:33:42 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:35:37 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:36:29 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:37:21 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:39:15 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:40:07 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:40:59 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:41:50 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:42:41 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:43:32 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:44:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:45:16 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:46:08 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:46:59 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:47:50 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:48:42 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:49:33 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:50:25 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:51:16 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:52:08 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:52:58 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:53:50 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:54:42 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:55:33 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:56:25 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:57:16 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:58:08 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:59:00 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 18:59:53 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:00:46 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:01:37 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:02:30 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:03:22 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:04:14 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:05:06 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:06:00 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:07:46 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:08:43 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:09:36 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:10:29 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:11:21 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:12:12 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:13:05 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:13:58 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:14:50 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:15:44 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:16:37 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:18:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:19:20 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:20:14 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:21:07 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:21:59 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:22:50 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:23:42 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:24:35 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:25:27 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:26:20 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:27:12 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:28:58 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:29:54 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:30:46 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:31:37 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:32:29 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:33:20 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:34:11 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:35:03 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:35:55 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:36:46 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:37:38 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:38:28 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:39:19 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:40:08 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:40:57 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:41:45 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:42:33 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:43:22 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:44:11 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:44:59 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:45:48 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:46:42 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:47:37 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:48:32 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 17 19:49:26 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Feb 18 17:15:40 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Feb 18 17:16:39 EST 2025</t>
+  </si>
+  <si>
+    <t>Tue Feb 18 17:17:34 EST 2025</t>
+  </si>
+  <si>
+    <t>Incorrect App ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1064,19 +775,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1093,10 +804,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1131,7 +842,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1183,7 +894,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1294,21 +1005,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1325,7 +1036,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1377,33 +1088,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office 2013 - 2022 Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="44.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="35.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
-    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="44.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1443,7 +1154,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
+        <v>117</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1472,7 +1183,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>118</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1501,7 +1212,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>216</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1533,7 +1244,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>120</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1565,7 +1276,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>218</v>
+        <v>121</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1597,7 +1308,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1626,8 +1337,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1635,8 +1346,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:K21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15:C21"/>
@@ -1644,16 +1355,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="52.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="52" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1693,7 +1404,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>123</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1716,7 +1427,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>124</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1739,7 +1450,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>125</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1762,7 +1473,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>223</v>
+        <v>126</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1788,7 +1499,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>224</v>
+        <v>127</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1814,7 +1525,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>225</v>
+        <v>128</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1837,7 +1548,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>129</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1860,7 +1571,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>130</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1883,7 +1594,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>131</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1906,7 +1617,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>229</v>
+        <v>132</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1929,7 +1640,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>230</v>
+        <v>133</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1952,7 +1663,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>134</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1975,7 +1686,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>232</v>
+        <v>135</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1998,7 +1709,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>233</v>
+        <v>136</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2018,7 +1729,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>234</v>
+        <v>137</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2044,7 +1755,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>235</v>
+        <v>138</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2067,7 +1778,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>236</v>
+        <v>139</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2090,7 +1801,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>237</v>
+        <v>140</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2113,7 +1824,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>238</v>
+        <v>141</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2122,7 +1833,7 @@
         <v>111</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>212</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2130,7 +1841,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>239</v>
+        <v>142</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2139,14 +1850,14 @@
         <v>111</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>211</v>
+        <v>115</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2154,8 +1865,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -2163,15 +1874,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2208,7 +1919,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>143</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2234,7 +1945,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>241</v>
+        <v>144</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2257,7 +1968,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>145</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2283,7 +1994,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>146</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2309,7 +2020,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>147</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2335,7 +2046,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>148</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2358,7 +2069,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2366,25 +2077,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:M61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" style="1" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="31.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="41.28515625" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="10" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="11" max="11" style="1" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="23.140625" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="41.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="10" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" style="1" collapsed="1"/>
+    <col min="12" max="12" width="23.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2430,7 +2141,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>246</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2453,7 +2164,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>247</v>
+        <v>150</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2479,7 +2190,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>151</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2505,7 +2216,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>152</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2531,7 +2242,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>250</v>
+        <v>153</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2557,7 +2268,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>154</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2580,7 +2291,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>252</v>
+        <v>155</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2606,7 +2317,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>253</v>
+        <v>156</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2632,7 +2343,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>254</v>
+        <v>157</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2658,7 +2369,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>255</v>
+        <v>158</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2684,7 +2395,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>256</v>
+        <v>159</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2707,7 +2418,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>257</v>
+        <v>160</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2733,7 +2444,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>161</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2759,7 +2470,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>259</v>
+        <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2785,7 +2496,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>260</v>
+        <v>163</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2806,12 +2517,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>261</v>
+        <v>164</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2835,12 +2546,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>262</v>
+        <v>165</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2864,12 +2575,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>263</v>
+        <v>166</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2893,12 +2604,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>264</v>
+        <v>167</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2916,12 +2627,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>265</v>
+        <v>168</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2945,12 +2656,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>266</v>
+        <v>169</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2974,12 +2685,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>267</v>
+        <v>170</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -3000,12 +2711,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>268</v>
+        <v>171</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -3029,12 +2740,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>269</v>
+        <v>172</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -3061,12 +2772,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>270</v>
+        <v>173</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -3090,12 +2801,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>271</v>
+        <v>221</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -3115,19 +2826,16 @@
       <c r="H27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K27" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>272</v>
+        <v>174</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -3150,13 +2858,16 @@
       <c r="K28" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>273</v>
+        <v>175</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -3180,12 +2891,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>274</v>
+        <v>176</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -3209,12 +2920,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>275</v>
+        <v>177</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -3238,12 +2949,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>276</v>
+        <v>178</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -3261,12 +2972,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>277</v>
+        <v>179</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -3290,12 +3001,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>278</v>
+        <v>180</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -3319,12 +3030,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>279</v>
+        <v>181</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -3345,12 +3056,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>280</v>
+        <v>182</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -3374,12 +3085,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>281</v>
+        <v>183</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3406,12 +3117,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>282</v>
+        <v>184</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3435,12 +3146,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>283</v>
+        <v>222</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3460,19 +3171,16 @@
       <c r="H39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K39" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>284</v>
+        <v>185</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3495,13 +3203,16 @@
       <c r="K40" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>285</v>
+        <v>186</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3525,12 +3236,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>286</v>
+        <v>187</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3554,12 +3265,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>287</v>
+        <v>188</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3583,12 +3294,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>288</v>
+        <v>189</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3606,12 +3317,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>289</v>
+        <v>190</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3635,12 +3346,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>290</v>
+        <v>191</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3664,12 +3375,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>291</v>
+        <v>192</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3690,12 +3401,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>292</v>
+        <v>193</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3719,12 +3430,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>293</v>
+        <v>194</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3751,12 +3462,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>294</v>
+        <v>195</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3780,12 +3491,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>295</v>
+        <v>223</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3805,19 +3516,16 @@
       <c r="H51" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I51" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K51" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>113</v>
       </c>
       <c r="B52" t="s">
-        <v>296</v>
+        <v>196</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3840,13 +3548,16 @@
       <c r="K52" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>297</v>
+        <v>197</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>32</v>
@@ -3855,18 +3566,18 @@
         <v>16</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>212</v>
+        <v>116</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>298</v>
+        <v>198</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>32</v>
@@ -3875,7 +3586,7 @@
         <v>16</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>211</v>
+        <v>115</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>114</v>
@@ -3884,12 +3595,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>299</v>
+        <v>199</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>32</v>
@@ -3910,12 +3621,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>32</v>
@@ -3924,18 +3635,18 @@
         <v>16</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>212</v>
+        <v>116</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B57" t="s">
-        <v>301</v>
+        <v>201</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>32</v>
@@ -3944,7 +3655,7 @@
         <v>16</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>211</v>
+        <v>115</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>37</v>
@@ -3953,12 +3664,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>302</v>
+        <v>202</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>32</v>
@@ -3979,12 +3690,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B59" t="s">
-        <v>303</v>
+        <v>203</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>32</v>
@@ -3993,18 +3704,18 @@
         <v>16</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>212</v>
+        <v>116</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B60" t="s">
-        <v>304</v>
+        <v>204</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>32</v>
@@ -4013,7 +3724,7 @@
         <v>16</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>211</v>
+        <v>115</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>18</v>
@@ -4022,12 +3733,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B61" t="s">
-        <v>305</v>
+        <v>205</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>32</v>
@@ -4051,7 +3762,7 @@
   </sheetData>
   <autoFilter ref="E1:E52" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4059,8 +3770,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -4068,15 +3779,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4178,7 +3889,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4186,8 +3897,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
@@ -4195,14 +3906,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4236,7 +3947,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>308</v>
+        <v>208</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4259,7 +3970,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>309</v>
+        <v>209</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -4282,7 +3993,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>310</v>
+        <v>210</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -4305,7 +4016,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>311</v>
+        <v>211</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4328,7 +4039,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>312</v>
+        <v>212</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4351,7 +4062,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>313</v>
+        <v>213</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -4371,7 +4082,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>314</v>
+        <v>214</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -4391,7 +4102,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>315</v>
+        <v>215</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -4407,13 +4118,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -4421,14 +4132,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4459,7 +4170,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>316</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4482,7 +4193,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>317</v>
+        <v>217</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -4505,7 +4216,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>318</v>
+        <v>218</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -4528,7 +4239,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>319</v>
+        <v>219</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4551,7 +4262,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4570,26 +4281,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4617,7 +4328,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>306</v>
+        <v>206</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4637,7 +4348,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>307</v>
+        <v>207</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -4650,6 +4361,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RAD UI and BeforePayments Test Cases
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/BeforePayments.xlsx
+++ b/KatalonData/RADTestData/BeforePayments.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t465179\Documents\git\VPS-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{5024DE7A-EA9E-4B08-9ED9-4439761CC728}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFD618C-73FC-4360-8EBB-C06DC494E129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="15840" windowWidth="29040" xWindow="28680" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}" yWindow="-3945"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{D99FAB39-5CE6-4AA4-B9C6-99B1EFA0654E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Estimated" r:id="rId1" sheetId="1"/>
-    <sheet name="Existing" r:id="rId2" sheetId="2"/>
-    <sheet name="Extension" r:id="rId3" sheetId="3"/>
-    <sheet name="NewTaxReturn" r:id="rId4" sheetId="4"/>
-    <sheet name="Personal" r:id="rId5" sheetId="5"/>
-    <sheet name="Personal_IND" r:id="rId6" sheetId="6"/>
-    <sheet name="Personal_JNT" r:id="rId7" sheetId="7"/>
-    <sheet name="Personal_EL" r:id="rId8" sheetId="8"/>
+    <sheet name="Estimated" sheetId="1" r:id="rId1"/>
+    <sheet name="Existing" sheetId="2" r:id="rId2"/>
+    <sheet name="Extension" sheetId="3" r:id="rId3"/>
+    <sheet name="NewTaxReturn" sheetId="4" r:id="rId4"/>
+    <sheet name="Personal" sheetId="5" r:id="rId5"/>
+    <sheet name="Personal_IND" sheetId="6" r:id="rId6"/>
+    <sheet name="Personal_JNT" sheetId="7" r:id="rId7"/>
+    <sheet name="Personal_EL" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">NewTaxReturn!$E$1:$E$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">NewTaxReturn!$E$1:$E$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="225">
   <si>
     <t>Result</t>
   </si>
@@ -399,273 +399,21 @@
     <t>Digital Advertising Gross Revenues</t>
   </si>
   <si>
-    <t>Mon Feb 17 18:12:12 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:14:06 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:16:00 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:16:51 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:17:43 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:19:37 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:21:33 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:23:28 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:25:23 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:26:15 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:27:06 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:29:00 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:30:56 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:32:50 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:33:42 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:35:37 EST 2025</t>
-  </si>
-  <si>
     <t>Mon Feb 17 18:36:29 EST 2025</t>
   </si>
   <si>
-    <t>Mon Feb 17 18:37:21 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:39:15 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:40:07 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:40:59 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:41:50 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:42:41 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:43:32 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:44:23 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:45:16 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:46:08 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:46:59 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:47:50 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:48:42 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:49:33 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:50:25 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:51:16 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:52:08 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:52:58 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:53:50 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:54:42 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:55:33 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:56:25 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:57:16 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:58:08 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:59:00 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 18:59:53 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:00:46 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:01:37 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:02:30 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:03:22 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:04:14 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:05:06 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:06:00 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:07:46 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:08:43 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:09:36 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:10:29 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:11:21 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:12:12 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:13:05 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:13:58 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:14:50 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:15:44 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:16:37 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:18:23 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:19:20 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:20:14 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:21:07 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:21:59 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:22:50 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:23:42 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:24:35 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:25:27 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:26:20 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:27:12 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:28:58 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:29:54 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:30:46 EST 2025</t>
-  </si>
-  <si>
     <t>Mon Feb 17 19:31:37 EST 2025</t>
   </si>
   <si>
-    <t>Mon Feb 17 19:32:29 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:33:20 EST 2025</t>
-  </si>
-  <si>
     <t>Mon Feb 17 19:34:11 EST 2025</t>
   </si>
   <si>
-    <t>Mon Feb 17 19:35:03 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:35:55 EST 2025</t>
-  </si>
-  <si>
     <t>Mon Feb 17 19:36:46 EST 2025</t>
   </si>
   <si>
-    <t>Mon Feb 17 19:37:38 EST 2025</t>
-  </si>
-  <si>
     <t>Mon Feb 17 19:38:28 EST 2025</t>
   </si>
   <si>
-    <t>Mon Feb 17 19:39:19 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:40:08 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:40:57 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:41:45 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:42:33 EST 2025</t>
-  </si>
-  <si>
     <t>Mon Feb 17 19:43:22 EST 2025</t>
   </si>
   <si>
@@ -675,119 +423,310 @@
     <t>Mon Feb 17 19:44:59 EST 2025</t>
   </si>
   <si>
-    <t>Mon Feb 17 19:45:48 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:46:42 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:47:37 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:48:32 EST 2025</t>
-  </si>
-  <si>
-    <t>Mon Feb 17 19:49:26 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 18 17:15:40 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 18 17:16:39 EST 2025</t>
-  </si>
-  <si>
-    <t>Tue Feb 18 17:17:34 EST 2025</t>
-  </si>
-  <si>
     <t>Incorrect App ID</t>
   </si>
   <si>
-    <t>Tue Oct 07 18:43:13 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 18:43:47 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 18:44:20 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 18:44:50 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 18:45:20 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 18:45:50 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:26:45 EDT 2025</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:46:16 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:46:45 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:47:14 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:47:42 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:48:10 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:48:39 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:49:07 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:49:35 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:50:04 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:50:32 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:51:00 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:51:28 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:51:57 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:52:25 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:52:53 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:53:21 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:53:49 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:54:17 EDT 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 07 20:54:45 EDT 2025</t>
+    <t>Mon Oct 13 20:50:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:51:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:51:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:52:40 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:53:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:54:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:54:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:55:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:56:08 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:56:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:57:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:58:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:58:47 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:59:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:00:09 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:00:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:01:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:02:08 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:02:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:03:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:04:07 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:04:47 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:05:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:06:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:06:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:11:40 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:12:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:13:37 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:14:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:15:01 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:15:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:16:41 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:17:23 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:18:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:18:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:19:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:20:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:21:01 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:21:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:22:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:23:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:24:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:24:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:25:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:26:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:27:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:28:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:28:40 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:31:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:33:44 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:34:37 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:35:21 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:36:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:37:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:38:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:38:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:39:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:40:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:41:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:42:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:42:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:43:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:44:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:45:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:46:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:46:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:47:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:48:40 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:49:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:50:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:51:30 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:52:10 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:52:53 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:53:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:54:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:55:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:56:09 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:57:13 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:58:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 21:58:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 14:57:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 14:58:10 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 14:58:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 14:59:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 15:00:07 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 15:03:07 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 15:03:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 15:04:38 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 15:05:23 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 15:06:07 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 22:16:58 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 22:17:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 22:18:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 22:19:01 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 22:19:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 22:20:33 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 22:26:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 22:27:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 22:29:08 EDT 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -836,19 +775,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -865,10 +804,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -903,7 +842,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -955,7 +894,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1066,21 +1005,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1097,7 +1036,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1149,15 +1088,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office 2013 - 2022 Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDCA51-7A9D-4BB2-A660-F3BEEC814D67}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
@@ -1165,17 +1104,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.1796875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="14.54296875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="44.54296875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="35.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="15.26953125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.26953125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="19.54296875" collapsed="true"/>
-    <col min="9" max="9" style="1" width="9.1796875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="18.453125" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="9.1796875" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="44.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.1796875" style="1" collapsed="1"/>
+    <col min="10" max="10" width="18.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -1215,7 +1154,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1244,7 +1183,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1273,7 +1212,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1305,7 +1244,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>129</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1337,7 +1276,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>130</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1369,7 +1308,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>131</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1398,8 +1337,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1407,25 +1346,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
-  <dimension ref="A1:K21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB49CF7-E4D4-4F06-BD88-EA9191F7BC6F}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="14.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.26953125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="12.6328125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="52.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="32.453125" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.1796875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.26953125" collapsed="true"/>
-    <col min="9" max="9" style="1" width="9.1796875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="28.26953125" collapsed="true"/>
-    <col min="11" max="16384" style="1" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="14.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.6328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="52" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.1796875" style="1" collapsed="1"/>
+    <col min="8" max="8" width="16.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.1796875" style="1" collapsed="1"/>
+    <col min="10" max="10" width="28.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -1465,7 +1404,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>132</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -1488,7 +1427,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>133</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1511,7 +1450,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>134</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1534,7 +1473,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1560,7 +1499,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>136</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -1586,7 +1525,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>231</v>
+        <v>137</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1609,7 +1548,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>232</v>
+        <v>138</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -1632,7 +1571,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>233</v>
+        <v>139</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1655,7 +1594,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>234</v>
+        <v>140</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -1678,7 +1617,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>235</v>
+        <v>141</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1701,7 +1640,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>142</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1724,7 +1663,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>237</v>
+        <v>143</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -1747,7 +1686,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>238</v>
+        <v>144</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1770,7 +1709,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>239</v>
+        <v>145</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1790,7 +1729,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>240</v>
+        <v>146</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1816,7 +1755,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>241</v>
+        <v>147</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1839,7 +1778,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>242</v>
+        <v>148</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1862,7 +1801,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>36</v>
@@ -1885,7 +1824,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>243</v>
+        <v>149</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -1902,7 +1841,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>244</v>
+        <v>150</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -1918,7 +1857,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1926,8 +1865,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22222EF-2A37-441E-9CE4-90FD36DC8DDC}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -1935,15 +1874,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.26953125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.1796875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="24.453125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="27.0" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.1796875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.26953125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="9.1796875" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.1796875" style="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -1980,7 +1919,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2006,7 +1945,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2029,7 +1968,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2055,7 +1994,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>219</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2081,7 +2020,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>220</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2107,7 +2046,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>221</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2130,7 +2069,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2138,25 +2077,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
-  <dimension ref="A1:M61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}">
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:XFD61"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="12.7265625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="31.7265625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="41.26953125" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.1796875" collapsed="true"/>
-    <col min="7" max="10" customWidth="true" style="1" width="19.81640625" collapsed="true"/>
-    <col min="11" max="11" style="1" width="9.1796875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="23.1796875" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="9.1796875" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="41.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.1796875" style="1" collapsed="1"/>
+    <col min="7" max="10" width="19.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.1796875" style="1" collapsed="1"/>
+    <col min="12" max="12" width="23.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -2202,7 +2141,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -2225,7 +2164,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -2251,7 +2190,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -2277,7 +2216,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -2303,7 +2242,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -2329,7 +2268,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2352,7 +2291,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -2378,7 +2317,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -2404,7 +2343,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -2430,7 +2369,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -2456,7 +2395,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2479,7 +2418,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>32</v>
@@ -2505,7 +2444,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2531,7 +2470,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2557,7 +2496,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2583,7 +2522,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -2612,7 +2551,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -2641,7 +2580,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -2670,7 +2609,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>32</v>
@@ -2693,7 +2632,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -2722,7 +2661,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2751,7 +2690,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2777,7 +2716,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2806,7 +2745,7 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>165</v>
+        <v>222</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -2838,7 +2777,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2867,7 +2806,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2896,7 +2835,7 @@
         <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>167</v>
+        <v>224</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2920,7 +2859,7 @@
         <v>92</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>217</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
@@ -2928,7 +2867,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2957,7 +2896,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>32</v>
@@ -2986,7 +2925,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>32</v>
@@ -3015,7 +2954,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -3038,7 +2977,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -3067,7 +3006,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -3096,7 +3035,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -3122,7 +3061,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -3151,7 +3090,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
@@ -3183,7 +3122,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
@@ -3212,7 +3151,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
@@ -3241,7 +3180,7 @@
         <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -3265,7 +3204,7 @@
         <v>92</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>217</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
@@ -3273,7 +3212,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
@@ -3302,7 +3241,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>32</v>
@@ -3331,7 +3270,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>32</v>
@@ -3360,7 +3299,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -3383,7 +3322,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -3412,7 +3351,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3441,7 +3380,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -3467,7 +3406,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>32</v>
@@ -3496,7 +3435,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -3528,7 +3467,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -3557,7 +3496,7 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>32</v>
@@ -3586,7 +3525,7 @@
         <v>113</v>
       </c>
       <c r="B52" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -3610,7 +3549,7 @@
         <v>92</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>217</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
@@ -3618,7 +3557,7 @@
         <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>32</v>
@@ -3638,7 +3577,7 @@
         <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>32</v>
@@ -3661,7 +3600,7 @@
         <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>192</v>
+        <v>118</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>36</v>
@@ -3687,7 +3626,7 @@
         <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>32</v>
@@ -3707,7 +3646,7 @@
         <v>35</v>
       </c>
       <c r="B57" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>32</v>
@@ -3730,7 +3669,7 @@
         <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>195</v>
+        <v>119</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>36</v>
@@ -3756,7 +3695,7 @@
         <v>35</v>
       </c>
       <c r="B59" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>32</v>
@@ -3776,7 +3715,7 @@
         <v>35</v>
       </c>
       <c r="B60" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>32</v>
@@ -3799,7 +3738,7 @@
         <v>35</v>
       </c>
       <c r="B61" t="s">
-        <v>198</v>
+        <v>120</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>36</v>
@@ -3823,7 +3762,7 @@
   </sheetData>
   <autoFilter ref="E1:E52" xr:uid="{E3B7105E-5E71-456F-8D2A-C4C503B29111}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3831,8 +3770,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C48EC9F-E6C0-40A2-877C-8FE515BAA791}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -3840,12 +3779,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.1796875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="22.453125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="26.26953125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.81640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.26953125" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="9.1796875" style="1" collapsed="1"/>
+    <col min="2" max="2" width="22.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -3950,7 +3889,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3958,8 +3897,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13C096-3F8A-4B4D-A3EE-3415763F7F13}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -3967,14 +3906,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="15.1796875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.81640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.26953125" collapsed="true"/>
-    <col min="6" max="7" style="1" width="9.1796875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="23.453125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="9.1796875" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.1796875" style="1" collapsed="1"/>
+    <col min="8" max="8" width="23.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -4008,7 +3947,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4031,7 +3970,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -4054,7 +3993,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -4077,7 +4016,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4100,7 +4039,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4123,7 +4062,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>36</v>
@@ -4143,7 +4082,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
+        <v>123</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>36</v>
@@ -4163,7 +4102,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>208</v>
+        <v>124</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>36</v>
@@ -4179,13 +4118,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A156AB6-80FF-4E48-B399-7CA373BDFD42}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -4193,14 +4132,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.453125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.26953125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.81640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.26953125" collapsed="true"/>
-    <col min="6" max="6" style="1" width="9.1796875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.1796875" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="9.1796875" style="1" collapsed="1"/>
+    <col min="2" max="2" width="26.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.1796875" style="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -4231,7 +4170,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4254,7 +4193,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -4277,7 +4216,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -4300,7 +4239,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -4323,7 +4262,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -4342,13 +4281,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F3D31C-4F04-42F4-8C54-828F1948951D}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -4356,12 +4295,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.1796875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="32.453125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.7265625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="50.81640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="46.26953125" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="9.1796875" style="1" collapsed="1"/>
+    <col min="2" max="2" width="32.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="46.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -4389,7 +4328,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -4409,7 +4348,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>121</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>36</v>
@@ -4422,6 +4361,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>